<commit_message>
Se agrego la liga de Francia. Se cambio eliminarEspacios para eliminar cualquier numero de espacios (antes solo servia para 1 espacio). Se entreno la red con los datos de Francia
</commit_message>
<xml_diff>
--- a/DatosAle1/DP1213.xlsx
+++ b/DatosAle1/DP1213.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="19155" windowHeight="8505"/>
+    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="D1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="141">
   <si>
     <t>Div</t>
   </si>
@@ -1259,9 +1259,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BR244"/>
+  <dimension ref="A1:BR253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -52993,6 +52993,1914 @@
         <v>1.8</v>
       </c>
     </row>
+    <row r="245" spans="1:70">
+      <c r="A245" t="s">
+        <v>70</v>
+      </c>
+      <c r="B245" s="1">
+        <v>41398</v>
+      </c>
+      <c r="C245" t="s">
+        <v>89</v>
+      </c>
+      <c r="D245" t="s">
+        <v>77</v>
+      </c>
+      <c r="E245">
+        <v>3</v>
+      </c>
+      <c r="F245">
+        <v>0</v>
+      </c>
+      <c r="G245" t="s">
+        <v>74</v>
+      </c>
+      <c r="H245">
+        <v>1</v>
+      </c>
+      <c r="I245">
+        <v>0</v>
+      </c>
+      <c r="J245" t="s">
+        <v>74</v>
+      </c>
+      <c r="K245">
+        <v>17</v>
+      </c>
+      <c r="L245">
+        <v>15</v>
+      </c>
+      <c r="M245">
+        <v>8</v>
+      </c>
+      <c r="N245">
+        <v>4</v>
+      </c>
+      <c r="O245">
+        <v>23</v>
+      </c>
+      <c r="P245">
+        <v>16</v>
+      </c>
+      <c r="Q245">
+        <v>3</v>
+      </c>
+      <c r="R245">
+        <v>3</v>
+      </c>
+      <c r="S245">
+        <v>3</v>
+      </c>
+      <c r="T245">
+        <v>3</v>
+      </c>
+      <c r="U245">
+        <v>0</v>
+      </c>
+      <c r="V245">
+        <v>0</v>
+      </c>
+      <c r="W245">
+        <v>2</v>
+      </c>
+      <c r="X245">
+        <v>3.4</v>
+      </c>
+      <c r="Y245">
+        <v>3.75</v>
+      </c>
+      <c r="Z245">
+        <v>2</v>
+      </c>
+      <c r="AA245">
+        <v>3.5</v>
+      </c>
+      <c r="AB245">
+        <v>3.6</v>
+      </c>
+      <c r="AC245">
+        <v>2</v>
+      </c>
+      <c r="AD245">
+        <v>3.5</v>
+      </c>
+      <c r="AE245">
+        <v>3.6</v>
+      </c>
+      <c r="AF245">
+        <v>2.1</v>
+      </c>
+      <c r="AG245">
+        <v>3.3</v>
+      </c>
+      <c r="AH245">
+        <v>3.3</v>
+      </c>
+      <c r="AI245">
+        <v>2</v>
+      </c>
+      <c r="AJ245">
+        <v>3.3</v>
+      </c>
+      <c r="AK245">
+        <v>3.75</v>
+      </c>
+      <c r="AL245">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="AM245">
+        <v>3.55</v>
+      </c>
+      <c r="AN245">
+        <v>4.07</v>
+      </c>
+      <c r="AO245">
+        <v>2</v>
+      </c>
+      <c r="AP245">
+        <v>3.4</v>
+      </c>
+      <c r="AQ245">
+        <v>3.75</v>
+      </c>
+      <c r="AR245">
+        <v>1.91</v>
+      </c>
+      <c r="AS245">
+        <v>3.4</v>
+      </c>
+      <c r="AT245">
+        <v>3.8</v>
+      </c>
+      <c r="AU245">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AV245">
+        <v>3.5</v>
+      </c>
+      <c r="AW245">
+        <v>3.9</v>
+      </c>
+      <c r="AX245">
+        <v>2</v>
+      </c>
+      <c r="AY245">
+        <v>3.5</v>
+      </c>
+      <c r="AZ245">
+        <v>3.6</v>
+      </c>
+      <c r="BA245">
+        <v>38</v>
+      </c>
+      <c r="BB245">
+        <v>2.1</v>
+      </c>
+      <c r="BC245">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="BD245">
+        <v>3.55</v>
+      </c>
+      <c r="BE245">
+        <v>3.39</v>
+      </c>
+      <c r="BF245">
+        <v>4.24</v>
+      </c>
+      <c r="BG245">
+        <v>3.82</v>
+      </c>
+      <c r="BH245">
+        <v>34</v>
+      </c>
+      <c r="BI245">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="BJ245">
+        <v>2.13</v>
+      </c>
+      <c r="BK245">
+        <v>1.78</v>
+      </c>
+      <c r="BL245">
+        <v>1.7</v>
+      </c>
+      <c r="BM245">
+        <v>23</v>
+      </c>
+      <c r="BN245">
+        <v>-0.25</v>
+      </c>
+      <c r="BO245">
+        <v>1.78</v>
+      </c>
+      <c r="BP245">
+        <v>1.74</v>
+      </c>
+      <c r="BQ245">
+        <v>2.25</v>
+      </c>
+      <c r="BR245">
+        <v>2.17</v>
+      </c>
+    </row>
+    <row r="246" spans="1:70">
+      <c r="A246" t="s">
+        <v>70</v>
+      </c>
+      <c r="B246" s="1">
+        <v>41429</v>
+      </c>
+      <c r="C246" t="s">
+        <v>72</v>
+      </c>
+      <c r="D246" t="s">
+        <v>76</v>
+      </c>
+      <c r="E246">
+        <v>4</v>
+      </c>
+      <c r="F246">
+        <v>2</v>
+      </c>
+      <c r="G246" t="s">
+        <v>74</v>
+      </c>
+      <c r="H246">
+        <v>1</v>
+      </c>
+      <c r="I246">
+        <v>2</v>
+      </c>
+      <c r="J246" t="s">
+        <v>78</v>
+      </c>
+      <c r="K246">
+        <v>13</v>
+      </c>
+      <c r="L246">
+        <v>12</v>
+      </c>
+      <c r="M246">
+        <v>7</v>
+      </c>
+      <c r="N246">
+        <v>8</v>
+      </c>
+      <c r="O246">
+        <v>12</v>
+      </c>
+      <c r="P246">
+        <v>21</v>
+      </c>
+      <c r="Q246">
+        <v>4</v>
+      </c>
+      <c r="R246">
+        <v>7</v>
+      </c>
+      <c r="S246">
+        <v>1</v>
+      </c>
+      <c r="T246">
+        <v>4</v>
+      </c>
+      <c r="U246">
+        <v>0</v>
+      </c>
+      <c r="V246">
+        <v>0</v>
+      </c>
+      <c r="W246">
+        <v>1.3</v>
+      </c>
+      <c r="X246">
+        <v>5.5</v>
+      </c>
+      <c r="Y246">
+        <v>9</v>
+      </c>
+      <c r="Z246">
+        <v>1.3</v>
+      </c>
+      <c r="AA246">
+        <v>5.75</v>
+      </c>
+      <c r="AB246">
+        <v>8.25</v>
+      </c>
+      <c r="AC246">
+        <v>1.3</v>
+      </c>
+      <c r="AD246">
+        <v>5.75</v>
+      </c>
+      <c r="AE246">
+        <v>8.25</v>
+      </c>
+      <c r="AF246">
+        <v>1.33</v>
+      </c>
+      <c r="AG246">
+        <v>5</v>
+      </c>
+      <c r="AH246">
+        <v>7.8</v>
+      </c>
+      <c r="AI246">
+        <v>1.3</v>
+      </c>
+      <c r="AJ246">
+        <v>5.5</v>
+      </c>
+      <c r="AK246">
+        <v>9</v>
+      </c>
+      <c r="AL246">
+        <v>1.36</v>
+      </c>
+      <c r="AM246">
+        <v>5.63</v>
+      </c>
+      <c r="AN246">
+        <v>9.4</v>
+      </c>
+      <c r="AO246">
+        <v>1.36</v>
+      </c>
+      <c r="AP246">
+        <v>4.5</v>
+      </c>
+      <c r="AQ246">
+        <v>9</v>
+      </c>
+      <c r="AR246">
+        <v>1.33</v>
+      </c>
+      <c r="AS246">
+        <v>5.75</v>
+      </c>
+      <c r="AT246">
+        <v>7.5</v>
+      </c>
+      <c r="AU246">
+        <v>1.33</v>
+      </c>
+      <c r="AV246">
+        <v>5.75</v>
+      </c>
+      <c r="AW246">
+        <v>9.5</v>
+      </c>
+      <c r="AX246">
+        <v>1.3</v>
+      </c>
+      <c r="AY246">
+        <v>5.5</v>
+      </c>
+      <c r="AZ246">
+        <v>9</v>
+      </c>
+      <c r="BA246">
+        <v>38</v>
+      </c>
+      <c r="BB246">
+        <v>1.36</v>
+      </c>
+      <c r="BC246">
+        <v>1.33</v>
+      </c>
+      <c r="BD246">
+        <v>5.75</v>
+      </c>
+      <c r="BE246">
+        <v>5.33</v>
+      </c>
+      <c r="BF246">
+        <v>10</v>
+      </c>
+      <c r="BG246">
+        <v>8.43</v>
+      </c>
+      <c r="BH246">
+        <v>24</v>
+      </c>
+      <c r="BI246">
+        <v>1.52</v>
+      </c>
+      <c r="BJ246">
+        <v>1.45</v>
+      </c>
+      <c r="BK246">
+        <v>2.75</v>
+      </c>
+      <c r="BL246">
+        <v>2.62</v>
+      </c>
+      <c r="BM246">
+        <v>24</v>
+      </c>
+      <c r="BN246">
+        <v>-1.5</v>
+      </c>
+      <c r="BO246">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="BP246">
+        <v>1.96</v>
+      </c>
+      <c r="BQ246">
+        <v>1.95</v>
+      </c>
+      <c r="BR246">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="247" spans="1:70">
+      <c r="A247" t="s">
+        <v>70</v>
+      </c>
+      <c r="B247" s="1">
+        <v>41429</v>
+      </c>
+      <c r="C247" t="s">
+        <v>80</v>
+      </c>
+      <c r="D247" t="s">
+        <v>85</v>
+      </c>
+      <c r="E247">
+        <v>0</v>
+      </c>
+      <c r="F247">
+        <v>1</v>
+      </c>
+      <c r="G247" t="s">
+        <v>78</v>
+      </c>
+      <c r="H247">
+        <v>0</v>
+      </c>
+      <c r="I247">
+        <v>0</v>
+      </c>
+      <c r="J247" t="s">
+        <v>79</v>
+      </c>
+      <c r="K247">
+        <v>13</v>
+      </c>
+      <c r="L247">
+        <v>15</v>
+      </c>
+      <c r="M247">
+        <v>4</v>
+      </c>
+      <c r="N247">
+        <v>5</v>
+      </c>
+      <c r="O247">
+        <v>16</v>
+      </c>
+      <c r="P247">
+        <v>11</v>
+      </c>
+      <c r="Q247">
+        <v>7</v>
+      </c>
+      <c r="R247">
+        <v>9</v>
+      </c>
+      <c r="S247">
+        <v>1</v>
+      </c>
+      <c r="T247">
+        <v>2</v>
+      </c>
+      <c r="U247">
+        <v>0</v>
+      </c>
+      <c r="V247">
+        <v>0</v>
+      </c>
+      <c r="W247">
+        <v>6</v>
+      </c>
+      <c r="X247">
+        <v>4</v>
+      </c>
+      <c r="Y247">
+        <v>1.53</v>
+      </c>
+      <c r="Z247">
+        <v>5.5</v>
+      </c>
+      <c r="AA247">
+        <v>4.33</v>
+      </c>
+      <c r="AB247">
+        <v>1.53</v>
+      </c>
+      <c r="AC247">
+        <v>5.5</v>
+      </c>
+      <c r="AD247">
+        <v>4.33</v>
+      </c>
+      <c r="AE247">
+        <v>1.53</v>
+      </c>
+      <c r="AF247">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="AG247">
+        <v>3.6</v>
+      </c>
+      <c r="AH247">
+        <v>1.65</v>
+      </c>
+      <c r="AI247">
+        <v>6</v>
+      </c>
+      <c r="AJ247">
+        <v>4</v>
+      </c>
+      <c r="AK247">
+        <v>1.53</v>
+      </c>
+      <c r="AL247">
+        <v>6.6</v>
+      </c>
+      <c r="AM247">
+        <v>4.3</v>
+      </c>
+      <c r="AN247">
+        <v>1.57</v>
+      </c>
+      <c r="AO247">
+        <v>5.5</v>
+      </c>
+      <c r="AP247">
+        <v>3.75</v>
+      </c>
+      <c r="AQ247">
+        <v>1.62</v>
+      </c>
+      <c r="AR247">
+        <v>5.8</v>
+      </c>
+      <c r="AS247">
+        <v>4</v>
+      </c>
+      <c r="AT247">
+        <v>1.53</v>
+      </c>
+      <c r="AU247">
+        <v>6.5</v>
+      </c>
+      <c r="AV247">
+        <v>4.3</v>
+      </c>
+      <c r="AW247">
+        <v>1.55</v>
+      </c>
+      <c r="AX247">
+        <v>6</v>
+      </c>
+      <c r="AY247">
+        <v>4.2</v>
+      </c>
+      <c r="AZ247">
+        <v>1.53</v>
+      </c>
+      <c r="BA247">
+        <v>38</v>
+      </c>
+      <c r="BB247">
+        <v>6.24</v>
+      </c>
+      <c r="BC247">
+        <v>5.7</v>
+      </c>
+      <c r="BD247">
+        <v>4.33</v>
+      </c>
+      <c r="BE247">
+        <v>4.05</v>
+      </c>
+      <c r="BF247">
+        <v>1.65</v>
+      </c>
+      <c r="BG247">
+        <v>1.57</v>
+      </c>
+      <c r="BH247">
+        <v>34</v>
+      </c>
+      <c r="BI247">
+        <v>1.79</v>
+      </c>
+      <c r="BJ247">
+        <v>1.7</v>
+      </c>
+      <c r="BK247">
+        <v>2.25</v>
+      </c>
+      <c r="BL247">
+        <v>2.13</v>
+      </c>
+      <c r="BM247">
+        <v>24</v>
+      </c>
+      <c r="BN247">
+        <v>1</v>
+      </c>
+      <c r="BO247">
+        <v>1.96</v>
+      </c>
+      <c r="BP247">
+        <v>1.9</v>
+      </c>
+      <c r="BQ247">
+        <v>2.02</v>
+      </c>
+      <c r="BR247">
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="248" spans="1:70">
+      <c r="A248" t="s">
+        <v>70</v>
+      </c>
+      <c r="B248" s="1">
+        <v>41429</v>
+      </c>
+      <c r="C248" t="s">
+        <v>86</v>
+      </c>
+      <c r="D248" t="s">
+        <v>82</v>
+      </c>
+      <c r="E248">
+        <v>0</v>
+      </c>
+      <c r="F248">
+        <v>1</v>
+      </c>
+      <c r="G248" t="s">
+        <v>78</v>
+      </c>
+      <c r="H248">
+        <v>0</v>
+      </c>
+      <c r="I248">
+        <v>0</v>
+      </c>
+      <c r="J248" t="s">
+        <v>79</v>
+      </c>
+      <c r="K248">
+        <v>13</v>
+      </c>
+      <c r="L248">
+        <v>8</v>
+      </c>
+      <c r="M248">
+        <v>5</v>
+      </c>
+      <c r="N248">
+        <v>3</v>
+      </c>
+      <c r="O248">
+        <v>15</v>
+      </c>
+      <c r="P248">
+        <v>12</v>
+      </c>
+      <c r="Q248">
+        <v>6</v>
+      </c>
+      <c r="R248">
+        <v>1</v>
+      </c>
+      <c r="S248">
+        <v>2</v>
+      </c>
+      <c r="T248">
+        <v>0</v>
+      </c>
+      <c r="U248">
+        <v>0</v>
+      </c>
+      <c r="V248">
+        <v>0</v>
+      </c>
+      <c r="W248">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="X248">
+        <v>3.3</v>
+      </c>
+      <c r="Y248">
+        <v>3.1</v>
+      </c>
+      <c r="Z248">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AA248">
+        <v>3.25</v>
+      </c>
+      <c r="AB248">
+        <v>3.1</v>
+      </c>
+      <c r="AC248">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AD248">
+        <v>3.25</v>
+      </c>
+      <c r="AE248">
+        <v>3.1</v>
+      </c>
+      <c r="AF248">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AG248">
+        <v>3.2</v>
+      </c>
+      <c r="AH248">
+        <v>3</v>
+      </c>
+      <c r="AI248">
+        <v>2.25</v>
+      </c>
+      <c r="AJ248">
+        <v>3.2</v>
+      </c>
+      <c r="AK248">
+        <v>3.25</v>
+      </c>
+      <c r="AL248">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="AM248">
+        <v>3.49</v>
+      </c>
+      <c r="AN248">
+        <v>3.31</v>
+      </c>
+      <c r="AO248">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AP248">
+        <v>3.2</v>
+      </c>
+      <c r="AQ248">
+        <v>3.2</v>
+      </c>
+      <c r="AR248">
+        <v>2.25</v>
+      </c>
+      <c r="AS248">
+        <v>3.3</v>
+      </c>
+      <c r="AT248">
+        <v>3.13</v>
+      </c>
+      <c r="AU248">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AV248">
+        <v>3.4</v>
+      </c>
+      <c r="AW248">
+        <v>3.2</v>
+      </c>
+      <c r="AX248">
+        <v>2.25</v>
+      </c>
+      <c r="AY248">
+        <v>3.3</v>
+      </c>
+      <c r="AZ248">
+        <v>3.2</v>
+      </c>
+      <c r="BA248">
+        <v>38</v>
+      </c>
+      <c r="BB248">
+        <v>2.38</v>
+      </c>
+      <c r="BC248">
+        <v>2.29</v>
+      </c>
+      <c r="BD248">
+        <v>3.53</v>
+      </c>
+      <c r="BE248">
+        <v>3.34</v>
+      </c>
+      <c r="BF248">
+        <v>3.25</v>
+      </c>
+      <c r="BG248">
+        <v>3.1</v>
+      </c>
+      <c r="BH248">
+        <v>34</v>
+      </c>
+      <c r="BI248">
+        <v>2.04</v>
+      </c>
+      <c r="BJ248">
+        <v>1.96</v>
+      </c>
+      <c r="BK248">
+        <v>1.92</v>
+      </c>
+      <c r="BL248">
+        <v>1.83</v>
+      </c>
+      <c r="BM248">
+        <v>23</v>
+      </c>
+      <c r="BN248">
+        <v>-0.25</v>
+      </c>
+      <c r="BO248">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="BP248">
+        <v>1.99</v>
+      </c>
+      <c r="BQ248">
+        <v>1.94</v>
+      </c>
+      <c r="BR248">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="249" spans="1:70">
+      <c r="A249" t="s">
+        <v>70</v>
+      </c>
+      <c r="B249" s="1">
+        <v>41429</v>
+      </c>
+      <c r="C249" t="s">
+        <v>81</v>
+      </c>
+      <c r="D249" t="s">
+        <v>94</v>
+      </c>
+      <c r="E249">
+        <v>1</v>
+      </c>
+      <c r="F249">
+        <v>1</v>
+      </c>
+      <c r="G249" t="s">
+        <v>79</v>
+      </c>
+      <c r="H249">
+        <v>1</v>
+      </c>
+      <c r="I249">
+        <v>0</v>
+      </c>
+      <c r="J249" t="s">
+        <v>74</v>
+      </c>
+      <c r="K249">
+        <v>14</v>
+      </c>
+      <c r="L249">
+        <v>11</v>
+      </c>
+      <c r="M249">
+        <v>7</v>
+      </c>
+      <c r="N249">
+        <v>2</v>
+      </c>
+      <c r="O249">
+        <v>15</v>
+      </c>
+      <c r="P249">
+        <v>13</v>
+      </c>
+      <c r="Q249">
+        <v>5</v>
+      </c>
+      <c r="R249">
+        <v>4</v>
+      </c>
+      <c r="S249">
+        <v>2</v>
+      </c>
+      <c r="T249">
+        <v>3</v>
+      </c>
+      <c r="U249">
+        <v>0</v>
+      </c>
+      <c r="V249">
+        <v>0</v>
+      </c>
+      <c r="W249">
+        <v>1.5</v>
+      </c>
+      <c r="X249">
+        <v>4.33</v>
+      </c>
+      <c r="Y249">
+        <v>6</v>
+      </c>
+      <c r="Z249">
+        <v>1.5</v>
+      </c>
+      <c r="AA249">
+        <v>4.5</v>
+      </c>
+      <c r="AB249">
+        <v>5.75</v>
+      </c>
+      <c r="AC249">
+        <v>1.5</v>
+      </c>
+      <c r="AD249">
+        <v>4.5</v>
+      </c>
+      <c r="AE249">
+        <v>5.75</v>
+      </c>
+      <c r="AF249">
+        <v>1.55</v>
+      </c>
+      <c r="AG249">
+        <v>3.9</v>
+      </c>
+      <c r="AH249">
+        <v>5.6</v>
+      </c>
+      <c r="AI249">
+        <v>1.53</v>
+      </c>
+      <c r="AJ249">
+        <v>4</v>
+      </c>
+      <c r="AK249">
+        <v>6</v>
+      </c>
+      <c r="AL249">
+        <v>1.52</v>
+      </c>
+      <c r="AM249">
+        <v>4.55</v>
+      </c>
+      <c r="AN249">
+        <v>6.94</v>
+      </c>
+      <c r="AO249">
+        <v>1.53</v>
+      </c>
+      <c r="AP249">
+        <v>4</v>
+      </c>
+      <c r="AQ249">
+        <v>6</v>
+      </c>
+      <c r="AR249">
+        <v>1.5</v>
+      </c>
+      <c r="AS249">
+        <v>4.33</v>
+      </c>
+      <c r="AT249">
+        <v>6</v>
+      </c>
+      <c r="AU249">
+        <v>1.5</v>
+      </c>
+      <c r="AV249">
+        <v>4.5</v>
+      </c>
+      <c r="AW249">
+        <v>6.5</v>
+      </c>
+      <c r="AX249">
+        <v>1.5</v>
+      </c>
+      <c r="AY249">
+        <v>4.5</v>
+      </c>
+      <c r="AZ249">
+        <v>6</v>
+      </c>
+      <c r="BA249">
+        <v>38</v>
+      </c>
+      <c r="BB249">
+        <v>1.55</v>
+      </c>
+      <c r="BC249">
+        <v>1.51</v>
+      </c>
+      <c r="BD249">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="BE249">
+        <v>4.28</v>
+      </c>
+      <c r="BF249">
+        <v>6.8</v>
+      </c>
+      <c r="BG249">
+        <v>6.1</v>
+      </c>
+      <c r="BH249">
+        <v>30</v>
+      </c>
+      <c r="BI249">
+        <v>1.68</v>
+      </c>
+      <c r="BJ249">
+        <v>1.63</v>
+      </c>
+      <c r="BK249">
+        <v>2.38</v>
+      </c>
+      <c r="BL249">
+        <v>2.23</v>
+      </c>
+      <c r="BM249">
+        <v>24</v>
+      </c>
+      <c r="BN249">
+        <v>-1</v>
+      </c>
+      <c r="BO249">
+        <v>1.87</v>
+      </c>
+      <c r="BP249">
+        <v>1.83</v>
+      </c>
+      <c r="BQ249">
+        <v>2.1</v>
+      </c>
+      <c r="BR249">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="250" spans="1:70">
+      <c r="A250" t="s">
+        <v>70</v>
+      </c>
+      <c r="B250" s="1">
+        <v>41429</v>
+      </c>
+      <c r="C250" t="s">
+        <v>88</v>
+      </c>
+      <c r="D250" t="s">
+        <v>84</v>
+      </c>
+      <c r="E250">
+        <v>1</v>
+      </c>
+      <c r="F250">
+        <v>0</v>
+      </c>
+      <c r="G250" t="s">
+        <v>74</v>
+      </c>
+      <c r="H250">
+        <v>0</v>
+      </c>
+      <c r="I250">
+        <v>0</v>
+      </c>
+      <c r="J250" t="s">
+        <v>79</v>
+      </c>
+      <c r="K250">
+        <v>19</v>
+      </c>
+      <c r="L250">
+        <v>20</v>
+      </c>
+      <c r="M250">
+        <v>6</v>
+      </c>
+      <c r="N250">
+        <v>8</v>
+      </c>
+      <c r="O250">
+        <v>10</v>
+      </c>
+      <c r="P250">
+        <v>16</v>
+      </c>
+      <c r="Q250">
+        <v>2</v>
+      </c>
+      <c r="R250">
+        <v>6</v>
+      </c>
+      <c r="S250">
+        <v>0</v>
+      </c>
+      <c r="T250">
+        <v>2</v>
+      </c>
+      <c r="U250">
+        <v>0</v>
+      </c>
+      <c r="V250">
+        <v>1</v>
+      </c>
+      <c r="W250">
+        <v>1.62</v>
+      </c>
+      <c r="X250">
+        <v>3.75</v>
+      </c>
+      <c r="Y250">
+        <v>5.5</v>
+      </c>
+      <c r="Z250">
+        <v>1.6</v>
+      </c>
+      <c r="AA250">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AB250">
+        <v>5</v>
+      </c>
+      <c r="AC250">
+        <v>1.6</v>
+      </c>
+      <c r="AD250">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AE250">
+        <v>5</v>
+      </c>
+      <c r="AF250">
+        <v>1.5</v>
+      </c>
+      <c r="AG250">
+        <v>4</v>
+      </c>
+      <c r="AH250">
+        <v>6.1</v>
+      </c>
+      <c r="AI250">
+        <v>1.61</v>
+      </c>
+      <c r="AJ250">
+        <v>3.75</v>
+      </c>
+      <c r="AK250">
+        <v>5.5</v>
+      </c>
+      <c r="AL250">
+        <v>1.66</v>
+      </c>
+      <c r="AM250">
+        <v>4</v>
+      </c>
+      <c r="AN250">
+        <v>5.93</v>
+      </c>
+      <c r="AO250">
+        <v>1.67</v>
+      </c>
+      <c r="AP250">
+        <v>3.5</v>
+      </c>
+      <c r="AQ250">
+        <v>5.5</v>
+      </c>
+      <c r="AR250">
+        <v>1.62</v>
+      </c>
+      <c r="AS250">
+        <v>4</v>
+      </c>
+      <c r="AT250">
+        <v>5</v>
+      </c>
+      <c r="AU250">
+        <v>1.67</v>
+      </c>
+      <c r="AV250">
+        <v>3.9</v>
+      </c>
+      <c r="AW250">
+        <v>5.75</v>
+      </c>
+      <c r="AX250">
+        <v>1.62</v>
+      </c>
+      <c r="AY250">
+        <v>4</v>
+      </c>
+      <c r="AZ250">
+        <v>5.4</v>
+      </c>
+      <c r="BA250">
+        <v>38</v>
+      </c>
+      <c r="BB250">
+        <v>1.68</v>
+      </c>
+      <c r="BC250">
+        <v>1.62</v>
+      </c>
+      <c r="BD250">
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="BE250">
+        <v>3.9</v>
+      </c>
+      <c r="BF250">
+        <v>6.1</v>
+      </c>
+      <c r="BG250">
+        <v>5.42</v>
+      </c>
+      <c r="BH250">
+        <v>34</v>
+      </c>
+      <c r="BI250">
+        <v>2.14</v>
+      </c>
+      <c r="BJ250">
+        <v>2.02</v>
+      </c>
+      <c r="BK250">
+        <v>1.85</v>
+      </c>
+      <c r="BL250">
+        <v>1.79</v>
+      </c>
+      <c r="BM250">
+        <v>24</v>
+      </c>
+      <c r="BN250">
+        <v>-1</v>
+      </c>
+      <c r="BO250">
+        <v>2.23</v>
+      </c>
+      <c r="BP250">
+        <v>2.15</v>
+      </c>
+      <c r="BQ250">
+        <v>1.78</v>
+      </c>
+      <c r="BR250">
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="251" spans="1:70">
+      <c r="A251" t="s">
+        <v>70</v>
+      </c>
+      <c r="B251" s="1">
+        <v>41429</v>
+      </c>
+      <c r="C251" t="s">
+        <v>73</v>
+      </c>
+      <c r="D251" t="s">
+        <v>92</v>
+      </c>
+      <c r="E251">
+        <v>0</v>
+      </c>
+      <c r="F251">
+        <v>2</v>
+      </c>
+      <c r="G251" t="s">
+        <v>78</v>
+      </c>
+      <c r="H251">
+        <v>0</v>
+      </c>
+      <c r="I251">
+        <v>0</v>
+      </c>
+      <c r="J251" t="s">
+        <v>79</v>
+      </c>
+      <c r="K251">
+        <v>9</v>
+      </c>
+      <c r="L251">
+        <v>17</v>
+      </c>
+      <c r="M251">
+        <v>5</v>
+      </c>
+      <c r="N251">
+        <v>9</v>
+      </c>
+      <c r="O251">
+        <v>14</v>
+      </c>
+      <c r="P251">
+        <v>17</v>
+      </c>
+      <c r="Q251">
+        <v>9</v>
+      </c>
+      <c r="R251">
+        <v>5</v>
+      </c>
+      <c r="S251">
+        <v>1</v>
+      </c>
+      <c r="T251">
+        <v>1</v>
+      </c>
+      <c r="U251">
+        <v>0</v>
+      </c>
+      <c r="V251">
+        <v>0</v>
+      </c>
+      <c r="W251">
+        <v>2.6</v>
+      </c>
+      <c r="X251">
+        <v>3.4</v>
+      </c>
+      <c r="Y251">
+        <v>2.6</v>
+      </c>
+      <c r="Z251">
+        <v>2.6</v>
+      </c>
+      <c r="AA251">
+        <v>3.5</v>
+      </c>
+      <c r="AB251">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AC251">
+        <v>2.6</v>
+      </c>
+      <c r="AD251">
+        <v>3.5</v>
+      </c>
+      <c r="AE251">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AF251">
+        <v>2.75</v>
+      </c>
+      <c r="AG251">
+        <v>3.3</v>
+      </c>
+      <c r="AH251">
+        <v>2.4</v>
+      </c>
+      <c r="AI251">
+        <v>2.6</v>
+      </c>
+      <c r="AJ251">
+        <v>3.4</v>
+      </c>
+      <c r="AK251">
+        <v>2.6</v>
+      </c>
+      <c r="AL251">
+        <v>2.64</v>
+      </c>
+      <c r="AM251">
+        <v>3.69</v>
+      </c>
+      <c r="AN251">
+        <v>2.7</v>
+      </c>
+      <c r="AO251">
+        <v>2.62</v>
+      </c>
+      <c r="AP251">
+        <v>3.1</v>
+      </c>
+      <c r="AQ251">
+        <v>2.75</v>
+      </c>
+      <c r="AR251">
+        <v>2.5</v>
+      </c>
+      <c r="AS251">
+        <v>3.4</v>
+      </c>
+      <c r="AT251">
+        <v>2.6</v>
+      </c>
+      <c r="AU251">
+        <v>2.62</v>
+      </c>
+      <c r="AV251">
+        <v>3.6</v>
+      </c>
+      <c r="AW251">
+        <v>2.62</v>
+      </c>
+      <c r="AX251">
+        <v>2.6</v>
+      </c>
+      <c r="AY251">
+        <v>3.4</v>
+      </c>
+      <c r="AZ251">
+        <v>2.6</v>
+      </c>
+      <c r="BA251">
+        <v>38</v>
+      </c>
+      <c r="BB251">
+        <v>2.75</v>
+      </c>
+      <c r="BC251">
+        <v>2.6</v>
+      </c>
+      <c r="BD251">
+        <v>3.7</v>
+      </c>
+      <c r="BE251">
+        <v>3.46</v>
+      </c>
+      <c r="BF251">
+        <v>2.75</v>
+      </c>
+      <c r="BG251">
+        <v>2.59</v>
+      </c>
+      <c r="BH251">
+        <v>25</v>
+      </c>
+      <c r="BI251">
+        <v>1.6</v>
+      </c>
+      <c r="BJ251">
+        <v>1.53</v>
+      </c>
+      <c r="BK251">
+        <v>2.6</v>
+      </c>
+      <c r="BL251">
+        <v>2.4</v>
+      </c>
+      <c r="BM251">
+        <v>22</v>
+      </c>
+      <c r="BN251">
+        <v>0</v>
+      </c>
+      <c r="BO251">
+        <v>1.97</v>
+      </c>
+      <c r="BP251">
+        <v>1.93</v>
+      </c>
+      <c r="BQ251">
+        <v>1.99</v>
+      </c>
+      <c r="BR251">
+        <v>1.93</v>
+      </c>
+    </row>
+    <row r="252" spans="1:70">
+      <c r="A252" t="s">
+        <v>70</v>
+      </c>
+      <c r="B252" s="1">
+        <v>41459</v>
+      </c>
+      <c r="C252" t="s">
+        <v>91</v>
+      </c>
+      <c r="D252" t="s">
+        <v>93</v>
+      </c>
+      <c r="E252">
+        <v>0</v>
+      </c>
+      <c r="F252">
+        <v>0</v>
+      </c>
+      <c r="G252" t="s">
+        <v>79</v>
+      </c>
+      <c r="H252">
+        <v>0</v>
+      </c>
+      <c r="I252">
+        <v>0</v>
+      </c>
+      <c r="J252" t="s">
+        <v>79</v>
+      </c>
+      <c r="K252">
+        <v>13</v>
+      </c>
+      <c r="L252">
+        <v>14</v>
+      </c>
+      <c r="M252">
+        <v>1</v>
+      </c>
+      <c r="N252">
+        <v>6</v>
+      </c>
+      <c r="O252">
+        <v>22</v>
+      </c>
+      <c r="P252">
+        <v>9</v>
+      </c>
+      <c r="Q252">
+        <v>6</v>
+      </c>
+      <c r="R252">
+        <v>6</v>
+      </c>
+      <c r="S252">
+        <v>0</v>
+      </c>
+      <c r="T252">
+        <v>0</v>
+      </c>
+      <c r="U252">
+        <v>0</v>
+      </c>
+      <c r="V252">
+        <v>0</v>
+      </c>
+      <c r="W252">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="X252">
+        <v>3.3</v>
+      </c>
+      <c r="Y252">
+        <v>3.1</v>
+      </c>
+      <c r="Z252">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AA252">
+        <v>3.4</v>
+      </c>
+      <c r="AB252">
+        <v>3</v>
+      </c>
+      <c r="AC252">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AD252">
+        <v>3.4</v>
+      </c>
+      <c r="AE252">
+        <v>3</v>
+      </c>
+      <c r="AF252">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AG252">
+        <v>3.3</v>
+      </c>
+      <c r="AH252">
+        <v>3.1</v>
+      </c>
+      <c r="AI252">
+        <v>2.25</v>
+      </c>
+      <c r="AJ252">
+        <v>3.3</v>
+      </c>
+      <c r="AK252">
+        <v>3.2</v>
+      </c>
+      <c r="AL252">
+        <v>2.4</v>
+      </c>
+      <c r="AM252">
+        <v>3.51</v>
+      </c>
+      <c r="AN252">
+        <v>3.14</v>
+      </c>
+      <c r="AO252">
+        <v>2.4</v>
+      </c>
+      <c r="AP252">
+        <v>3.1</v>
+      </c>
+      <c r="AQ252">
+        <v>3.1</v>
+      </c>
+      <c r="AR252">
+        <v>2.25</v>
+      </c>
+      <c r="AS252">
+        <v>3.4</v>
+      </c>
+      <c r="AT252">
+        <v>3</v>
+      </c>
+      <c r="AU252">
+        <v>2.4</v>
+      </c>
+      <c r="AV252">
+        <v>3.5</v>
+      </c>
+      <c r="AW252">
+        <v>3</v>
+      </c>
+      <c r="AX252">
+        <v>2.25</v>
+      </c>
+      <c r="AY252">
+        <v>3.3</v>
+      </c>
+      <c r="AZ252">
+        <v>3.2</v>
+      </c>
+      <c r="BA252">
+        <v>38</v>
+      </c>
+      <c r="BB252">
+        <v>2.41</v>
+      </c>
+      <c r="BC252">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="BD252">
+        <v>3.55</v>
+      </c>
+      <c r="BE252">
+        <v>3.34</v>
+      </c>
+      <c r="BF252">
+        <v>3.23</v>
+      </c>
+      <c r="BG252">
+        <v>3.04</v>
+      </c>
+      <c r="BH252">
+        <v>33</v>
+      </c>
+      <c r="BI252">
+        <v>1.8</v>
+      </c>
+      <c r="BJ252">
+        <v>1.71</v>
+      </c>
+      <c r="BK252">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BL252">
+        <v>2.1</v>
+      </c>
+      <c r="BM252">
+        <v>23</v>
+      </c>
+      <c r="BN252">
+        <v>-0.25</v>
+      </c>
+      <c r="BO252">
+        <v>2.08</v>
+      </c>
+      <c r="BP252">
+        <v>2.04</v>
+      </c>
+      <c r="BQ252">
+        <v>1.87</v>
+      </c>
+      <c r="BR252">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="253" spans="1:70">
+      <c r="A253" t="s">
+        <v>70</v>
+      </c>
+      <c r="B253" s="1">
+        <v>41459</v>
+      </c>
+      <c r="C253" t="s">
+        <v>87</v>
+      </c>
+      <c r="D253" t="s">
+        <v>83</v>
+      </c>
+      <c r="E253">
+        <v>2</v>
+      </c>
+      <c r="F253">
+        <v>1</v>
+      </c>
+      <c r="G253" t="s">
+        <v>74</v>
+      </c>
+      <c r="H253">
+        <v>0</v>
+      </c>
+      <c r="I253">
+        <v>0</v>
+      </c>
+      <c r="J253" t="s">
+        <v>79</v>
+      </c>
+      <c r="K253">
+        <v>5</v>
+      </c>
+      <c r="L253">
+        <v>12</v>
+      </c>
+      <c r="M253">
+        <v>4</v>
+      </c>
+      <c r="N253">
+        <v>3</v>
+      </c>
+      <c r="O253">
+        <v>16</v>
+      </c>
+      <c r="P253">
+        <v>12</v>
+      </c>
+      <c r="Q253">
+        <v>2</v>
+      </c>
+      <c r="R253">
+        <v>6</v>
+      </c>
+      <c r="S253">
+        <v>2</v>
+      </c>
+      <c r="T253">
+        <v>1</v>
+      </c>
+      <c r="U253">
+        <v>0</v>
+      </c>
+      <c r="V253">
+        <v>0</v>
+      </c>
+      <c r="W253">
+        <v>2.4</v>
+      </c>
+      <c r="X253">
+        <v>3.2</v>
+      </c>
+      <c r="Y253">
+        <v>3</v>
+      </c>
+      <c r="Z253">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AA253">
+        <v>3.25</v>
+      </c>
+      <c r="AB253">
+        <v>2.85</v>
+      </c>
+      <c r="AC253">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AD253">
+        <v>3.25</v>
+      </c>
+      <c r="AE253">
+        <v>2.85</v>
+      </c>
+      <c r="AF253">
+        <v>2.4</v>
+      </c>
+      <c r="AG253">
+        <v>3.3</v>
+      </c>
+      <c r="AH253">
+        <v>2.75</v>
+      </c>
+      <c r="AI253">
+        <v>2.4</v>
+      </c>
+      <c r="AJ253">
+        <v>3.2</v>
+      </c>
+      <c r="AK253">
+        <v>3</v>
+      </c>
+      <c r="AL253">
+        <v>2.48</v>
+      </c>
+      <c r="AM253">
+        <v>3.35</v>
+      </c>
+      <c r="AN253">
+        <v>3.14</v>
+      </c>
+      <c r="AO253">
+        <v>2.5</v>
+      </c>
+      <c r="AP253">
+        <v>3.2</v>
+      </c>
+      <c r="AQ253">
+        <v>2.8</v>
+      </c>
+      <c r="AR253">
+        <v>2.4</v>
+      </c>
+      <c r="AS253">
+        <v>3.3</v>
+      </c>
+      <c r="AT253">
+        <v>2.88</v>
+      </c>
+      <c r="AU253">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AV253">
+        <v>3.3</v>
+      </c>
+      <c r="AW253">
+        <v>3.12</v>
+      </c>
+      <c r="AX253">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AY253">
+        <v>3.25</v>
+      </c>
+      <c r="AZ253">
+        <v>3.1</v>
+      </c>
+      <c r="BA253">
+        <v>38</v>
+      </c>
+      <c r="BB253">
+        <v>2.5</v>
+      </c>
+      <c r="BC253">
+        <v>2.41</v>
+      </c>
+      <c r="BD253">
+        <v>3.4</v>
+      </c>
+      <c r="BE253">
+        <v>3.26</v>
+      </c>
+      <c r="BF253">
+        <v>3.2</v>
+      </c>
+      <c r="BG253">
+        <v>2.96</v>
+      </c>
+      <c r="BH253">
+        <v>32</v>
+      </c>
+      <c r="BI253">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="BJ253">
+        <v>2.14</v>
+      </c>
+      <c r="BK253">
+        <v>1.76</v>
+      </c>
+      <c r="BL253">
+        <v>1.69</v>
+      </c>
+      <c r="BM253">
+        <v>23</v>
+      </c>
+      <c r="BN253">
+        <v>-0.25</v>
+      </c>
+      <c r="BO253">
+        <v>2.11</v>
+      </c>
+      <c r="BP253">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="BQ253">
+        <v>1.86</v>
+      </c>
+      <c r="BR253">
+        <v>1.81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se modifico encontrarPartido porque incluia el partido que se queria predecir. La precision bajo a 50%
</commit_message>
<xml_diff>
--- a/DatosAle1/DP1213.xlsx
+++ b/DatosAle1/DP1213.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="8220"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="19155" windowHeight="8505"/>
   </bookViews>
   <sheets>
     <sheet name="D1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="143">
   <si>
     <t>Div</t>
   </si>
@@ -437,6 +437,12 @@
   </si>
   <si>
     <t>31/03/13</t>
+  </si>
+  <si>
+    <t>13/04/13</t>
+  </si>
+  <si>
+    <t>14/04/13</t>
   </si>
 </sst>
 </file>
@@ -1259,9 +1265,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BR253"/>
+  <dimension ref="A1:BR262"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C254" sqref="C254:C262"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -54901,6 +54909,1914 @@
         <v>1.81</v>
       </c>
     </row>
+    <row r="254" spans="1:70">
+      <c r="A254" t="s">
+        <v>70</v>
+      </c>
+      <c r="B254" s="1">
+        <v>41612</v>
+      </c>
+      <c r="C254" t="s">
+        <v>82</v>
+      </c>
+      <c r="D254" t="s">
+        <v>91</v>
+      </c>
+      <c r="E254">
+        <v>3</v>
+      </c>
+      <c r="F254">
+        <v>1</v>
+      </c>
+      <c r="G254" t="s">
+        <v>74</v>
+      </c>
+      <c r="H254">
+        <v>2</v>
+      </c>
+      <c r="I254">
+        <v>1</v>
+      </c>
+      <c r="J254" t="s">
+        <v>74</v>
+      </c>
+      <c r="K254">
+        <v>15</v>
+      </c>
+      <c r="L254">
+        <v>10</v>
+      </c>
+      <c r="M254">
+        <v>5</v>
+      </c>
+      <c r="N254">
+        <v>3</v>
+      </c>
+      <c r="O254">
+        <v>13</v>
+      </c>
+      <c r="P254">
+        <v>23</v>
+      </c>
+      <c r="Q254">
+        <v>6</v>
+      </c>
+      <c r="R254">
+        <v>4</v>
+      </c>
+      <c r="S254">
+        <v>1</v>
+      </c>
+      <c r="T254">
+        <v>2</v>
+      </c>
+      <c r="U254">
+        <v>0</v>
+      </c>
+      <c r="V254">
+        <v>0</v>
+      </c>
+      <c r="W254">
+        <v>1.7</v>
+      </c>
+      <c r="X254">
+        <v>3.6</v>
+      </c>
+      <c r="Y254">
+        <v>5</v>
+      </c>
+      <c r="Z254">
+        <v>1.72</v>
+      </c>
+      <c r="AA254">
+        <v>3.7</v>
+      </c>
+      <c r="AB254">
+        <v>4.75</v>
+      </c>
+      <c r="AC254">
+        <v>1.72</v>
+      </c>
+      <c r="AD254">
+        <v>3.7</v>
+      </c>
+      <c r="AE254">
+        <v>4.75</v>
+      </c>
+      <c r="AF254">
+        <v>1.9</v>
+      </c>
+      <c r="AG254">
+        <v>3.6</v>
+      </c>
+      <c r="AH254">
+        <v>3.6</v>
+      </c>
+      <c r="AI254">
+        <v>1.66</v>
+      </c>
+      <c r="AJ254">
+        <v>3.75</v>
+      </c>
+      <c r="AK254">
+        <v>5</v>
+      </c>
+      <c r="AL254">
+        <v>1.71</v>
+      </c>
+      <c r="AM254">
+        <v>3.9</v>
+      </c>
+      <c r="AN254">
+        <v>5.55</v>
+      </c>
+      <c r="AO254">
+        <v>1.67</v>
+      </c>
+      <c r="AP254">
+        <v>3.8</v>
+      </c>
+      <c r="AQ254">
+        <v>5</v>
+      </c>
+      <c r="AR254">
+        <v>1.67</v>
+      </c>
+      <c r="AS254">
+        <v>3.6</v>
+      </c>
+      <c r="AT254">
+        <v>5</v>
+      </c>
+      <c r="AU254">
+        <v>1.7</v>
+      </c>
+      <c r="AV254">
+        <v>3.9</v>
+      </c>
+      <c r="AW254">
+        <v>5.5</v>
+      </c>
+      <c r="AX254">
+        <v>1.73</v>
+      </c>
+      <c r="AY254">
+        <v>3.6</v>
+      </c>
+      <c r="AZ254">
+        <v>4.75</v>
+      </c>
+      <c r="BA254">
+        <v>39</v>
+      </c>
+      <c r="BB254">
+        <v>1.9</v>
+      </c>
+      <c r="BC254">
+        <v>1.71</v>
+      </c>
+      <c r="BD254">
+        <v>3.95</v>
+      </c>
+      <c r="BE254">
+        <v>3.74</v>
+      </c>
+      <c r="BF254">
+        <v>5.55</v>
+      </c>
+      <c r="BG254">
+        <v>4.93</v>
+      </c>
+      <c r="BH254">
+        <v>36</v>
+      </c>
+      <c r="BI254">
+        <v>1.94</v>
+      </c>
+      <c r="BJ254">
+        <v>1.87</v>
+      </c>
+      <c r="BK254">
+        <v>2.04</v>
+      </c>
+      <c r="BL254">
+        <v>1.93</v>
+      </c>
+      <c r="BM254">
+        <v>24</v>
+      </c>
+      <c r="BN254">
+        <v>-0.75</v>
+      </c>
+      <c r="BO254">
+        <v>1.94</v>
+      </c>
+      <c r="BP254">
+        <v>1.91</v>
+      </c>
+      <c r="BQ254">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="BR254">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="255" spans="1:70">
+      <c r="A255" t="s">
+        <v>70</v>
+      </c>
+      <c r="B255" t="s">
+        <v>141</v>
+      </c>
+      <c r="C255" t="s">
+        <v>85</v>
+      </c>
+      <c r="D255" t="s">
+        <v>87</v>
+      </c>
+      <c r="E255">
+        <v>4</v>
+      </c>
+      <c r="F255">
+        <v>0</v>
+      </c>
+      <c r="G255" t="s">
+        <v>74</v>
+      </c>
+      <c r="H255">
+        <v>3</v>
+      </c>
+      <c r="I255">
+        <v>0</v>
+      </c>
+      <c r="J255" t="s">
+        <v>74</v>
+      </c>
+      <c r="K255">
+        <v>21</v>
+      </c>
+      <c r="L255">
+        <v>9</v>
+      </c>
+      <c r="M255">
+        <v>10</v>
+      </c>
+      <c r="N255">
+        <v>4</v>
+      </c>
+      <c r="O255">
+        <v>11</v>
+      </c>
+      <c r="P255">
+        <v>14</v>
+      </c>
+      <c r="Q255">
+        <v>12</v>
+      </c>
+      <c r="R255">
+        <v>4</v>
+      </c>
+      <c r="S255">
+        <v>1</v>
+      </c>
+      <c r="T255">
+        <v>2</v>
+      </c>
+      <c r="U255">
+        <v>0</v>
+      </c>
+      <c r="V255">
+        <v>0</v>
+      </c>
+      <c r="W255">
+        <v>1.22</v>
+      </c>
+      <c r="X255">
+        <v>6</v>
+      </c>
+      <c r="Y255">
+        <v>13</v>
+      </c>
+      <c r="Z255">
+        <v>1.22</v>
+      </c>
+      <c r="AA255">
+        <v>6.75</v>
+      </c>
+      <c r="AB255">
+        <v>10.5</v>
+      </c>
+      <c r="AC255">
+        <v>1.22</v>
+      </c>
+      <c r="AD255">
+        <v>6.75</v>
+      </c>
+      <c r="AE255">
+        <v>10.5</v>
+      </c>
+      <c r="AF255">
+        <v>1.2</v>
+      </c>
+      <c r="AG255">
+        <v>5.8</v>
+      </c>
+      <c r="AH255">
+        <v>13</v>
+      </c>
+      <c r="AI255">
+        <v>1.2</v>
+      </c>
+      <c r="AJ255">
+        <v>6.5</v>
+      </c>
+      <c r="AK255">
+        <v>13</v>
+      </c>
+      <c r="AL255">
+        <v>1.24</v>
+      </c>
+      <c r="AM255">
+        <v>6.85</v>
+      </c>
+      <c r="AN255">
+        <v>15.5</v>
+      </c>
+      <c r="AO255">
+        <v>1.25</v>
+      </c>
+      <c r="AP255">
+        <v>5.5</v>
+      </c>
+      <c r="AQ255">
+        <v>12</v>
+      </c>
+      <c r="AR255">
+        <v>1.2</v>
+      </c>
+      <c r="AS255">
+        <v>6</v>
+      </c>
+      <c r="AT255">
+        <v>12</v>
+      </c>
+      <c r="AU255">
+        <v>1.22</v>
+      </c>
+      <c r="AV255">
+        <v>6.5</v>
+      </c>
+      <c r="AW255">
+        <v>15</v>
+      </c>
+      <c r="AX255">
+        <v>1.2</v>
+      </c>
+      <c r="AY255">
+        <v>6.5</v>
+      </c>
+      <c r="AZ255">
+        <v>13</v>
+      </c>
+      <c r="BA255">
+        <v>39</v>
+      </c>
+      <c r="BB255">
+        <v>1.25</v>
+      </c>
+      <c r="BC255">
+        <v>1.22</v>
+      </c>
+      <c r="BD255">
+        <v>6.9</v>
+      </c>
+      <c r="BE255">
+        <v>6.18</v>
+      </c>
+      <c r="BF255">
+        <v>16</v>
+      </c>
+      <c r="BG255">
+        <v>13.12</v>
+      </c>
+      <c r="BH255">
+        <v>29</v>
+      </c>
+      <c r="BI255">
+        <v>1.53</v>
+      </c>
+      <c r="BJ255">
+        <v>1.46</v>
+      </c>
+      <c r="BK255">
+        <v>2.78</v>
+      </c>
+      <c r="BL255">
+        <v>2.57</v>
+      </c>
+      <c r="BM255">
+        <v>25</v>
+      </c>
+      <c r="BN255">
+        <v>-2</v>
+      </c>
+      <c r="BO255">
+        <v>2.13</v>
+      </c>
+      <c r="BP255">
+        <v>2.06</v>
+      </c>
+      <c r="BQ255">
+        <v>1.86</v>
+      </c>
+      <c r="BR255">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="256" spans="1:70">
+      <c r="A256" t="s">
+        <v>70</v>
+      </c>
+      <c r="B256" t="s">
+        <v>141</v>
+      </c>
+      <c r="C256" t="s">
+        <v>77</v>
+      </c>
+      <c r="D256" t="s">
+        <v>73</v>
+      </c>
+      <c r="E256">
+        <v>2</v>
+      </c>
+      <c r="F256">
+        <v>2</v>
+      </c>
+      <c r="G256" t="s">
+        <v>79</v>
+      </c>
+      <c r="H256">
+        <v>1</v>
+      </c>
+      <c r="I256">
+        <v>1</v>
+      </c>
+      <c r="J256" t="s">
+        <v>79</v>
+      </c>
+      <c r="K256">
+        <v>8</v>
+      </c>
+      <c r="L256">
+        <v>16</v>
+      </c>
+      <c r="M256">
+        <v>3</v>
+      </c>
+      <c r="N256">
+        <v>4</v>
+      </c>
+      <c r="O256">
+        <v>20</v>
+      </c>
+      <c r="P256">
+        <v>24</v>
+      </c>
+      <c r="Q256">
+        <v>3</v>
+      </c>
+      <c r="R256">
+        <v>1</v>
+      </c>
+      <c r="S256">
+        <v>1</v>
+      </c>
+      <c r="T256">
+        <v>3</v>
+      </c>
+      <c r="U256">
+        <v>0</v>
+      </c>
+      <c r="V256">
+        <v>0</v>
+      </c>
+      <c r="W256">
+        <v>2.8</v>
+      </c>
+      <c r="X256">
+        <v>3.3</v>
+      </c>
+      <c r="Y256">
+        <v>2.5</v>
+      </c>
+      <c r="Z256">
+        <v>2.7</v>
+      </c>
+      <c r="AA256">
+        <v>3.5</v>
+      </c>
+      <c r="AB256">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AC256">
+        <v>2.7</v>
+      </c>
+      <c r="AD256">
+        <v>3.5</v>
+      </c>
+      <c r="AE256">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AF256">
+        <v>2.6</v>
+      </c>
+      <c r="AG256">
+        <v>3.2</v>
+      </c>
+      <c r="AH256">
+        <v>2.6</v>
+      </c>
+      <c r="AI256">
+        <v>2.75</v>
+      </c>
+      <c r="AJ256">
+        <v>3.3</v>
+      </c>
+      <c r="AK256">
+        <v>2.5</v>
+      </c>
+      <c r="AL256">
+        <v>2.93</v>
+      </c>
+      <c r="AM256">
+        <v>3.55</v>
+      </c>
+      <c r="AN256">
+        <v>2.52</v>
+      </c>
+      <c r="AO256">
+        <v>2.8</v>
+      </c>
+      <c r="AP256">
+        <v>3.2</v>
+      </c>
+      <c r="AQ256">
+        <v>2.5</v>
+      </c>
+      <c r="AR256">
+        <v>2.8</v>
+      </c>
+      <c r="AS256">
+        <v>3.4</v>
+      </c>
+      <c r="AT256">
+        <v>2.4</v>
+      </c>
+      <c r="AU256">
+        <v>2.9</v>
+      </c>
+      <c r="AV256">
+        <v>3.5</v>
+      </c>
+      <c r="AW256">
+        <v>2.5</v>
+      </c>
+      <c r="AX256">
+        <v>2.8</v>
+      </c>
+      <c r="AY256">
+        <v>3.3</v>
+      </c>
+      <c r="AZ256">
+        <v>2.5</v>
+      </c>
+      <c r="BA256">
+        <v>39</v>
+      </c>
+      <c r="BB256">
+        <v>2.94</v>
+      </c>
+      <c r="BC256">
+        <v>2.79</v>
+      </c>
+      <c r="BD256">
+        <v>3.55</v>
+      </c>
+      <c r="BE256">
+        <v>3.34</v>
+      </c>
+      <c r="BF256">
+        <v>2.6</v>
+      </c>
+      <c r="BG256">
+        <v>2.48</v>
+      </c>
+      <c r="BH256">
+        <v>34</v>
+      </c>
+      <c r="BI256">
+        <v>1.8</v>
+      </c>
+      <c r="BJ256">
+        <v>1.73</v>
+      </c>
+      <c r="BK256">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="BL256">
+        <v>2.08</v>
+      </c>
+      <c r="BM256">
+        <v>24</v>
+      </c>
+      <c r="BN256">
+        <v>0.25</v>
+      </c>
+      <c r="BO256">
+        <v>1.79</v>
+      </c>
+      <c r="BP256">
+        <v>1.75</v>
+      </c>
+      <c r="BQ256">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BR256">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="257" spans="1:70">
+      <c r="A257" t="s">
+        <v>70</v>
+      </c>
+      <c r="B257" t="s">
+        <v>141</v>
+      </c>
+      <c r="C257" t="s">
+        <v>84</v>
+      </c>
+      <c r="D257" t="s">
+        <v>72</v>
+      </c>
+      <c r="E257">
+        <v>1</v>
+      </c>
+      <c r="F257">
+        <v>6</v>
+      </c>
+      <c r="G257" t="s">
+        <v>78</v>
+      </c>
+      <c r="H257">
+        <v>0</v>
+      </c>
+      <c r="I257">
+        <v>5</v>
+      </c>
+      <c r="J257" t="s">
+        <v>78</v>
+      </c>
+      <c r="K257">
+        <v>9</v>
+      </c>
+      <c r="L257">
+        <v>15</v>
+      </c>
+      <c r="M257">
+        <v>3</v>
+      </c>
+      <c r="N257">
+        <v>9</v>
+      </c>
+      <c r="O257">
+        <v>12</v>
+      </c>
+      <c r="P257">
+        <v>11</v>
+      </c>
+      <c r="Q257">
+        <v>1</v>
+      </c>
+      <c r="R257">
+        <v>5</v>
+      </c>
+      <c r="S257">
+        <v>0</v>
+      </c>
+      <c r="T257">
+        <v>1</v>
+      </c>
+      <c r="U257">
+        <v>0</v>
+      </c>
+      <c r="V257">
+        <v>0</v>
+      </c>
+      <c r="W257">
+        <v>7.5</v>
+      </c>
+      <c r="X257">
+        <v>4.75</v>
+      </c>
+      <c r="Y257">
+        <v>1.4</v>
+      </c>
+      <c r="Z257">
+        <v>6.75</v>
+      </c>
+      <c r="AA257">
+        <v>5</v>
+      </c>
+      <c r="AB257">
+        <v>1.4</v>
+      </c>
+      <c r="AC257">
+        <v>6.75</v>
+      </c>
+      <c r="AD257">
+        <v>5</v>
+      </c>
+      <c r="AE257">
+        <v>1.4</v>
+      </c>
+      <c r="AF257">
+        <v>7</v>
+      </c>
+      <c r="AG257">
+        <v>4</v>
+      </c>
+      <c r="AH257">
+        <v>1.45</v>
+      </c>
+      <c r="AI257">
+        <v>7</v>
+      </c>
+      <c r="AJ257">
+        <v>4.33</v>
+      </c>
+      <c r="AK257">
+        <v>1.44</v>
+      </c>
+      <c r="AL257">
+        <v>7.83</v>
+      </c>
+      <c r="AM257">
+        <v>4.79</v>
+      </c>
+      <c r="AN257">
+        <v>1.46</v>
+      </c>
+      <c r="AO257">
+        <v>7</v>
+      </c>
+      <c r="AP257">
+        <v>4.33</v>
+      </c>
+      <c r="AQ257">
+        <v>1.44</v>
+      </c>
+      <c r="AR257">
+        <v>7.5</v>
+      </c>
+      <c r="AS257">
+        <v>4.33</v>
+      </c>
+      <c r="AT257">
+        <v>1.4</v>
+      </c>
+      <c r="AU257">
+        <v>8</v>
+      </c>
+      <c r="AV257">
+        <v>4.75</v>
+      </c>
+      <c r="AW257">
+        <v>1.44</v>
+      </c>
+      <c r="AX257">
+        <v>7</v>
+      </c>
+      <c r="AY257">
+        <v>4.33</v>
+      </c>
+      <c r="AZ257">
+        <v>1.44</v>
+      </c>
+      <c r="BA257">
+        <v>39</v>
+      </c>
+      <c r="BB257">
+        <v>8</v>
+      </c>
+      <c r="BC257">
+        <v>7.34</v>
+      </c>
+      <c r="BD257">
+        <v>4.83</v>
+      </c>
+      <c r="BE257">
+        <v>4.41</v>
+      </c>
+      <c r="BF257">
+        <v>1.47</v>
+      </c>
+      <c r="BG257">
+        <v>1.44</v>
+      </c>
+      <c r="BH257">
+        <v>34</v>
+      </c>
+      <c r="BI257">
+        <v>1.7</v>
+      </c>
+      <c r="BJ257">
+        <v>1.64</v>
+      </c>
+      <c r="BK257">
+        <v>2.36</v>
+      </c>
+      <c r="BL257">
+        <v>2.23</v>
+      </c>
+      <c r="BM257">
+        <v>25</v>
+      </c>
+      <c r="BN257">
+        <v>1.5</v>
+      </c>
+      <c r="BO257">
+        <v>1.74</v>
+      </c>
+      <c r="BP257">
+        <v>1.69</v>
+      </c>
+      <c r="BQ257">
+        <v>2.29</v>
+      </c>
+      <c r="BR257">
+        <v>2.2200000000000002</v>
+      </c>
+    </row>
+    <row r="258" spans="1:70">
+      <c r="A258" t="s">
+        <v>70</v>
+      </c>
+      <c r="B258" t="s">
+        <v>141</v>
+      </c>
+      <c r="C258" t="s">
+        <v>83</v>
+      </c>
+      <c r="D258" t="s">
+        <v>86</v>
+      </c>
+      <c r="E258">
+        <v>1</v>
+      </c>
+      <c r="F258">
+        <v>2</v>
+      </c>
+      <c r="G258" t="s">
+        <v>78</v>
+      </c>
+      <c r="H258">
+        <v>0</v>
+      </c>
+      <c r="I258">
+        <v>0</v>
+      </c>
+      <c r="J258" t="s">
+        <v>79</v>
+      </c>
+      <c r="K258">
+        <v>12</v>
+      </c>
+      <c r="L258">
+        <v>12</v>
+      </c>
+      <c r="M258">
+        <v>2</v>
+      </c>
+      <c r="N258">
+        <v>4</v>
+      </c>
+      <c r="O258">
+        <v>15</v>
+      </c>
+      <c r="P258">
+        <v>16</v>
+      </c>
+      <c r="Q258">
+        <v>2</v>
+      </c>
+      <c r="R258">
+        <v>1</v>
+      </c>
+      <c r="S258">
+        <v>2</v>
+      </c>
+      <c r="T258">
+        <v>1</v>
+      </c>
+      <c r="U258">
+        <v>0</v>
+      </c>
+      <c r="V258">
+        <v>0</v>
+      </c>
+      <c r="W258">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="X258">
+        <v>3.4</v>
+      </c>
+      <c r="Y258">
+        <v>3.6</v>
+      </c>
+      <c r="Z258">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AA258">
+        <v>3.5</v>
+      </c>
+      <c r="AB258">
+        <v>3.4</v>
+      </c>
+      <c r="AC258">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AD258">
+        <v>3.5</v>
+      </c>
+      <c r="AE258">
+        <v>3.4</v>
+      </c>
+      <c r="AF258">
+        <v>2.15</v>
+      </c>
+      <c r="AG258">
+        <v>3.3</v>
+      </c>
+      <c r="AH258">
+        <v>3.2</v>
+      </c>
+      <c r="AI258">
+        <v>2.1</v>
+      </c>
+      <c r="AJ258">
+        <v>3.3</v>
+      </c>
+      <c r="AK258">
+        <v>3.5</v>
+      </c>
+      <c r="AL258">
+        <v>2.08</v>
+      </c>
+      <c r="AM258">
+        <v>3.61</v>
+      </c>
+      <c r="AN258">
+        <v>3.81</v>
+      </c>
+      <c r="AO258">
+        <v>2.15</v>
+      </c>
+      <c r="AP258">
+        <v>3.3</v>
+      </c>
+      <c r="AQ258">
+        <v>3.4</v>
+      </c>
+      <c r="AR258">
+        <v>2</v>
+      </c>
+      <c r="AS258">
+        <v>3.3</v>
+      </c>
+      <c r="AT258">
+        <v>3.6</v>
+      </c>
+      <c r="AU258">
+        <v>2.15</v>
+      </c>
+      <c r="AV258">
+        <v>3.5</v>
+      </c>
+      <c r="AW258">
+        <v>3.7</v>
+      </c>
+      <c r="AX258">
+        <v>2.1</v>
+      </c>
+      <c r="AY258">
+        <v>3.4</v>
+      </c>
+      <c r="AZ258">
+        <v>3.4</v>
+      </c>
+      <c r="BA258">
+        <v>39</v>
+      </c>
+      <c r="BB258">
+        <v>2.15</v>
+      </c>
+      <c r="BC258">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="BD258">
+        <v>3.61</v>
+      </c>
+      <c r="BE258">
+        <v>3.4</v>
+      </c>
+      <c r="BF258">
+        <v>3.81</v>
+      </c>
+      <c r="BG258">
+        <v>3.52</v>
+      </c>
+      <c r="BH258">
+        <v>36</v>
+      </c>
+      <c r="BI258">
+        <v>2.11</v>
+      </c>
+      <c r="BJ258">
+        <v>2.04</v>
+      </c>
+      <c r="BK258">
+        <v>1.85</v>
+      </c>
+      <c r="BL258">
+        <v>1.77</v>
+      </c>
+      <c r="BM258">
+        <v>24</v>
+      </c>
+      <c r="BN258">
+        <v>-0.25</v>
+      </c>
+      <c r="BO258">
+        <v>1.83</v>
+      </c>
+      <c r="BP258">
+        <v>1.78</v>
+      </c>
+      <c r="BQ258">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="BR258">
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="259" spans="1:70">
+      <c r="A259" t="s">
+        <v>70</v>
+      </c>
+      <c r="B259" t="s">
+        <v>141</v>
+      </c>
+      <c r="C259" t="s">
+        <v>92</v>
+      </c>
+      <c r="D259" t="s">
+        <v>81</v>
+      </c>
+      <c r="E259">
+        <v>2</v>
+      </c>
+      <c r="F259">
+        <v>2</v>
+      </c>
+      <c r="G259" t="s">
+        <v>79</v>
+      </c>
+      <c r="H259">
+        <v>0</v>
+      </c>
+      <c r="I259">
+        <v>1</v>
+      </c>
+      <c r="J259" t="s">
+        <v>78</v>
+      </c>
+      <c r="K259">
+        <v>16</v>
+      </c>
+      <c r="L259">
+        <v>18</v>
+      </c>
+      <c r="M259">
+        <v>9</v>
+      </c>
+      <c r="N259">
+        <v>8</v>
+      </c>
+      <c r="O259">
+        <v>11</v>
+      </c>
+      <c r="P259">
+        <v>14</v>
+      </c>
+      <c r="Q259">
+        <v>7</v>
+      </c>
+      <c r="R259">
+        <v>7</v>
+      </c>
+      <c r="S259">
+        <v>2</v>
+      </c>
+      <c r="T259">
+        <v>3</v>
+      </c>
+      <c r="U259">
+        <v>0</v>
+      </c>
+      <c r="V259">
+        <v>1</v>
+      </c>
+      <c r="W259">
+        <v>2.25</v>
+      </c>
+      <c r="X259">
+        <v>3.4</v>
+      </c>
+      <c r="Y259">
+        <v>3.1</v>
+      </c>
+      <c r="Z259">
+        <v>2.4</v>
+      </c>
+      <c r="AA259">
+        <v>3.4</v>
+      </c>
+      <c r="AB259">
+        <v>2.85</v>
+      </c>
+      <c r="AC259">
+        <v>2.4</v>
+      </c>
+      <c r="AD259">
+        <v>3.4</v>
+      </c>
+      <c r="AE259">
+        <v>2.85</v>
+      </c>
+      <c r="AF259">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AG259">
+        <v>3.3</v>
+      </c>
+      <c r="AH259">
+        <v>3.1</v>
+      </c>
+      <c r="AI259">
+        <v>2.25</v>
+      </c>
+      <c r="AJ259">
+        <v>3.4</v>
+      </c>
+      <c r="AK259">
+        <v>3.1</v>
+      </c>
+      <c r="AL259">
+        <v>2.44</v>
+      </c>
+      <c r="AM259">
+        <v>3.57</v>
+      </c>
+      <c r="AN259">
+        <v>3.03</v>
+      </c>
+      <c r="AO259">
+        <v>2.4</v>
+      </c>
+      <c r="AP259">
+        <v>3.2</v>
+      </c>
+      <c r="AQ259">
+        <v>3</v>
+      </c>
+      <c r="AR259">
+        <v>2.38</v>
+      </c>
+      <c r="AS259">
+        <v>3.3</v>
+      </c>
+      <c r="AT259">
+        <v>2.88</v>
+      </c>
+      <c r="AU259">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AV259">
+        <v>3.5</v>
+      </c>
+      <c r="AW259">
+        <v>2.9</v>
+      </c>
+      <c r="AX259">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AY259">
+        <v>3.4</v>
+      </c>
+      <c r="AZ259">
+        <v>3.2</v>
+      </c>
+      <c r="BA259">
+        <v>39</v>
+      </c>
+      <c r="BB259">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="BC259">
+        <v>2.34</v>
+      </c>
+      <c r="BD259">
+        <v>3.6</v>
+      </c>
+      <c r="BE259">
+        <v>3.38</v>
+      </c>
+      <c r="BF259">
+        <v>3.15</v>
+      </c>
+      <c r="BG259">
+        <v>2.98</v>
+      </c>
+      <c r="BH259">
+        <v>34</v>
+      </c>
+      <c r="BI259">
+        <v>1.75</v>
+      </c>
+      <c r="BJ259">
+        <v>1.67</v>
+      </c>
+      <c r="BK259">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="BL259">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="BM259">
+        <v>24</v>
+      </c>
+      <c r="BN259">
+        <v>-0.25</v>
+      </c>
+      <c r="BO259">
+        <v>2.12</v>
+      </c>
+      <c r="BP259">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="BQ259">
+        <v>1.85</v>
+      </c>
+      <c r="BR259">
+        <v>1.81</v>
+      </c>
+    </row>
+    <row r="260" spans="1:70">
+      <c r="A260" t="s">
+        <v>70</v>
+      </c>
+      <c r="B260" t="s">
+        <v>141</v>
+      </c>
+      <c r="C260" t="s">
+        <v>94</v>
+      </c>
+      <c r="D260" t="s">
+        <v>89</v>
+      </c>
+      <c r="E260">
+        <v>2</v>
+      </c>
+      <c r="F260">
+        <v>2</v>
+      </c>
+      <c r="G260" t="s">
+        <v>79</v>
+      </c>
+      <c r="H260">
+        <v>1</v>
+      </c>
+      <c r="I260">
+        <v>1</v>
+      </c>
+      <c r="J260" t="s">
+        <v>79</v>
+      </c>
+      <c r="K260">
+        <v>13</v>
+      </c>
+      <c r="L260">
+        <v>10</v>
+      </c>
+      <c r="M260">
+        <v>5</v>
+      </c>
+      <c r="N260">
+        <v>5</v>
+      </c>
+      <c r="O260">
+        <v>24</v>
+      </c>
+      <c r="P260">
+        <v>24</v>
+      </c>
+      <c r="Q260">
+        <v>2</v>
+      </c>
+      <c r="R260">
+        <v>4</v>
+      </c>
+      <c r="S260">
+        <v>2</v>
+      </c>
+      <c r="T260">
+        <v>1</v>
+      </c>
+      <c r="U260">
+        <v>0</v>
+      </c>
+      <c r="V260">
+        <v>0</v>
+      </c>
+      <c r="W260">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="X260">
+        <v>3.3</v>
+      </c>
+      <c r="Y260">
+        <v>3.3</v>
+      </c>
+      <c r="Z260">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AA260">
+        <v>3.4</v>
+      </c>
+      <c r="AB260">
+        <v>3.5</v>
+      </c>
+      <c r="AC260">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AD260">
+        <v>3.4</v>
+      </c>
+      <c r="AE260">
+        <v>3.5</v>
+      </c>
+      <c r="AF260">
+        <v>2.1</v>
+      </c>
+      <c r="AG260">
+        <v>3.4</v>
+      </c>
+      <c r="AH260">
+        <v>3.2</v>
+      </c>
+      <c r="AI260">
+        <v>2.1</v>
+      </c>
+      <c r="AJ260">
+        <v>3.3</v>
+      </c>
+      <c r="AK260">
+        <v>3.5</v>
+      </c>
+      <c r="AL260">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AM260">
+        <v>3.53</v>
+      </c>
+      <c r="AN260">
+        <v>3.54</v>
+      </c>
+      <c r="AO260">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AP260">
+        <v>3.3</v>
+      </c>
+      <c r="AQ260">
+        <v>3.3</v>
+      </c>
+      <c r="AR260">
+        <v>2.1</v>
+      </c>
+      <c r="AS260">
+        <v>3.3</v>
+      </c>
+      <c r="AT260">
+        <v>3.3</v>
+      </c>
+      <c r="AU260">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AV260">
+        <v>3.5</v>
+      </c>
+      <c r="AW260">
+        <v>3.5</v>
+      </c>
+      <c r="AX260">
+        <v>2.1</v>
+      </c>
+      <c r="AY260">
+        <v>3.4</v>
+      </c>
+      <c r="AZ260">
+        <v>3.4</v>
+      </c>
+      <c r="BA260">
+        <v>39</v>
+      </c>
+      <c r="BB260">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="BC260">
+        <v>2.14</v>
+      </c>
+      <c r="BD260">
+        <v>3.52</v>
+      </c>
+      <c r="BE260">
+        <v>3.38</v>
+      </c>
+      <c r="BF260">
+        <v>3.75</v>
+      </c>
+      <c r="BG260">
+        <v>3.38</v>
+      </c>
+      <c r="BH260">
+        <v>36</v>
+      </c>
+      <c r="BI260">
+        <v>2</v>
+      </c>
+      <c r="BJ260">
+        <v>1.93</v>
+      </c>
+      <c r="BK260">
+        <v>1.96</v>
+      </c>
+      <c r="BL260">
+        <v>1.87</v>
+      </c>
+      <c r="BM260">
+        <v>24</v>
+      </c>
+      <c r="BN260">
+        <v>-0.25</v>
+      </c>
+      <c r="BO260">
+        <v>1.92</v>
+      </c>
+      <c r="BP260">
+        <v>1.86</v>
+      </c>
+      <c r="BQ260">
+        <v>2.06</v>
+      </c>
+      <c r="BR260">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="261" spans="1:70">
+      <c r="A261" t="s">
+        <v>70</v>
+      </c>
+      <c r="B261" t="s">
+        <v>142</v>
+      </c>
+      <c r="C261" t="s">
+        <v>76</v>
+      </c>
+      <c r="D261" t="s">
+        <v>80</v>
+      </c>
+      <c r="E261">
+        <v>2</v>
+      </c>
+      <c r="F261">
+        <v>0</v>
+      </c>
+      <c r="G261" t="s">
+        <v>74</v>
+      </c>
+      <c r="H261">
+        <v>1</v>
+      </c>
+      <c r="I261">
+        <v>0</v>
+      </c>
+      <c r="J261" t="s">
+        <v>74</v>
+      </c>
+      <c r="K261">
+        <v>19</v>
+      </c>
+      <c r="L261">
+        <v>8</v>
+      </c>
+      <c r="M261">
+        <v>4</v>
+      </c>
+      <c r="N261">
+        <v>3</v>
+      </c>
+      <c r="O261">
+        <v>12</v>
+      </c>
+      <c r="P261">
+        <v>18</v>
+      </c>
+      <c r="Q261">
+        <v>5</v>
+      </c>
+      <c r="R261">
+        <v>3</v>
+      </c>
+      <c r="S261">
+        <v>3</v>
+      </c>
+      <c r="T261">
+        <v>2</v>
+      </c>
+      <c r="U261">
+        <v>0</v>
+      </c>
+      <c r="V261">
+        <v>0</v>
+      </c>
+      <c r="W261">
+        <v>2.38</v>
+      </c>
+      <c r="X261">
+        <v>3.25</v>
+      </c>
+      <c r="Y261">
+        <v>3</v>
+      </c>
+      <c r="Z261">
+        <v>2.4</v>
+      </c>
+      <c r="AA261">
+        <v>3.4</v>
+      </c>
+      <c r="AB261">
+        <v>2.85</v>
+      </c>
+      <c r="AC261">
+        <v>2.4</v>
+      </c>
+      <c r="AD261">
+        <v>3.4</v>
+      </c>
+      <c r="AE261">
+        <v>2.85</v>
+      </c>
+      <c r="AF261">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AG261">
+        <v>3.3</v>
+      </c>
+      <c r="AH261">
+        <v>2.9</v>
+      </c>
+      <c r="AI261">
+        <v>2.37</v>
+      </c>
+      <c r="AJ261">
+        <v>3.25</v>
+      </c>
+      <c r="AK261">
+        <v>3</v>
+      </c>
+      <c r="AL261">
+        <v>2.41</v>
+      </c>
+      <c r="AM261">
+        <v>3.42</v>
+      </c>
+      <c r="AN261">
+        <v>3.2</v>
+      </c>
+      <c r="AO261">
+        <v>2.4</v>
+      </c>
+      <c r="AP261">
+        <v>3.1</v>
+      </c>
+      <c r="AQ261">
+        <v>3.1</v>
+      </c>
+      <c r="AR261">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AS261">
+        <v>3.2</v>
+      </c>
+      <c r="AT261">
+        <v>3</v>
+      </c>
+      <c r="AU261">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AV261">
+        <v>3.4</v>
+      </c>
+      <c r="AW261">
+        <v>3.1</v>
+      </c>
+      <c r="AX261">
+        <v>2.38</v>
+      </c>
+      <c r="AY261">
+        <v>3.3</v>
+      </c>
+      <c r="AZ261">
+        <v>3</v>
+      </c>
+      <c r="BA261">
+        <v>38</v>
+      </c>
+      <c r="BB261">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="BC261">
+        <v>2.38</v>
+      </c>
+      <c r="BD261">
+        <v>3.42</v>
+      </c>
+      <c r="BE261">
+        <v>3.26</v>
+      </c>
+      <c r="BF261">
+        <v>3.2</v>
+      </c>
+      <c r="BG261">
+        <v>3.02</v>
+      </c>
+      <c r="BH261">
+        <v>36</v>
+      </c>
+      <c r="BI261">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BJ261">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="BK261">
+        <v>1.82</v>
+      </c>
+      <c r="BL261">
+        <v>1.74</v>
+      </c>
+      <c r="BM261">
+        <v>24</v>
+      </c>
+      <c r="BN261">
+        <v>-0.25</v>
+      </c>
+      <c r="BO261">
+        <v>2.1</v>
+      </c>
+      <c r="BP261">
+        <v>2.06</v>
+      </c>
+      <c r="BQ261">
+        <v>1.88</v>
+      </c>
+      <c r="BR261">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="262" spans="1:70">
+      <c r="A262" t="s">
+        <v>70</v>
+      </c>
+      <c r="B262" t="s">
+        <v>142</v>
+      </c>
+      <c r="C262" t="s">
+        <v>93</v>
+      </c>
+      <c r="D262" t="s">
+        <v>88</v>
+      </c>
+      <c r="E262">
+        <v>2</v>
+      </c>
+      <c r="F262">
+        <v>0</v>
+      </c>
+      <c r="G262" t="s">
+        <v>74</v>
+      </c>
+      <c r="H262">
+        <v>2</v>
+      </c>
+      <c r="I262">
+        <v>0</v>
+      </c>
+      <c r="J262" t="s">
+        <v>74</v>
+      </c>
+      <c r="K262">
+        <v>16</v>
+      </c>
+      <c r="L262">
+        <v>10</v>
+      </c>
+      <c r="M262">
+        <v>5</v>
+      </c>
+      <c r="N262">
+        <v>2</v>
+      </c>
+      <c r="O262">
+        <v>14</v>
+      </c>
+      <c r="P262">
+        <v>9</v>
+      </c>
+      <c r="Q262">
+        <v>4</v>
+      </c>
+      <c r="R262">
+        <v>3</v>
+      </c>
+      <c r="S262">
+        <v>0</v>
+      </c>
+      <c r="T262">
+        <v>0</v>
+      </c>
+      <c r="U262">
+        <v>0</v>
+      </c>
+      <c r="V262">
+        <v>0</v>
+      </c>
+      <c r="W262">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="X262">
+        <v>3.3</v>
+      </c>
+      <c r="Y262">
+        <v>3.3</v>
+      </c>
+      <c r="Z262">
+        <v>2.25</v>
+      </c>
+      <c r="AA262">
+        <v>3.25</v>
+      </c>
+      <c r="AB262">
+        <v>3.2</v>
+      </c>
+      <c r="AC262">
+        <v>2.25</v>
+      </c>
+      <c r="AD262">
+        <v>3.25</v>
+      </c>
+      <c r="AE262">
+        <v>3.2</v>
+      </c>
+      <c r="AF262">
+        <v>2.4</v>
+      </c>
+      <c r="AG262">
+        <v>3.3</v>
+      </c>
+      <c r="AH262">
+        <v>2.75</v>
+      </c>
+      <c r="AI262">
+        <v>2.25</v>
+      </c>
+      <c r="AJ262">
+        <v>3.25</v>
+      </c>
+      <c r="AK262">
+        <v>3.2</v>
+      </c>
+      <c r="AL262">
+        <v>2.31</v>
+      </c>
+      <c r="AM262">
+        <v>3.39</v>
+      </c>
+      <c r="AN262">
+        <v>3.42</v>
+      </c>
+      <c r="AO262">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AP262">
+        <v>3.2</v>
+      </c>
+      <c r="AQ262">
+        <v>3.2</v>
+      </c>
+      <c r="AR262">
+        <v>2.1</v>
+      </c>
+      <c r="AS262">
+        <v>3.25</v>
+      </c>
+      <c r="AT262">
+        <v>3.25</v>
+      </c>
+      <c r="AU262">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AV262">
+        <v>3.3</v>
+      </c>
+      <c r="AW262">
+        <v>3.4</v>
+      </c>
+      <c r="AX262">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AY262">
+        <v>3.3</v>
+      </c>
+      <c r="AZ262">
+        <v>3.3</v>
+      </c>
+      <c r="BA262">
+        <v>38</v>
+      </c>
+      <c r="BB262">
+        <v>2.4</v>
+      </c>
+      <c r="BC262">
+        <v>2.25</v>
+      </c>
+      <c r="BD262">
+        <v>3.4</v>
+      </c>
+      <c r="BE262">
+        <v>3.29</v>
+      </c>
+      <c r="BF262">
+        <v>3.5</v>
+      </c>
+      <c r="BG262">
+        <v>3.22</v>
+      </c>
+      <c r="BH262">
+        <v>35</v>
+      </c>
+      <c r="BI262">
+        <v>2.23</v>
+      </c>
+      <c r="BJ262">
+        <v>2.11</v>
+      </c>
+      <c r="BK262">
+        <v>1.78</v>
+      </c>
+      <c r="BL262">
+        <v>1.71</v>
+      </c>
+      <c r="BM262">
+        <v>24</v>
+      </c>
+      <c r="BN262">
+        <v>-0.25</v>
+      </c>
+      <c r="BO262">
+        <v>1.99</v>
+      </c>
+      <c r="BP262">
+        <v>1.94</v>
+      </c>
+      <c r="BQ262">
+        <v>1.97</v>
+      </c>
+      <c r="BR262">
+        <v>1.93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agrego la prediccion con los nombres. Se calculan las apuestas de todas las ligas juntas en el algoritmo genetico, se repite el algoritmo y luego se calcula el promedio de las apuestas de la jornada.
</commit_message>
<xml_diff>
--- a/DatosAle1/DP1213.xlsx
+++ b/DatosAle1/DP1213.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="19155" windowHeight="8505"/>
+    <workbookView xWindow="720" yWindow="885" windowWidth="18435" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="D1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1538" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="146">
   <si>
     <t>Div</t>
   </si>
@@ -443,6 +443,15 @@
   </si>
   <si>
     <t>14/04/13</t>
+  </si>
+  <si>
+    <t>19/04/13</t>
+  </si>
+  <si>
+    <t>20/04/13</t>
+  </si>
+  <si>
+    <t>21/04/13</t>
   </si>
 </sst>
 </file>
@@ -1265,10 +1274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BR262"/>
+  <dimension ref="A1:BR271"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C254" sqref="C254:C262"/>
+    <sheetView tabSelected="1" topLeftCell="A249" workbookViewId="0">
+      <selection activeCell="B269" sqref="B269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -56817,6 +56826,1914 @@
         <v>1.93</v>
       </c>
     </row>
+    <row r="263" spans="1:70">
+      <c r="A263" t="s">
+        <v>70</v>
+      </c>
+      <c r="B263" t="s">
+        <v>143</v>
+      </c>
+      <c r="C263" t="s">
+        <v>88</v>
+      </c>
+      <c r="D263" t="s">
+        <v>76</v>
+      </c>
+      <c r="E263">
+        <v>1</v>
+      </c>
+      <c r="F263">
+        <v>0</v>
+      </c>
+      <c r="G263" t="s">
+        <v>74</v>
+      </c>
+      <c r="H263">
+        <v>1</v>
+      </c>
+      <c r="I263">
+        <v>0</v>
+      </c>
+      <c r="J263" t="s">
+        <v>74</v>
+      </c>
+      <c r="K263">
+        <v>23</v>
+      </c>
+      <c r="L263">
+        <v>11</v>
+      </c>
+      <c r="M263">
+        <v>5</v>
+      </c>
+      <c r="N263">
+        <v>2</v>
+      </c>
+      <c r="O263">
+        <v>18</v>
+      </c>
+      <c r="P263">
+        <v>14</v>
+      </c>
+      <c r="Q263">
+        <v>6</v>
+      </c>
+      <c r="R263">
+        <v>5</v>
+      </c>
+      <c r="S263">
+        <v>4</v>
+      </c>
+      <c r="T263">
+        <v>1</v>
+      </c>
+      <c r="U263">
+        <v>0</v>
+      </c>
+      <c r="V263">
+        <v>1</v>
+      </c>
+      <c r="W263">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="X263">
+        <v>3.2</v>
+      </c>
+      <c r="Y263">
+        <v>3.1</v>
+      </c>
+      <c r="Z263">
+        <v>2.35</v>
+      </c>
+      <c r="AA263">
+        <v>3.25</v>
+      </c>
+      <c r="AB263">
+        <v>3</v>
+      </c>
+      <c r="AC263">
+        <v>2.35</v>
+      </c>
+      <c r="AD263">
+        <v>3.25</v>
+      </c>
+      <c r="AE263">
+        <v>3</v>
+      </c>
+      <c r="AF263">
+        <v>2.1</v>
+      </c>
+      <c r="AG263">
+        <v>3.3</v>
+      </c>
+      <c r="AH263">
+        <v>3.3</v>
+      </c>
+      <c r="AI263">
+        <v>2.25</v>
+      </c>
+      <c r="AJ263">
+        <v>3.3</v>
+      </c>
+      <c r="AK263">
+        <v>3.2</v>
+      </c>
+      <c r="AL263">
+        <v>2.39</v>
+      </c>
+      <c r="AM263">
+        <v>3.41</v>
+      </c>
+      <c r="AN263">
+        <v>3.24</v>
+      </c>
+      <c r="AO263">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AP263">
+        <v>3.3</v>
+      </c>
+      <c r="AQ263">
+        <v>3.1</v>
+      </c>
+      <c r="AR263">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AS263">
+        <v>3.2</v>
+      </c>
+      <c r="AT263">
+        <v>3</v>
+      </c>
+      <c r="AU263">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AV263">
+        <v>3.4</v>
+      </c>
+      <c r="AW263">
+        <v>3.12</v>
+      </c>
+      <c r="AX263">
+        <v>2.4</v>
+      </c>
+      <c r="AY263">
+        <v>3.3</v>
+      </c>
+      <c r="AZ263">
+        <v>2.9</v>
+      </c>
+      <c r="BA263">
+        <v>38</v>
+      </c>
+      <c r="BB263">
+        <v>2.41</v>
+      </c>
+      <c r="BC263">
+        <v>2.31</v>
+      </c>
+      <c r="BD263">
+        <v>3.41</v>
+      </c>
+      <c r="BE263">
+        <v>3.28</v>
+      </c>
+      <c r="BF263">
+        <v>3.35</v>
+      </c>
+      <c r="BG263">
+        <v>3.15</v>
+      </c>
+      <c r="BH263">
+        <v>35</v>
+      </c>
+      <c r="BI263">
+        <v>2.13</v>
+      </c>
+      <c r="BJ263">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="BK263">
+        <v>1.83</v>
+      </c>
+      <c r="BL263">
+        <v>1.76</v>
+      </c>
+      <c r="BM263">
+        <v>22</v>
+      </c>
+      <c r="BN263">
+        <v>0</v>
+      </c>
+      <c r="BO263">
+        <v>1.72</v>
+      </c>
+      <c r="BP263">
+        <v>1.67</v>
+      </c>
+      <c r="BQ263">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="BR263">
+        <v>2.2599999999999998</v>
+      </c>
+    </row>
+    <row r="264" spans="1:70">
+      <c r="A264" t="s">
+        <v>70</v>
+      </c>
+      <c r="B264" t="s">
+        <v>144</v>
+      </c>
+      <c r="C264" t="s">
+        <v>72</v>
+      </c>
+      <c r="D264" t="s">
+        <v>83</v>
+      </c>
+      <c r="E264">
+        <v>2</v>
+      </c>
+      <c r="F264">
+        <v>0</v>
+      </c>
+      <c r="G264" t="s">
+        <v>74</v>
+      </c>
+      <c r="H264">
+        <v>1</v>
+      </c>
+      <c r="I264">
+        <v>0</v>
+      </c>
+      <c r="J264" t="s">
+        <v>74</v>
+      </c>
+      <c r="K264">
+        <v>22</v>
+      </c>
+      <c r="L264">
+        <v>5</v>
+      </c>
+      <c r="M264">
+        <v>7</v>
+      </c>
+      <c r="N264">
+        <v>0</v>
+      </c>
+      <c r="O264">
+        <v>12</v>
+      </c>
+      <c r="P264">
+        <v>16</v>
+      </c>
+      <c r="Q264">
+        <v>8</v>
+      </c>
+      <c r="R264">
+        <v>4</v>
+      </c>
+      <c r="S264">
+        <v>3</v>
+      </c>
+      <c r="T264">
+        <v>3</v>
+      </c>
+      <c r="U264">
+        <v>0</v>
+      </c>
+      <c r="V264">
+        <v>0</v>
+      </c>
+      <c r="W264">
+        <v>1.44</v>
+      </c>
+      <c r="X264">
+        <v>4.5</v>
+      </c>
+      <c r="Y264">
+        <v>6.5</v>
+      </c>
+      <c r="Z264">
+        <v>1.45</v>
+      </c>
+      <c r="AA264">
+        <v>4.5</v>
+      </c>
+      <c r="AB264">
+        <v>6.5</v>
+      </c>
+      <c r="AC264">
+        <v>1.45</v>
+      </c>
+      <c r="AD264">
+        <v>4.5</v>
+      </c>
+      <c r="AE264">
+        <v>6.5</v>
+      </c>
+      <c r="AF264">
+        <v>1.5</v>
+      </c>
+      <c r="AG264">
+        <v>4</v>
+      </c>
+      <c r="AH264">
+        <v>6.1</v>
+      </c>
+      <c r="AI264">
+        <v>1.5</v>
+      </c>
+      <c r="AJ264">
+        <v>4.33</v>
+      </c>
+      <c r="AK264">
+        <v>6</v>
+      </c>
+      <c r="AL264">
+        <v>1.52</v>
+      </c>
+      <c r="AM264">
+        <v>4.68</v>
+      </c>
+      <c r="AN264">
+        <v>6.77</v>
+      </c>
+      <c r="AO264">
+        <v>1.53</v>
+      </c>
+      <c r="AP264">
+        <v>4</v>
+      </c>
+      <c r="AQ264">
+        <v>6</v>
+      </c>
+      <c r="AR264">
+        <v>1.44</v>
+      </c>
+      <c r="AS264">
+        <v>4.33</v>
+      </c>
+      <c r="AT264">
+        <v>6.25</v>
+      </c>
+      <c r="AU264">
+        <v>1.53</v>
+      </c>
+      <c r="AV264">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AW264">
+        <v>6.5</v>
+      </c>
+      <c r="AX264">
+        <v>1.44</v>
+      </c>
+      <c r="AY264">
+        <v>4.33</v>
+      </c>
+      <c r="AZ264">
+        <v>7</v>
+      </c>
+      <c r="BA264">
+        <v>38</v>
+      </c>
+      <c r="BB264">
+        <v>1.53</v>
+      </c>
+      <c r="BC264">
+        <v>1.48</v>
+      </c>
+      <c r="BD264">
+        <v>4.68</v>
+      </c>
+      <c r="BE264">
+        <v>4.3</v>
+      </c>
+      <c r="BF264">
+        <v>7.1</v>
+      </c>
+      <c r="BG264">
+        <v>6.45</v>
+      </c>
+      <c r="BH264">
+        <v>26</v>
+      </c>
+      <c r="BI264">
+        <v>1.65</v>
+      </c>
+      <c r="BJ264">
+        <v>1.57</v>
+      </c>
+      <c r="BK264">
+        <v>2.5</v>
+      </c>
+      <c r="BL264">
+        <v>2.31</v>
+      </c>
+      <c r="BM264">
+        <v>24</v>
+      </c>
+      <c r="BN264">
+        <v>-1</v>
+      </c>
+      <c r="BO264">
+        <v>1.85</v>
+      </c>
+      <c r="BP264">
+        <v>1.79</v>
+      </c>
+      <c r="BQ264">
+        <v>2.15</v>
+      </c>
+      <c r="BR264">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="265" spans="1:70">
+      <c r="A265" t="s">
+        <v>70</v>
+      </c>
+      <c r="B265" t="s">
+        <v>144</v>
+      </c>
+      <c r="C265" t="s">
+        <v>80</v>
+      </c>
+      <c r="D265" t="s">
+        <v>92</v>
+      </c>
+      <c r="E265">
+        <v>1</v>
+      </c>
+      <c r="F265">
+        <v>0</v>
+      </c>
+      <c r="G265" t="s">
+        <v>74</v>
+      </c>
+      <c r="H265">
+        <v>1</v>
+      </c>
+      <c r="I265">
+        <v>0</v>
+      </c>
+      <c r="J265" t="s">
+        <v>74</v>
+      </c>
+      <c r="K265">
+        <v>10</v>
+      </c>
+      <c r="L265">
+        <v>10</v>
+      </c>
+      <c r="M265">
+        <v>3</v>
+      </c>
+      <c r="N265">
+        <v>7</v>
+      </c>
+      <c r="O265">
+        <v>16</v>
+      </c>
+      <c r="P265">
+        <v>27</v>
+      </c>
+      <c r="Q265">
+        <v>0</v>
+      </c>
+      <c r="R265">
+        <v>4</v>
+      </c>
+      <c r="S265">
+        <v>3</v>
+      </c>
+      <c r="T265">
+        <v>3</v>
+      </c>
+      <c r="U265">
+        <v>0</v>
+      </c>
+      <c r="V265">
+        <v>0</v>
+      </c>
+      <c r="W265">
+        <v>3</v>
+      </c>
+      <c r="X265">
+        <v>3.4</v>
+      </c>
+      <c r="Y265">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Z265">
+        <v>2.95</v>
+      </c>
+      <c r="AA265">
+        <v>3.4</v>
+      </c>
+      <c r="AB265">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AC265">
+        <v>2.95</v>
+      </c>
+      <c r="AD265">
+        <v>3.4</v>
+      </c>
+      <c r="AE265">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AF265">
+        <v>2.9</v>
+      </c>
+      <c r="AG265">
+        <v>3.3</v>
+      </c>
+      <c r="AH265">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AI265">
+        <v>3</v>
+      </c>
+      <c r="AJ265">
+        <v>3.4</v>
+      </c>
+      <c r="AK265">
+        <v>2.29</v>
+      </c>
+      <c r="AL265">
+        <v>3.19</v>
+      </c>
+      <c r="AM265">
+        <v>3.55</v>
+      </c>
+      <c r="AN265">
+        <v>2.35</v>
+      </c>
+      <c r="AO265">
+        <v>3.1</v>
+      </c>
+      <c r="AP265">
+        <v>3.3</v>
+      </c>
+      <c r="AQ265">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AR265">
+        <v>3</v>
+      </c>
+      <c r="AS265">
+        <v>3.3</v>
+      </c>
+      <c r="AT265">
+        <v>2.25</v>
+      </c>
+      <c r="AU265">
+        <v>3</v>
+      </c>
+      <c r="AV265">
+        <v>3.5</v>
+      </c>
+      <c r="AW265">
+        <v>2.4</v>
+      </c>
+      <c r="AX265">
+        <v>3.1</v>
+      </c>
+      <c r="AY265">
+        <v>3.4</v>
+      </c>
+      <c r="AZ265">
+        <v>2.25</v>
+      </c>
+      <c r="BA265">
+        <v>38</v>
+      </c>
+      <c r="BB265">
+        <v>3.2</v>
+      </c>
+      <c r="BC265">
+        <v>3.01</v>
+      </c>
+      <c r="BD265">
+        <v>3.6</v>
+      </c>
+      <c r="BE265">
+        <v>3.4</v>
+      </c>
+      <c r="BF265">
+        <v>2.4</v>
+      </c>
+      <c r="BG265">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="BH265">
+        <v>35</v>
+      </c>
+      <c r="BI265">
+        <v>1.8</v>
+      </c>
+      <c r="BJ265">
+        <v>1.72</v>
+      </c>
+      <c r="BK265">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="BL265">
+        <v>2.09</v>
+      </c>
+      <c r="BM265">
+        <v>23</v>
+      </c>
+      <c r="BN265">
+        <v>0.25</v>
+      </c>
+      <c r="BO265">
+        <v>1.91</v>
+      </c>
+      <c r="BP265">
+        <v>1.88</v>
+      </c>
+      <c r="BQ265">
+        <v>2.04</v>
+      </c>
+      <c r="BR265">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="266" spans="1:70">
+      <c r="A266" t="s">
+        <v>70</v>
+      </c>
+      <c r="B266" t="s">
+        <v>144</v>
+      </c>
+      <c r="C266" t="s">
+        <v>86</v>
+      </c>
+      <c r="D266" t="s">
+        <v>77</v>
+      </c>
+      <c r="E266">
+        <v>2</v>
+      </c>
+      <c r="F266">
+        <v>1</v>
+      </c>
+      <c r="G266" t="s">
+        <v>74</v>
+      </c>
+      <c r="H266">
+        <v>2</v>
+      </c>
+      <c r="I266">
+        <v>1</v>
+      </c>
+      <c r="J266" t="s">
+        <v>74</v>
+      </c>
+      <c r="K266">
+        <v>17</v>
+      </c>
+      <c r="L266">
+        <v>12</v>
+      </c>
+      <c r="M266">
+        <v>4</v>
+      </c>
+      <c r="N266">
+        <v>5</v>
+      </c>
+      <c r="O266">
+        <v>21</v>
+      </c>
+      <c r="P266">
+        <v>19</v>
+      </c>
+      <c r="Q266">
+        <v>5</v>
+      </c>
+      <c r="R266">
+        <v>3</v>
+      </c>
+      <c r="S266">
+        <v>2</v>
+      </c>
+      <c r="T266">
+        <v>3</v>
+      </c>
+      <c r="U266">
+        <v>0</v>
+      </c>
+      <c r="V266">
+        <v>0</v>
+      </c>
+      <c r="W266">
+        <v>1.83</v>
+      </c>
+      <c r="X266">
+        <v>3.5</v>
+      </c>
+      <c r="Y266">
+        <v>4.33</v>
+      </c>
+      <c r="Z266">
+        <v>1.83</v>
+      </c>
+      <c r="AA266">
+        <v>3.6</v>
+      </c>
+      <c r="AB266">
+        <v>4.2</v>
+      </c>
+      <c r="AC266">
+        <v>1.83</v>
+      </c>
+      <c r="AD266">
+        <v>3.6</v>
+      </c>
+      <c r="AE266">
+        <v>4.2</v>
+      </c>
+      <c r="AF266">
+        <v>1.75</v>
+      </c>
+      <c r="AG266">
+        <v>3.7</v>
+      </c>
+      <c r="AH266">
+        <v>4.2</v>
+      </c>
+      <c r="AI266">
+        <v>1.83</v>
+      </c>
+      <c r="AJ266">
+        <v>3.5</v>
+      </c>
+      <c r="AK266">
+        <v>4.33</v>
+      </c>
+      <c r="AL266">
+        <v>1.83</v>
+      </c>
+      <c r="AM266">
+        <v>3.78</v>
+      </c>
+      <c r="AN266">
+        <v>4.79</v>
+      </c>
+      <c r="AO266">
+        <v>1.85</v>
+      </c>
+      <c r="AP266">
+        <v>3.3</v>
+      </c>
+      <c r="AQ266">
+        <v>4.5</v>
+      </c>
+      <c r="AR266">
+        <v>1.8</v>
+      </c>
+      <c r="AS266">
+        <v>3.4</v>
+      </c>
+      <c r="AT266">
+        <v>4.33</v>
+      </c>
+      <c r="AU266">
+        <v>1.85</v>
+      </c>
+      <c r="AV266">
+        <v>3.75</v>
+      </c>
+      <c r="AW266">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AX266">
+        <v>1.83</v>
+      </c>
+      <c r="AY266">
+        <v>3.5</v>
+      </c>
+      <c r="AZ266">
+        <v>4.33</v>
+      </c>
+      <c r="BA266">
+        <v>38</v>
+      </c>
+      <c r="BB266">
+        <v>1.9</v>
+      </c>
+      <c r="BC266">
+        <v>1.82</v>
+      </c>
+      <c r="BD266">
+        <v>3.76</v>
+      </c>
+      <c r="BE266">
+        <v>3.58</v>
+      </c>
+      <c r="BF266">
+        <v>5</v>
+      </c>
+      <c r="BG266">
+        <v>4.32</v>
+      </c>
+      <c r="BH266">
+        <v>35</v>
+      </c>
+      <c r="BI266">
+        <v>2.02</v>
+      </c>
+      <c r="BJ266">
+        <v>1.86</v>
+      </c>
+      <c r="BK266">
+        <v>2.09</v>
+      </c>
+      <c r="BL266">
+        <v>1.93</v>
+      </c>
+      <c r="BM266">
+        <v>23</v>
+      </c>
+      <c r="BN266">
+        <v>-0.75</v>
+      </c>
+      <c r="BO266">
+        <v>2.13</v>
+      </c>
+      <c r="BP266">
+        <v>2.09</v>
+      </c>
+      <c r="BQ266">
+        <v>1.86</v>
+      </c>
+      <c r="BR266">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="267" spans="1:70">
+      <c r="A267" t="s">
+        <v>70</v>
+      </c>
+      <c r="B267" t="s">
+        <v>144</v>
+      </c>
+      <c r="C267" t="s">
+        <v>91</v>
+      </c>
+      <c r="D267" t="s">
+        <v>85</v>
+      </c>
+      <c r="E267">
+        <v>1</v>
+      </c>
+      <c r="F267">
+        <v>6</v>
+      </c>
+      <c r="G267" t="s">
+        <v>78</v>
+      </c>
+      <c r="H267">
+        <v>0</v>
+      </c>
+      <c r="I267">
+        <v>3</v>
+      </c>
+      <c r="J267" t="s">
+        <v>78</v>
+      </c>
+      <c r="K267">
+        <v>7</v>
+      </c>
+      <c r="L267">
+        <v>14</v>
+      </c>
+      <c r="M267">
+        <v>4</v>
+      </c>
+      <c r="N267">
+        <v>5</v>
+      </c>
+      <c r="O267">
+        <v>7</v>
+      </c>
+      <c r="P267">
+        <v>9</v>
+      </c>
+      <c r="Q267">
+        <v>2</v>
+      </c>
+      <c r="R267">
+        <v>9</v>
+      </c>
+      <c r="S267">
+        <v>0</v>
+      </c>
+      <c r="T267">
+        <v>1</v>
+      </c>
+      <c r="U267">
+        <v>0</v>
+      </c>
+      <c r="V267">
+        <v>0</v>
+      </c>
+      <c r="W267">
+        <v>5.5</v>
+      </c>
+      <c r="X267">
+        <v>4</v>
+      </c>
+      <c r="Y267">
+        <v>1.57</v>
+      </c>
+      <c r="Z267">
+        <v>5.75</v>
+      </c>
+      <c r="AA267">
+        <v>3.9</v>
+      </c>
+      <c r="AB267">
+        <v>1.57</v>
+      </c>
+      <c r="AC267">
+        <v>5.75</v>
+      </c>
+      <c r="AD267">
+        <v>3.9</v>
+      </c>
+      <c r="AE267">
+        <v>1.57</v>
+      </c>
+      <c r="AF267">
+        <v>4.3</v>
+      </c>
+      <c r="AG267">
+        <v>3.9</v>
+      </c>
+      <c r="AH267">
+        <v>1.7</v>
+      </c>
+      <c r="AI267">
+        <v>5.5</v>
+      </c>
+      <c r="AJ267">
+        <v>4</v>
+      </c>
+      <c r="AK267">
+        <v>1.57</v>
+      </c>
+      <c r="AL267">
+        <v>6.37</v>
+      </c>
+      <c r="AM267">
+        <v>4.25</v>
+      </c>
+      <c r="AN267">
+        <v>1.59</v>
+      </c>
+      <c r="AO267">
+        <v>5.5</v>
+      </c>
+      <c r="AP267">
+        <v>3.75</v>
+      </c>
+      <c r="AQ267">
+        <v>1.62</v>
+      </c>
+      <c r="AR267">
+        <v>6</v>
+      </c>
+      <c r="AS267">
+        <v>3.75</v>
+      </c>
+      <c r="AT267">
+        <v>1.53</v>
+      </c>
+      <c r="AU267">
+        <v>5.75</v>
+      </c>
+      <c r="AV267">
+        <v>4.3</v>
+      </c>
+      <c r="AW267">
+        <v>1.62</v>
+      </c>
+      <c r="AX267">
+        <v>5.5</v>
+      </c>
+      <c r="AY267">
+        <v>3.8</v>
+      </c>
+      <c r="AZ267">
+        <v>1.62</v>
+      </c>
+      <c r="BA267">
+        <v>38</v>
+      </c>
+      <c r="BB267">
+        <v>6.4</v>
+      </c>
+      <c r="BC267">
+        <v>5.67</v>
+      </c>
+      <c r="BD267">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="BE267">
+        <v>3.93</v>
+      </c>
+      <c r="BF267">
+        <v>1.7</v>
+      </c>
+      <c r="BG267">
+        <v>1.59</v>
+      </c>
+      <c r="BH267">
+        <v>35</v>
+      </c>
+      <c r="BI267">
+        <v>1.77</v>
+      </c>
+      <c r="BJ267">
+        <v>1.7</v>
+      </c>
+      <c r="BK267">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="BL267">
+        <v>2.12</v>
+      </c>
+      <c r="BM267">
+        <v>24</v>
+      </c>
+      <c r="BN267">
+        <v>1</v>
+      </c>
+      <c r="BO267">
+        <v>1.95</v>
+      </c>
+      <c r="BP267">
+        <v>1.88</v>
+      </c>
+      <c r="BQ267">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="BR267">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="268" spans="1:70">
+      <c r="A268" t="s">
+        <v>70</v>
+      </c>
+      <c r="B268" t="s">
+        <v>144</v>
+      </c>
+      <c r="C268" t="s">
+        <v>81</v>
+      </c>
+      <c r="D268" t="s">
+        <v>89</v>
+      </c>
+      <c r="E268">
+        <v>5</v>
+      </c>
+      <c r="F268">
+        <v>0</v>
+      </c>
+      <c r="G268" t="s">
+        <v>74</v>
+      </c>
+      <c r="H268">
+        <v>2</v>
+      </c>
+      <c r="I268">
+        <v>0</v>
+      </c>
+      <c r="J268" t="s">
+        <v>74</v>
+      </c>
+      <c r="K268">
+        <v>22</v>
+      </c>
+      <c r="L268">
+        <v>5</v>
+      </c>
+      <c r="M268">
+        <v>9</v>
+      </c>
+      <c r="N268">
+        <v>2</v>
+      </c>
+      <c r="O268">
+        <v>11</v>
+      </c>
+      <c r="P268">
+        <v>9</v>
+      </c>
+      <c r="Q268">
+        <v>5</v>
+      </c>
+      <c r="R268">
+        <v>1</v>
+      </c>
+      <c r="S268">
+        <v>1</v>
+      </c>
+      <c r="T268">
+        <v>0</v>
+      </c>
+      <c r="U268">
+        <v>0</v>
+      </c>
+      <c r="V268">
+        <v>1</v>
+      </c>
+      <c r="W268">
+        <v>1.44</v>
+      </c>
+      <c r="X268">
+        <v>4.5</v>
+      </c>
+      <c r="Y268">
+        <v>6.5</v>
+      </c>
+      <c r="Z268">
+        <v>1.45</v>
+      </c>
+      <c r="AA268">
+        <v>4.75</v>
+      </c>
+      <c r="AB268">
+        <v>6</v>
+      </c>
+      <c r="AC268">
+        <v>1.45</v>
+      </c>
+      <c r="AD268">
+        <v>4.75</v>
+      </c>
+      <c r="AE268">
+        <v>6</v>
+      </c>
+      <c r="AF268">
+        <v>1.45</v>
+      </c>
+      <c r="AG268">
+        <v>4</v>
+      </c>
+      <c r="AH268">
+        <v>7</v>
+      </c>
+      <c r="AI268">
+        <v>1.44</v>
+      </c>
+      <c r="AJ268">
+        <v>4.5</v>
+      </c>
+      <c r="AK268">
+        <v>6.5</v>
+      </c>
+      <c r="AL268">
+        <v>1.49</v>
+      </c>
+      <c r="AM268">
+        <v>4.76</v>
+      </c>
+      <c r="AN268">
+        <v>7.31</v>
+      </c>
+      <c r="AO268">
+        <v>1.5</v>
+      </c>
+      <c r="AP268">
+        <v>4</v>
+      </c>
+      <c r="AQ268">
+        <v>7</v>
+      </c>
+      <c r="AR268">
+        <v>1.44</v>
+      </c>
+      <c r="AS268">
+        <v>4</v>
+      </c>
+      <c r="AT268">
+        <v>7</v>
+      </c>
+      <c r="AU268">
+        <v>1.5</v>
+      </c>
+      <c r="AV268">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AW268">
+        <v>7</v>
+      </c>
+      <c r="AX268">
+        <v>1.44</v>
+      </c>
+      <c r="AY268">
+        <v>4.33</v>
+      </c>
+      <c r="AZ268">
+        <v>7</v>
+      </c>
+      <c r="BA268">
+        <v>38</v>
+      </c>
+      <c r="BB268">
+        <v>1.5</v>
+      </c>
+      <c r="BC268">
+        <v>1.47</v>
+      </c>
+      <c r="BD268">
+        <v>4.8</v>
+      </c>
+      <c r="BE268">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="BF268">
+        <v>7.6</v>
+      </c>
+      <c r="BG268">
+        <v>6.86</v>
+      </c>
+      <c r="BH268">
+        <v>26</v>
+      </c>
+      <c r="BI268">
+        <v>1.68</v>
+      </c>
+      <c r="BJ268">
+        <v>1.62</v>
+      </c>
+      <c r="BK268">
+        <v>2.38</v>
+      </c>
+      <c r="BL268">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="BM268">
+        <v>24</v>
+      </c>
+      <c r="BN268">
+        <v>-1</v>
+      </c>
+      <c r="BO268">
+        <v>1.8</v>
+      </c>
+      <c r="BP268">
+        <v>1.76</v>
+      </c>
+      <c r="BQ268">
+        <v>2.16</v>
+      </c>
+      <c r="BR268">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="269" spans="1:70">
+      <c r="A269" t="s">
+        <v>70</v>
+      </c>
+      <c r="B269" t="s">
+        <v>144</v>
+      </c>
+      <c r="C269" t="s">
+        <v>73</v>
+      </c>
+      <c r="D269" t="s">
+        <v>94</v>
+      </c>
+      <c r="E269">
+        <v>0</v>
+      </c>
+      <c r="F269">
+        <v>3</v>
+      </c>
+      <c r="G269" t="s">
+        <v>78</v>
+      </c>
+      <c r="H269">
+        <v>0</v>
+      </c>
+      <c r="I269">
+        <v>2</v>
+      </c>
+      <c r="J269" t="s">
+        <v>78</v>
+      </c>
+      <c r="K269">
+        <v>8</v>
+      </c>
+      <c r="L269">
+        <v>8</v>
+      </c>
+      <c r="M269">
+        <v>3</v>
+      </c>
+      <c r="N269">
+        <v>5</v>
+      </c>
+      <c r="O269">
+        <v>18</v>
+      </c>
+      <c r="P269">
+        <v>16</v>
+      </c>
+      <c r="Q269">
+        <v>6</v>
+      </c>
+      <c r="R269">
+        <v>3</v>
+      </c>
+      <c r="S269">
+        <v>3</v>
+      </c>
+      <c r="T269">
+        <v>1</v>
+      </c>
+      <c r="U269">
+        <v>0</v>
+      </c>
+      <c r="V269">
+        <v>0</v>
+      </c>
+      <c r="W269">
+        <v>2</v>
+      </c>
+      <c r="X269">
+        <v>3.6</v>
+      </c>
+      <c r="Y269">
+        <v>3.5</v>
+      </c>
+      <c r="Z269">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AA269">
+        <v>3.4</v>
+      </c>
+      <c r="AB269">
+        <v>3.5</v>
+      </c>
+      <c r="AC269">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AD269">
+        <v>3.4</v>
+      </c>
+      <c r="AE269">
+        <v>3.5</v>
+      </c>
+      <c r="AF269">
+        <v>2.1</v>
+      </c>
+      <c r="AG269">
+        <v>3.3</v>
+      </c>
+      <c r="AH269">
+        <v>3.3</v>
+      </c>
+      <c r="AI269">
+        <v>2.1</v>
+      </c>
+      <c r="AJ269">
+        <v>3.4</v>
+      </c>
+      <c r="AK269">
+        <v>3.4</v>
+      </c>
+      <c r="AL269">
+        <v>2.1</v>
+      </c>
+      <c r="AM269">
+        <v>3.69</v>
+      </c>
+      <c r="AN269">
+        <v>3.66</v>
+      </c>
+      <c r="AO269">
+        <v>2.15</v>
+      </c>
+      <c r="AP269">
+        <v>3.5</v>
+      </c>
+      <c r="AQ269">
+        <v>3.2</v>
+      </c>
+      <c r="AR269">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AS269">
+        <v>3.4</v>
+      </c>
+      <c r="AT269">
+        <v>3.3</v>
+      </c>
+      <c r="AU269">
+        <v>2.15</v>
+      </c>
+      <c r="AV269">
+        <v>3.5</v>
+      </c>
+      <c r="AW269">
+        <v>3.6</v>
+      </c>
+      <c r="AX269">
+        <v>2.15</v>
+      </c>
+      <c r="AY269">
+        <v>3.4</v>
+      </c>
+      <c r="AZ269">
+        <v>3.3</v>
+      </c>
+      <c r="BA269">
+        <v>38</v>
+      </c>
+      <c r="BB269">
+        <v>2.15</v>
+      </c>
+      <c r="BC269">
+        <v>2.09</v>
+      </c>
+      <c r="BD269">
+        <v>3.75</v>
+      </c>
+      <c r="BE269">
+        <v>3.48</v>
+      </c>
+      <c r="BF269">
+        <v>3.59</v>
+      </c>
+      <c r="BG269">
+        <v>3.38</v>
+      </c>
+      <c r="BH269">
+        <v>27</v>
+      </c>
+      <c r="BI269">
+        <v>1.68</v>
+      </c>
+      <c r="BJ269">
+        <v>1.59</v>
+      </c>
+      <c r="BK269">
+        <v>2.48</v>
+      </c>
+      <c r="BL269">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="BM269">
+        <v>21</v>
+      </c>
+      <c r="BN269">
+        <v>-0.25</v>
+      </c>
+      <c r="BO269">
+        <v>1.85</v>
+      </c>
+      <c r="BP269">
+        <v>1.8</v>
+      </c>
+      <c r="BQ269">
+        <v>2.14</v>
+      </c>
+      <c r="BR269">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="270" spans="1:70">
+      <c r="A270" t="s">
+        <v>70</v>
+      </c>
+      <c r="B270" t="s">
+        <v>145</v>
+      </c>
+      <c r="C270" t="s">
+        <v>87</v>
+      </c>
+      <c r="D270" t="s">
+        <v>84</v>
+      </c>
+      <c r="E270">
+        <v>0</v>
+      </c>
+      <c r="F270">
+        <v>1</v>
+      </c>
+      <c r="G270" t="s">
+        <v>78</v>
+      </c>
+      <c r="H270">
+        <v>0</v>
+      </c>
+      <c r="I270">
+        <v>1</v>
+      </c>
+      <c r="J270" t="s">
+        <v>78</v>
+      </c>
+      <c r="K270">
+        <v>23</v>
+      </c>
+      <c r="L270">
+        <v>15</v>
+      </c>
+      <c r="M270">
+        <v>8</v>
+      </c>
+      <c r="N270">
+        <v>3</v>
+      </c>
+      <c r="O270">
+        <v>12</v>
+      </c>
+      <c r="P270">
+        <v>25</v>
+      </c>
+      <c r="Q270">
+        <v>14</v>
+      </c>
+      <c r="R270">
+        <v>4</v>
+      </c>
+      <c r="S270">
+        <v>4</v>
+      </c>
+      <c r="T270">
+        <v>5</v>
+      </c>
+      <c r="U270">
+        <v>0</v>
+      </c>
+      <c r="V270">
+        <v>0</v>
+      </c>
+      <c r="W270">
+        <v>1.75</v>
+      </c>
+      <c r="X270">
+        <v>3.5</v>
+      </c>
+      <c r="Y270">
+        <v>4.75</v>
+      </c>
+      <c r="Z270">
+        <v>1.7</v>
+      </c>
+      <c r="AA270">
+        <v>3.6</v>
+      </c>
+      <c r="AB270">
+        <v>5</v>
+      </c>
+      <c r="AC270">
+        <v>1.7</v>
+      </c>
+      <c r="AD270">
+        <v>3.6</v>
+      </c>
+      <c r="AE270">
+        <v>5</v>
+      </c>
+      <c r="AF270">
+        <v>1.7</v>
+      </c>
+      <c r="AG270">
+        <v>3.7</v>
+      </c>
+      <c r="AH270">
+        <v>4.5</v>
+      </c>
+      <c r="AI270">
+        <v>1.72</v>
+      </c>
+      <c r="AJ270">
+        <v>3.5</v>
+      </c>
+      <c r="AK270">
+        <v>5</v>
+      </c>
+      <c r="AL270">
+        <v>1.77</v>
+      </c>
+      <c r="AM270">
+        <v>3.73</v>
+      </c>
+      <c r="AN270">
+        <v>5.37</v>
+      </c>
+      <c r="AO270">
+        <v>1.75</v>
+      </c>
+      <c r="AP270">
+        <v>3.4</v>
+      </c>
+      <c r="AQ270">
+        <v>5</v>
+      </c>
+      <c r="AR270">
+        <v>1.67</v>
+      </c>
+      <c r="AS270">
+        <v>3.6</v>
+      </c>
+      <c r="AT270">
+        <v>4.8</v>
+      </c>
+      <c r="AU270">
+        <v>1.75</v>
+      </c>
+      <c r="AV270">
+        <v>3.7</v>
+      </c>
+      <c r="AW270">
+        <v>5.4</v>
+      </c>
+      <c r="AX270">
+        <v>1.67</v>
+      </c>
+      <c r="AY270">
+        <v>3.75</v>
+      </c>
+      <c r="AZ270">
+        <v>5</v>
+      </c>
+      <c r="BA270">
+        <v>38</v>
+      </c>
+      <c r="BB270">
+        <v>1.8</v>
+      </c>
+      <c r="BC270">
+        <v>1.72</v>
+      </c>
+      <c r="BD270">
+        <v>3.85</v>
+      </c>
+      <c r="BE270">
+        <v>3.59</v>
+      </c>
+      <c r="BF270">
+        <v>5.5</v>
+      </c>
+      <c r="BG270">
+        <v>4.95</v>
+      </c>
+      <c r="BH270">
+        <v>36</v>
+      </c>
+      <c r="BI270">
+        <v>2.14</v>
+      </c>
+      <c r="BJ270">
+        <v>2.04</v>
+      </c>
+      <c r="BK270">
+        <v>1.83</v>
+      </c>
+      <c r="BL270">
+        <v>1.76</v>
+      </c>
+      <c r="BM270">
+        <v>23</v>
+      </c>
+      <c r="BN270">
+        <v>-1</v>
+      </c>
+      <c r="BO270">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="BP270">
+        <v>2.34</v>
+      </c>
+      <c r="BQ270">
+        <v>1.68</v>
+      </c>
+      <c r="BR270">
+        <v>1.63</v>
+      </c>
+    </row>
+    <row r="271" spans="1:70">
+      <c r="A271" t="s">
+        <v>70</v>
+      </c>
+      <c r="B271" t="s">
+        <v>145</v>
+      </c>
+      <c r="C271" t="s">
+        <v>93</v>
+      </c>
+      <c r="D271" t="s">
+        <v>82</v>
+      </c>
+      <c r="E271">
+        <v>2</v>
+      </c>
+      <c r="F271">
+        <v>1</v>
+      </c>
+      <c r="G271" t="s">
+        <v>74</v>
+      </c>
+      <c r="H271">
+        <v>2</v>
+      </c>
+      <c r="I271">
+        <v>0</v>
+      </c>
+      <c r="J271" t="s">
+        <v>74</v>
+      </c>
+      <c r="K271">
+        <v>15</v>
+      </c>
+      <c r="L271">
+        <v>11</v>
+      </c>
+      <c r="M271">
+        <v>7</v>
+      </c>
+      <c r="N271">
+        <v>3</v>
+      </c>
+      <c r="O271">
+        <v>14</v>
+      </c>
+      <c r="P271">
+        <v>15</v>
+      </c>
+      <c r="Q271">
+        <v>3</v>
+      </c>
+      <c r="R271">
+        <v>6</v>
+      </c>
+      <c r="S271">
+        <v>0</v>
+      </c>
+      <c r="T271">
+        <v>3</v>
+      </c>
+      <c r="U271">
+        <v>0</v>
+      </c>
+      <c r="V271">
+        <v>0</v>
+      </c>
+      <c r="W271">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="X271">
+        <v>3.4</v>
+      </c>
+      <c r="Y271">
+        <v>3</v>
+      </c>
+      <c r="Z271">
+        <v>2.4</v>
+      </c>
+      <c r="AA271">
+        <v>3.4</v>
+      </c>
+      <c r="AB271">
+        <v>2.85</v>
+      </c>
+      <c r="AC271">
+        <v>2.4</v>
+      </c>
+      <c r="AD271">
+        <v>3.4</v>
+      </c>
+      <c r="AE271">
+        <v>2.85</v>
+      </c>
+      <c r="AF271">
+        <v>2.4</v>
+      </c>
+      <c r="AG271">
+        <v>3.3</v>
+      </c>
+      <c r="AH271">
+        <v>2.75</v>
+      </c>
+      <c r="AI271">
+        <v>2.37</v>
+      </c>
+      <c r="AJ271">
+        <v>3.4</v>
+      </c>
+      <c r="AK271">
+        <v>2.87</v>
+      </c>
+      <c r="AL271">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AM271">
+        <v>3.51</v>
+      </c>
+      <c r="AN271">
+        <v>3.06</v>
+      </c>
+      <c r="AO271">
+        <v>2.5</v>
+      </c>
+      <c r="AP271">
+        <v>3.2</v>
+      </c>
+      <c r="AQ271">
+        <v>2.8</v>
+      </c>
+      <c r="AR271">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AS271">
+        <v>3.3</v>
+      </c>
+      <c r="AT271">
+        <v>2.88</v>
+      </c>
+      <c r="AU271">
+        <v>2.5</v>
+      </c>
+      <c r="AV271">
+        <v>3.5</v>
+      </c>
+      <c r="AW271">
+        <v>3</v>
+      </c>
+      <c r="AX271">
+        <v>2.38</v>
+      </c>
+      <c r="AY271">
+        <v>3.4</v>
+      </c>
+      <c r="AZ271">
+        <v>2.88</v>
+      </c>
+      <c r="BA271">
+        <v>38</v>
+      </c>
+      <c r="BB271">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="BC271">
+        <v>2.4</v>
+      </c>
+      <c r="BD271">
+        <v>3.51</v>
+      </c>
+      <c r="BE271">
+        <v>3.33</v>
+      </c>
+      <c r="BF271">
+        <v>3.13</v>
+      </c>
+      <c r="BG271">
+        <v>2.92</v>
+      </c>
+      <c r="BH271">
+        <v>34</v>
+      </c>
+      <c r="BI271">
+        <v>1.94</v>
+      </c>
+      <c r="BJ271">
+        <v>1.87</v>
+      </c>
+      <c r="BK271">
+        <v>2.02</v>
+      </c>
+      <c r="BL271">
+        <v>1.92</v>
+      </c>
+      <c r="BM271">
+        <v>21</v>
+      </c>
+      <c r="BN271">
+        <v>0</v>
+      </c>
+      <c r="BO271">
+        <v>1.76</v>
+      </c>
+      <c r="BP271">
+        <v>1.72</v>
+      </c>
+      <c r="BQ271">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="BR271">
+        <v>2.17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizado jornada 26-29 abril 2013. Creado archivo de fixtures para lo que queda de temporada
</commit_message>
<xml_diff>
--- a/DatosAle1/DP1213.xlsx
+++ b/DatosAle1/DP1213.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="885" windowWidth="18435" windowHeight="7650"/>
+    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="8220"/>
   </bookViews>
   <sheets>
     <sheet name="D1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="149">
   <si>
     <t>Div</t>
   </si>
@@ -452,6 +452,15 @@
   </si>
   <si>
     <t>21/04/13</t>
+  </si>
+  <si>
+    <t>26/04/13</t>
+  </si>
+  <si>
+    <t>27/04/13</t>
+  </si>
+  <si>
+    <t>28/04/13</t>
   </si>
 </sst>
 </file>
@@ -1274,10 +1283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BR271"/>
+  <dimension ref="A1:BR280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A249" workbookViewId="0">
-      <selection activeCell="B269" sqref="B269"/>
+    <sheetView tabSelected="1" topLeftCell="A255" workbookViewId="0">
+      <selection activeCell="B272" sqref="B272:B280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -58734,6 +58743,1914 @@
         <v>2.17</v>
       </c>
     </row>
+    <row r="272" spans="1:70">
+      <c r="A272" t="s">
+        <v>70</v>
+      </c>
+      <c r="B272" t="s">
+        <v>146</v>
+      </c>
+      <c r="C272" t="s">
+        <v>84</v>
+      </c>
+      <c r="D272" t="s">
+        <v>91</v>
+      </c>
+      <c r="E272">
+        <v>2</v>
+      </c>
+      <c r="F272">
+        <v>3</v>
+      </c>
+      <c r="G272" t="s">
+        <v>78</v>
+      </c>
+      <c r="H272">
+        <v>1</v>
+      </c>
+      <c r="I272">
+        <v>1</v>
+      </c>
+      <c r="J272" t="s">
+        <v>79</v>
+      </c>
+      <c r="K272">
+        <v>20</v>
+      </c>
+      <c r="L272">
+        <v>8</v>
+      </c>
+      <c r="M272">
+        <v>8</v>
+      </c>
+      <c r="N272">
+        <v>4</v>
+      </c>
+      <c r="O272">
+        <v>13</v>
+      </c>
+      <c r="P272">
+        <v>13</v>
+      </c>
+      <c r="Q272">
+        <v>6</v>
+      </c>
+      <c r="R272">
+        <v>5</v>
+      </c>
+      <c r="S272">
+        <v>1</v>
+      </c>
+      <c r="T272">
+        <v>5</v>
+      </c>
+      <c r="U272">
+        <v>0</v>
+      </c>
+      <c r="V272">
+        <v>0</v>
+      </c>
+      <c r="W272">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="X272">
+        <v>3.4</v>
+      </c>
+      <c r="Y272">
+        <v>3</v>
+      </c>
+      <c r="Z272">
+        <v>2.4</v>
+      </c>
+      <c r="AA272">
+        <v>3.4</v>
+      </c>
+      <c r="AB272">
+        <v>2.85</v>
+      </c>
+      <c r="AC272">
+        <v>2.4</v>
+      </c>
+      <c r="AD272">
+        <v>3.4</v>
+      </c>
+      <c r="AE272">
+        <v>2.85</v>
+      </c>
+      <c r="AF272">
+        <v>2.4</v>
+      </c>
+      <c r="AG272">
+        <v>3.3</v>
+      </c>
+      <c r="AH272">
+        <v>2.75</v>
+      </c>
+      <c r="AI272">
+        <v>2.29</v>
+      </c>
+      <c r="AJ272">
+        <v>3.4</v>
+      </c>
+      <c r="AK272">
+        <v>3</v>
+      </c>
+      <c r="AL272">
+        <v>2.41</v>
+      </c>
+      <c r="AM272">
+        <v>3.42</v>
+      </c>
+      <c r="AN272">
+        <v>3.19</v>
+      </c>
+      <c r="AO272">
+        <v>2.4</v>
+      </c>
+      <c r="AP272">
+        <v>3.4</v>
+      </c>
+      <c r="AQ272">
+        <v>2.88</v>
+      </c>
+      <c r="AR272">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AS272">
+        <v>3.3</v>
+      </c>
+      <c r="AT272">
+        <v>3</v>
+      </c>
+      <c r="AU272">
+        <v>2.38</v>
+      </c>
+      <c r="AV272">
+        <v>3.4</v>
+      </c>
+      <c r="AW272">
+        <v>3.12</v>
+      </c>
+      <c r="AX272">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AY272">
+        <v>3.3</v>
+      </c>
+      <c r="AZ272">
+        <v>3</v>
+      </c>
+      <c r="BA272">
+        <v>40</v>
+      </c>
+      <c r="BB272">
+        <v>2.42</v>
+      </c>
+      <c r="BC272">
+        <v>2.36</v>
+      </c>
+      <c r="BD272">
+        <v>3.46</v>
+      </c>
+      <c r="BE272">
+        <v>3.35</v>
+      </c>
+      <c r="BF272">
+        <v>3.17</v>
+      </c>
+      <c r="BG272">
+        <v>3</v>
+      </c>
+      <c r="BH272">
+        <v>37</v>
+      </c>
+      <c r="BI272">
+        <v>1.85</v>
+      </c>
+      <c r="BJ272">
+        <v>1.79</v>
+      </c>
+      <c r="BK272">
+        <v>2.14</v>
+      </c>
+      <c r="BL272">
+        <v>2.02</v>
+      </c>
+      <c r="BM272">
+        <v>25</v>
+      </c>
+      <c r="BN272">
+        <v>-0.25</v>
+      </c>
+      <c r="BO272">
+        <v>2.09</v>
+      </c>
+      <c r="BP272">
+        <v>2.04</v>
+      </c>
+      <c r="BQ272">
+        <v>1.88</v>
+      </c>
+      <c r="BR272">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="273" spans="1:70">
+      <c r="A273" t="s">
+        <v>70</v>
+      </c>
+      <c r="B273" t="s">
+        <v>147</v>
+      </c>
+      <c r="C273" t="s">
+        <v>76</v>
+      </c>
+      <c r="D273" t="s">
+        <v>93</v>
+      </c>
+      <c r="E273">
+        <v>3</v>
+      </c>
+      <c r="F273">
+        <v>0</v>
+      </c>
+      <c r="G273" t="s">
+        <v>74</v>
+      </c>
+      <c r="H273">
+        <v>0</v>
+      </c>
+      <c r="I273">
+        <v>0</v>
+      </c>
+      <c r="J273" t="s">
+        <v>79</v>
+      </c>
+      <c r="K273">
+        <v>22</v>
+      </c>
+      <c r="L273">
+        <v>7</v>
+      </c>
+      <c r="M273">
+        <v>7</v>
+      </c>
+      <c r="N273">
+        <v>3</v>
+      </c>
+      <c r="O273">
+        <v>15</v>
+      </c>
+      <c r="P273">
+        <v>13</v>
+      </c>
+      <c r="Q273">
+        <v>9</v>
+      </c>
+      <c r="R273">
+        <v>4</v>
+      </c>
+      <c r="S273">
+        <v>4</v>
+      </c>
+      <c r="T273">
+        <v>4</v>
+      </c>
+      <c r="U273">
+        <v>0</v>
+      </c>
+      <c r="V273">
+        <v>0</v>
+      </c>
+      <c r="W273">
+        <v>2.25</v>
+      </c>
+      <c r="X273">
+        <v>3.25</v>
+      </c>
+      <c r="Y273">
+        <v>3.25</v>
+      </c>
+      <c r="Z273">
+        <v>2.25</v>
+      </c>
+      <c r="AA273">
+        <v>3.5</v>
+      </c>
+      <c r="AB273">
+        <v>3</v>
+      </c>
+      <c r="AC273">
+        <v>2.25</v>
+      </c>
+      <c r="AD273">
+        <v>3.5</v>
+      </c>
+      <c r="AE273">
+        <v>3</v>
+      </c>
+      <c r="AF273">
+        <v>2.1</v>
+      </c>
+      <c r="AG273">
+        <v>3.3</v>
+      </c>
+      <c r="AH273">
+        <v>3.3</v>
+      </c>
+      <c r="AI273">
+        <v>2.25</v>
+      </c>
+      <c r="AJ273">
+        <v>3.25</v>
+      </c>
+      <c r="AK273">
+        <v>3.2</v>
+      </c>
+      <c r="AL273">
+        <v>2.27</v>
+      </c>
+      <c r="AM273">
+        <v>3.5</v>
+      </c>
+      <c r="AN273">
+        <v>3.4</v>
+      </c>
+      <c r="AO273">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AP273">
+        <v>3.2</v>
+      </c>
+      <c r="AQ273">
+        <v>3.2</v>
+      </c>
+      <c r="AR273">
+        <v>2.1</v>
+      </c>
+      <c r="AS273">
+        <v>3.3</v>
+      </c>
+      <c r="AT273">
+        <v>3.2</v>
+      </c>
+      <c r="AU273">
+        <v>2.25</v>
+      </c>
+      <c r="AV273">
+        <v>3.5</v>
+      </c>
+      <c r="AW273">
+        <v>3.3</v>
+      </c>
+      <c r="AX273">
+        <v>2.25</v>
+      </c>
+      <c r="AY273">
+        <v>3.4</v>
+      </c>
+      <c r="AZ273">
+        <v>3.1</v>
+      </c>
+      <c r="BA273">
+        <v>40</v>
+      </c>
+      <c r="BB273">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="BC273">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="BD273">
+        <v>3.5</v>
+      </c>
+      <c r="BE273">
+        <v>3.35</v>
+      </c>
+      <c r="BF273">
+        <v>3.45</v>
+      </c>
+      <c r="BG273">
+        <v>3.2</v>
+      </c>
+      <c r="BH273">
+        <v>37</v>
+      </c>
+      <c r="BI273">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="BJ273">
+        <v>1.96</v>
+      </c>
+      <c r="BK273">
+        <v>1.95</v>
+      </c>
+      <c r="BL273">
+        <v>1.83</v>
+      </c>
+      <c r="BM273">
+        <v>25</v>
+      </c>
+      <c r="BN273">
+        <v>-0.25</v>
+      </c>
+      <c r="BO273">
+        <v>1.98</v>
+      </c>
+      <c r="BP273">
+        <v>1.94</v>
+      </c>
+      <c r="BQ273">
+        <v>2.02</v>
+      </c>
+      <c r="BR273">
+        <v>1.94</v>
+      </c>
+    </row>
+    <row r="274" spans="1:70">
+      <c r="A274" t="s">
+        <v>70</v>
+      </c>
+      <c r="B274" t="s">
+        <v>147</v>
+      </c>
+      <c r="C274" t="s">
+        <v>85</v>
+      </c>
+      <c r="D274" t="s">
+        <v>82</v>
+      </c>
+      <c r="E274">
+        <v>1</v>
+      </c>
+      <c r="F274">
+        <v>0</v>
+      </c>
+      <c r="G274" t="s">
+        <v>74</v>
+      </c>
+      <c r="H274">
+        <v>1</v>
+      </c>
+      <c r="I274">
+        <v>0</v>
+      </c>
+      <c r="J274" t="s">
+        <v>74</v>
+      </c>
+      <c r="K274">
+        <v>16</v>
+      </c>
+      <c r="L274">
+        <v>8</v>
+      </c>
+      <c r="M274">
+        <v>4</v>
+      </c>
+      <c r="N274">
+        <v>2</v>
+      </c>
+      <c r="O274">
+        <v>9</v>
+      </c>
+      <c r="P274">
+        <v>17</v>
+      </c>
+      <c r="Q274">
+        <v>5</v>
+      </c>
+      <c r="R274">
+        <v>3</v>
+      </c>
+      <c r="S274">
+        <v>1</v>
+      </c>
+      <c r="T274">
+        <v>1</v>
+      </c>
+      <c r="U274">
+        <v>0</v>
+      </c>
+      <c r="V274">
+        <v>0</v>
+      </c>
+      <c r="W274">
+        <v>1.22</v>
+      </c>
+      <c r="X274">
+        <v>6</v>
+      </c>
+      <c r="Y274">
+        <v>12</v>
+      </c>
+      <c r="Z274">
+        <v>1.2</v>
+      </c>
+      <c r="AA274">
+        <v>7</v>
+      </c>
+      <c r="AB274">
+        <v>11</v>
+      </c>
+      <c r="AC274">
+        <v>1.2</v>
+      </c>
+      <c r="AD274">
+        <v>7</v>
+      </c>
+      <c r="AE274">
+        <v>11</v>
+      </c>
+      <c r="AF274">
+        <v>1.25</v>
+      </c>
+      <c r="AG274">
+        <v>5.5</v>
+      </c>
+      <c r="AH274">
+        <v>10.3</v>
+      </c>
+      <c r="AI274">
+        <v>1.22</v>
+      </c>
+      <c r="AJ274">
+        <v>6</v>
+      </c>
+      <c r="AK274">
+        <v>12</v>
+      </c>
+      <c r="AL274">
+        <v>1.25</v>
+      </c>
+      <c r="AM274">
+        <v>6.8</v>
+      </c>
+      <c r="AN274">
+        <v>14.08</v>
+      </c>
+      <c r="AO274">
+        <v>1.25</v>
+      </c>
+      <c r="AP274">
+        <v>5.5</v>
+      </c>
+      <c r="AQ274">
+        <v>12</v>
+      </c>
+      <c r="AR274">
+        <v>1.22</v>
+      </c>
+      <c r="AS274">
+        <v>5.5</v>
+      </c>
+      <c r="AT274">
+        <v>12</v>
+      </c>
+      <c r="AU274">
+        <v>1.2</v>
+      </c>
+      <c r="AV274">
+        <v>6.5</v>
+      </c>
+      <c r="AW274">
+        <v>15</v>
+      </c>
+      <c r="AX274">
+        <v>1.22</v>
+      </c>
+      <c r="AY274">
+        <v>6</v>
+      </c>
+      <c r="AZ274">
+        <v>13</v>
+      </c>
+      <c r="BA274">
+        <v>40</v>
+      </c>
+      <c r="BB274">
+        <v>1.25</v>
+      </c>
+      <c r="BC274">
+        <v>1.22</v>
+      </c>
+      <c r="BD274">
+        <v>7.1</v>
+      </c>
+      <c r="BE274">
+        <v>5.99</v>
+      </c>
+      <c r="BF274">
+        <v>18</v>
+      </c>
+      <c r="BG274">
+        <v>12.75</v>
+      </c>
+      <c r="BH274">
+        <v>26</v>
+      </c>
+      <c r="BI274">
+        <v>1.5</v>
+      </c>
+      <c r="BJ274">
+        <v>1.44</v>
+      </c>
+      <c r="BK274">
+        <v>2.92</v>
+      </c>
+      <c r="BL274">
+        <v>2.63</v>
+      </c>
+      <c r="BM274">
+        <v>26</v>
+      </c>
+      <c r="BN274">
+        <v>-2</v>
+      </c>
+      <c r="BO274">
+        <v>2.17</v>
+      </c>
+      <c r="BP274">
+        <v>2.1</v>
+      </c>
+      <c r="BQ274">
+        <v>1.89</v>
+      </c>
+      <c r="BR274">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="275" spans="1:70">
+      <c r="A275" t="s">
+        <v>70</v>
+      </c>
+      <c r="B275" t="s">
+        <v>147</v>
+      </c>
+      <c r="C275" t="s">
+        <v>77</v>
+      </c>
+      <c r="D275" t="s">
+        <v>72</v>
+      </c>
+      <c r="E275">
+        <v>1</v>
+      </c>
+      <c r="F275">
+        <v>2</v>
+      </c>
+      <c r="G275" t="s">
+        <v>78</v>
+      </c>
+      <c r="H275">
+        <v>0</v>
+      </c>
+      <c r="I275">
+        <v>1</v>
+      </c>
+      <c r="J275" t="s">
+        <v>78</v>
+      </c>
+      <c r="K275">
+        <v>8</v>
+      </c>
+      <c r="L275">
+        <v>9</v>
+      </c>
+      <c r="M275">
+        <v>3</v>
+      </c>
+      <c r="N275">
+        <v>6</v>
+      </c>
+      <c r="O275">
+        <v>15</v>
+      </c>
+      <c r="P275">
+        <v>11</v>
+      </c>
+      <c r="Q275">
+        <v>6</v>
+      </c>
+      <c r="R275">
+        <v>3</v>
+      </c>
+      <c r="S275">
+        <v>5</v>
+      </c>
+      <c r="T275">
+        <v>2</v>
+      </c>
+      <c r="U275">
+        <v>0</v>
+      </c>
+      <c r="V275">
+        <v>0</v>
+      </c>
+      <c r="W275">
+        <v>4.75</v>
+      </c>
+      <c r="X275">
+        <v>4</v>
+      </c>
+      <c r="Y275">
+        <v>1.67</v>
+      </c>
+      <c r="Z275">
+        <v>5</v>
+      </c>
+      <c r="AA275">
+        <v>3.9</v>
+      </c>
+      <c r="AB275">
+        <v>1.65</v>
+      </c>
+      <c r="AC275">
+        <v>5</v>
+      </c>
+      <c r="AD275">
+        <v>3.9</v>
+      </c>
+      <c r="AE275">
+        <v>1.65</v>
+      </c>
+      <c r="AF275">
+        <v>3.8</v>
+      </c>
+      <c r="AG275">
+        <v>3.6</v>
+      </c>
+      <c r="AH275">
+        <v>1.85</v>
+      </c>
+      <c r="AI275">
+        <v>5</v>
+      </c>
+      <c r="AJ275">
+        <v>3.8</v>
+      </c>
+      <c r="AK275">
+        <v>1.66</v>
+      </c>
+      <c r="AL275">
+        <v>5.2</v>
+      </c>
+      <c r="AM275">
+        <v>4.08</v>
+      </c>
+      <c r="AN275">
+        <v>1.71</v>
+      </c>
+      <c r="AO275">
+        <v>5</v>
+      </c>
+      <c r="AP275">
+        <v>3.5</v>
+      </c>
+      <c r="AQ275">
+        <v>1.73</v>
+      </c>
+      <c r="AR275">
+        <v>4.8</v>
+      </c>
+      <c r="AS275">
+        <v>3.75</v>
+      </c>
+      <c r="AT275">
+        <v>1.67</v>
+      </c>
+      <c r="AU275">
+        <v>5</v>
+      </c>
+      <c r="AV275">
+        <v>4</v>
+      </c>
+      <c r="AW275">
+        <v>1.7</v>
+      </c>
+      <c r="AX275">
+        <v>4.5</v>
+      </c>
+      <c r="AY275">
+        <v>3.8</v>
+      </c>
+      <c r="AZ275">
+        <v>1.73</v>
+      </c>
+      <c r="BA275">
+        <v>40</v>
+      </c>
+      <c r="BB275">
+        <v>5.2</v>
+      </c>
+      <c r="BC275">
+        <v>4.76</v>
+      </c>
+      <c r="BD275">
+        <v>4.08</v>
+      </c>
+      <c r="BE275">
+        <v>3.8</v>
+      </c>
+      <c r="BF275">
+        <v>1.85</v>
+      </c>
+      <c r="BG275">
+        <v>1.7</v>
+      </c>
+      <c r="BH275">
+        <v>35</v>
+      </c>
+      <c r="BI275">
+        <v>1.72</v>
+      </c>
+      <c r="BJ275">
+        <v>1.66</v>
+      </c>
+      <c r="BK275">
+        <v>2.46</v>
+      </c>
+      <c r="BL275">
+        <v>2.19</v>
+      </c>
+      <c r="BM275">
+        <v>25</v>
+      </c>
+      <c r="BN275">
+        <v>0.75</v>
+      </c>
+      <c r="BO275">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="BP275">
+        <v>1.99</v>
+      </c>
+      <c r="BQ275">
+        <v>1.94</v>
+      </c>
+      <c r="BR275">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="276" spans="1:70">
+      <c r="A276" t="s">
+        <v>70</v>
+      </c>
+      <c r="B276" t="s">
+        <v>147</v>
+      </c>
+      <c r="C276" t="s">
+        <v>89</v>
+      </c>
+      <c r="D276" t="s">
+        <v>87</v>
+      </c>
+      <c r="E276">
+        <v>2</v>
+      </c>
+      <c r="F276">
+        <v>1</v>
+      </c>
+      <c r="G276" t="s">
+        <v>74</v>
+      </c>
+      <c r="H276">
+        <v>2</v>
+      </c>
+      <c r="I276">
+        <v>0</v>
+      </c>
+      <c r="J276" t="s">
+        <v>74</v>
+      </c>
+      <c r="K276">
+        <v>23</v>
+      </c>
+      <c r="L276">
+        <v>8</v>
+      </c>
+      <c r="M276">
+        <v>11</v>
+      </c>
+      <c r="N276">
+        <v>2</v>
+      </c>
+      <c r="O276">
+        <v>13</v>
+      </c>
+      <c r="P276">
+        <v>21</v>
+      </c>
+      <c r="Q276">
+        <v>4</v>
+      </c>
+      <c r="R276">
+        <v>3</v>
+      </c>
+      <c r="S276">
+        <v>2</v>
+      </c>
+      <c r="T276">
+        <v>2</v>
+      </c>
+      <c r="U276">
+        <v>0</v>
+      </c>
+      <c r="V276">
+        <v>0</v>
+      </c>
+      <c r="W276">
+        <v>2</v>
+      </c>
+      <c r="X276">
+        <v>3.4</v>
+      </c>
+      <c r="Y276">
+        <v>3.75</v>
+      </c>
+      <c r="Z276">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AA276">
+        <v>3.5</v>
+      </c>
+      <c r="AB276">
+        <v>3.4</v>
+      </c>
+      <c r="AC276">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AD276">
+        <v>3.5</v>
+      </c>
+      <c r="AE276">
+        <v>3.4</v>
+      </c>
+      <c r="AF276">
+        <v>1.85</v>
+      </c>
+      <c r="AG276">
+        <v>3.45</v>
+      </c>
+      <c r="AH276">
+        <v>4</v>
+      </c>
+      <c r="AI276">
+        <v>2</v>
+      </c>
+      <c r="AJ276">
+        <v>3.4</v>
+      </c>
+      <c r="AK276">
+        <v>3.75</v>
+      </c>
+      <c r="AL276">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="AM276">
+        <v>3.53</v>
+      </c>
+      <c r="AN276">
+        <v>3.94</v>
+      </c>
+      <c r="AO276">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AP276">
+        <v>3.2</v>
+      </c>
+      <c r="AQ276">
+        <v>3.8</v>
+      </c>
+      <c r="AR276">
+        <v>2</v>
+      </c>
+      <c r="AS276">
+        <v>3.4</v>
+      </c>
+      <c r="AT276">
+        <v>3.6</v>
+      </c>
+      <c r="AU276">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AV276">
+        <v>3.5</v>
+      </c>
+      <c r="AW276">
+        <v>3.9</v>
+      </c>
+      <c r="AX276">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AY276">
+        <v>3.5</v>
+      </c>
+      <c r="AZ276">
+        <v>3.5</v>
+      </c>
+      <c r="BA276">
+        <v>40</v>
+      </c>
+      <c r="BB276">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="BC276">
+        <v>2.02</v>
+      </c>
+      <c r="BD276">
+        <v>3.57</v>
+      </c>
+      <c r="BE276">
+        <v>3.4</v>
+      </c>
+      <c r="BF276">
+        <v>4</v>
+      </c>
+      <c r="BG276">
+        <v>3.68</v>
+      </c>
+      <c r="BH276">
+        <v>37</v>
+      </c>
+      <c r="BI276">
+        <v>2.19</v>
+      </c>
+      <c r="BJ276">
+        <v>2.06</v>
+      </c>
+      <c r="BK276">
+        <v>1.83</v>
+      </c>
+      <c r="BL276">
+        <v>1.75</v>
+      </c>
+      <c r="BM276">
+        <v>23</v>
+      </c>
+      <c r="BN276">
+        <v>-0.75</v>
+      </c>
+      <c r="BO276">
+        <v>2.42</v>
+      </c>
+      <c r="BP276">
+        <v>2.36</v>
+      </c>
+      <c r="BQ276">
+        <v>1.65</v>
+      </c>
+      <c r="BR276">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="277" spans="1:70">
+      <c r="A277" t="s">
+        <v>70</v>
+      </c>
+      <c r="B277" t="s">
+        <v>147</v>
+      </c>
+      <c r="C277" t="s">
+        <v>81</v>
+      </c>
+      <c r="D277" t="s">
+        <v>73</v>
+      </c>
+      <c r="E277">
+        <v>1</v>
+      </c>
+      <c r="F277">
+        <v>0</v>
+      </c>
+      <c r="G277" t="s">
+        <v>74</v>
+      </c>
+      <c r="H277">
+        <v>1</v>
+      </c>
+      <c r="I277">
+        <v>0</v>
+      </c>
+      <c r="J277" t="s">
+        <v>74</v>
+      </c>
+      <c r="K277">
+        <v>8</v>
+      </c>
+      <c r="L277">
+        <v>11</v>
+      </c>
+      <c r="M277">
+        <v>2</v>
+      </c>
+      <c r="N277">
+        <v>4</v>
+      </c>
+      <c r="O277">
+        <v>22</v>
+      </c>
+      <c r="P277">
+        <v>18</v>
+      </c>
+      <c r="Q277">
+        <v>7</v>
+      </c>
+      <c r="R277">
+        <v>6</v>
+      </c>
+      <c r="S277">
+        <v>1</v>
+      </c>
+      <c r="T277">
+        <v>2</v>
+      </c>
+      <c r="U277">
+        <v>0</v>
+      </c>
+      <c r="V277">
+        <v>0</v>
+      </c>
+      <c r="W277">
+        <v>1.4</v>
+      </c>
+      <c r="X277">
+        <v>4.75</v>
+      </c>
+      <c r="Y277">
+        <v>7</v>
+      </c>
+      <c r="Z277">
+        <v>1.44</v>
+      </c>
+      <c r="AA277">
+        <v>4.5</v>
+      </c>
+      <c r="AB277">
+        <v>6.75</v>
+      </c>
+      <c r="AC277">
+        <v>1.44</v>
+      </c>
+      <c r="AD277">
+        <v>4.5</v>
+      </c>
+      <c r="AE277">
+        <v>6.75</v>
+      </c>
+      <c r="AF277">
+        <v>1.5</v>
+      </c>
+      <c r="AG277">
+        <v>4</v>
+      </c>
+      <c r="AH277">
+        <v>6.1</v>
+      </c>
+      <c r="AI277">
+        <v>1.44</v>
+      </c>
+      <c r="AJ277">
+        <v>4.33</v>
+      </c>
+      <c r="AK277">
+        <v>7</v>
+      </c>
+      <c r="AL277">
+        <v>1.43</v>
+      </c>
+      <c r="AM277">
+        <v>5.2</v>
+      </c>
+      <c r="AN277">
+        <v>7.75</v>
+      </c>
+      <c r="AO277">
+        <v>1.44</v>
+      </c>
+      <c r="AP277">
+        <v>4.5</v>
+      </c>
+      <c r="AQ277">
+        <v>6.5</v>
+      </c>
+      <c r="AR277">
+        <v>1.4</v>
+      </c>
+      <c r="AS277">
+        <v>4.33</v>
+      </c>
+      <c r="AT277">
+        <v>7</v>
+      </c>
+      <c r="AU277">
+        <v>1.44</v>
+      </c>
+      <c r="AV277">
+        <v>5</v>
+      </c>
+      <c r="AW277">
+        <v>7</v>
+      </c>
+      <c r="AX277">
+        <v>1.44</v>
+      </c>
+      <c r="AY277">
+        <v>4.5</v>
+      </c>
+      <c r="AZ277">
+        <v>7</v>
+      </c>
+      <c r="BA277">
+        <v>40</v>
+      </c>
+      <c r="BB277">
+        <v>1.5</v>
+      </c>
+      <c r="BC277">
+        <v>1.43</v>
+      </c>
+      <c r="BD277">
+        <v>5.25</v>
+      </c>
+      <c r="BE277">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="BF277">
+        <v>7.7</v>
+      </c>
+      <c r="BG277">
+        <v>6.89</v>
+      </c>
+      <c r="BH277">
+        <v>26</v>
+      </c>
+      <c r="BI277">
+        <v>1.5</v>
+      </c>
+      <c r="BJ277">
+        <v>1.45</v>
+      </c>
+      <c r="BK277">
+        <v>2.88</v>
+      </c>
+      <c r="BL277">
+        <v>2.63</v>
+      </c>
+      <c r="BM277">
+        <v>26</v>
+      </c>
+      <c r="BN277">
+        <v>-1</v>
+      </c>
+      <c r="BO277">
+        <v>1.7</v>
+      </c>
+      <c r="BP277">
+        <v>1.66</v>
+      </c>
+      <c r="BQ277">
+        <v>2.46</v>
+      </c>
+      <c r="BR277">
+        <v>2.29</v>
+      </c>
+    </row>
+    <row r="278" spans="1:70">
+      <c r="A278" t="s">
+        <v>70</v>
+      </c>
+      <c r="B278" t="s">
+        <v>147</v>
+      </c>
+      <c r="C278" t="s">
+        <v>94</v>
+      </c>
+      <c r="D278" t="s">
+        <v>88</v>
+      </c>
+      <c r="E278">
+        <v>3</v>
+      </c>
+      <c r="F278">
+        <v>1</v>
+      </c>
+      <c r="G278" t="s">
+        <v>74</v>
+      </c>
+      <c r="H278">
+        <v>1</v>
+      </c>
+      <c r="I278">
+        <v>0</v>
+      </c>
+      <c r="J278" t="s">
+        <v>74</v>
+      </c>
+      <c r="K278">
+        <v>17</v>
+      </c>
+      <c r="L278">
+        <v>6</v>
+      </c>
+      <c r="M278">
+        <v>5</v>
+      </c>
+      <c r="N278">
+        <v>4</v>
+      </c>
+      <c r="O278">
+        <v>5</v>
+      </c>
+      <c r="P278">
+        <v>14</v>
+      </c>
+      <c r="Q278">
+        <v>5</v>
+      </c>
+      <c r="R278">
+        <v>3</v>
+      </c>
+      <c r="S278">
+        <v>0</v>
+      </c>
+      <c r="T278">
+        <v>1</v>
+      </c>
+      <c r="U278">
+        <v>0</v>
+      </c>
+      <c r="V278">
+        <v>0</v>
+      </c>
+      <c r="W278">
+        <v>2.1</v>
+      </c>
+      <c r="X278">
+        <v>3.4</v>
+      </c>
+      <c r="Y278">
+        <v>3.4</v>
+      </c>
+      <c r="Z278">
+        <v>2.1</v>
+      </c>
+      <c r="AA278">
+        <v>3.3</v>
+      </c>
+      <c r="AB278">
+        <v>3.5</v>
+      </c>
+      <c r="AC278">
+        <v>2.1</v>
+      </c>
+      <c r="AD278">
+        <v>3.3</v>
+      </c>
+      <c r="AE278">
+        <v>3.5</v>
+      </c>
+      <c r="AF278">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AG278">
+        <v>3.3</v>
+      </c>
+      <c r="AH278">
+        <v>3.1</v>
+      </c>
+      <c r="AI278">
+        <v>2.15</v>
+      </c>
+      <c r="AJ278">
+        <v>3.3</v>
+      </c>
+      <c r="AK278">
+        <v>3.4</v>
+      </c>
+      <c r="AL278">
+        <v>2.19</v>
+      </c>
+      <c r="AM278">
+        <v>3.46</v>
+      </c>
+      <c r="AN278">
+        <v>3.64</v>
+      </c>
+      <c r="AO278">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AP278">
+        <v>3.2</v>
+      </c>
+      <c r="AQ278">
+        <v>3.4</v>
+      </c>
+      <c r="AR278">
+        <v>2.1</v>
+      </c>
+      <c r="AS278">
+        <v>3.3</v>
+      </c>
+      <c r="AT278">
+        <v>3.4</v>
+      </c>
+      <c r="AU278">
+        <v>2.15</v>
+      </c>
+      <c r="AV278">
+        <v>3.4</v>
+      </c>
+      <c r="AW278">
+        <v>3.6</v>
+      </c>
+      <c r="AX278">
+        <v>2.15</v>
+      </c>
+      <c r="AY278">
+        <v>3.4</v>
+      </c>
+      <c r="AZ278">
+        <v>3.3</v>
+      </c>
+      <c r="BA278">
+        <v>40</v>
+      </c>
+      <c r="BB278">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BC278">
+        <v>2.15</v>
+      </c>
+      <c r="BD278">
+        <v>3.5</v>
+      </c>
+      <c r="BE278">
+        <v>3.34</v>
+      </c>
+      <c r="BF278">
+        <v>3.7</v>
+      </c>
+      <c r="BG278">
+        <v>3.38</v>
+      </c>
+      <c r="BH278">
+        <v>37</v>
+      </c>
+      <c r="BI278">
+        <v>2.11</v>
+      </c>
+      <c r="BJ278">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="BK278">
+        <v>1.86</v>
+      </c>
+      <c r="BL278">
+        <v>1.79</v>
+      </c>
+      <c r="BM278">
+        <v>25</v>
+      </c>
+      <c r="BN278">
+        <v>-0.25</v>
+      </c>
+      <c r="BO278">
+        <v>1.89</v>
+      </c>
+      <c r="BP278">
+        <v>1.86</v>
+      </c>
+      <c r="BQ278">
+        <v>2.06</v>
+      </c>
+      <c r="BR278">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="279" spans="1:70">
+      <c r="A279" t="s">
+        <v>70</v>
+      </c>
+      <c r="B279" t="s">
+        <v>148</v>
+      </c>
+      <c r="C279" t="s">
+        <v>83</v>
+      </c>
+      <c r="D279" t="s">
+        <v>80</v>
+      </c>
+      <c r="E279">
+        <v>0</v>
+      </c>
+      <c r="F279">
+        <v>0</v>
+      </c>
+      <c r="G279" t="s">
+        <v>79</v>
+      </c>
+      <c r="H279">
+        <v>0</v>
+      </c>
+      <c r="I279">
+        <v>0</v>
+      </c>
+      <c r="J279" t="s">
+        <v>79</v>
+      </c>
+      <c r="K279">
+        <v>14</v>
+      </c>
+      <c r="L279">
+        <v>8</v>
+      </c>
+      <c r="M279">
+        <v>2</v>
+      </c>
+      <c r="N279">
+        <v>3</v>
+      </c>
+      <c r="O279">
+        <v>14</v>
+      </c>
+      <c r="P279">
+        <v>15</v>
+      </c>
+      <c r="Q279">
+        <v>7</v>
+      </c>
+      <c r="R279">
+        <v>7</v>
+      </c>
+      <c r="S279">
+        <v>0</v>
+      </c>
+      <c r="T279">
+        <v>2</v>
+      </c>
+      <c r="U279">
+        <v>0</v>
+      </c>
+      <c r="V279">
+        <v>0</v>
+      </c>
+      <c r="W279">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="X279">
+        <v>3.4</v>
+      </c>
+      <c r="Y279">
+        <v>3.5</v>
+      </c>
+      <c r="Z279">
+        <v>2.1</v>
+      </c>
+      <c r="AA279">
+        <v>3.5</v>
+      </c>
+      <c r="AB279">
+        <v>3.3</v>
+      </c>
+      <c r="AC279">
+        <v>2.1</v>
+      </c>
+      <c r="AD279">
+        <v>3.5</v>
+      </c>
+      <c r="AE279">
+        <v>3.3</v>
+      </c>
+      <c r="AF279">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AG279">
+        <v>3.3</v>
+      </c>
+      <c r="AH279">
+        <v>2.9</v>
+      </c>
+      <c r="AI279">
+        <v>2</v>
+      </c>
+      <c r="AJ279">
+        <v>3.4</v>
+      </c>
+      <c r="AK279">
+        <v>3.75</v>
+      </c>
+      <c r="AL279">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="AM279">
+        <v>3.62</v>
+      </c>
+      <c r="AN279">
+        <v>3.83</v>
+      </c>
+      <c r="AO279">
+        <v>2.1</v>
+      </c>
+      <c r="AP279">
+        <v>3.25</v>
+      </c>
+      <c r="AQ279">
+        <v>3.5</v>
+      </c>
+      <c r="AR279">
+        <v>2</v>
+      </c>
+      <c r="AS279">
+        <v>3.4</v>
+      </c>
+      <c r="AT279">
+        <v>3.5</v>
+      </c>
+      <c r="AU279">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AV279">
+        <v>3.6</v>
+      </c>
+      <c r="AW279">
+        <v>3.8</v>
+      </c>
+      <c r="AX279">
+        <v>2.1</v>
+      </c>
+      <c r="AY279">
+        <v>3.4</v>
+      </c>
+      <c r="AZ279">
+        <v>3.4</v>
+      </c>
+      <c r="BA279">
+        <v>40</v>
+      </c>
+      <c r="BB279">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="BC279">
+        <v>2.06</v>
+      </c>
+      <c r="BD279">
+        <v>3.65</v>
+      </c>
+      <c r="BE279">
+        <v>3.42</v>
+      </c>
+      <c r="BF279">
+        <v>3.9</v>
+      </c>
+      <c r="BG279">
+        <v>3.54</v>
+      </c>
+      <c r="BH279">
+        <v>37</v>
+      </c>
+      <c r="BI279">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="BJ279">
+        <v>1.95</v>
+      </c>
+      <c r="BK279">
+        <v>1.94</v>
+      </c>
+      <c r="BL279">
+        <v>1.85</v>
+      </c>
+      <c r="BM279">
+        <v>23</v>
+      </c>
+      <c r="BN279">
+        <v>-0.25</v>
+      </c>
+      <c r="BO279">
+        <v>1.8</v>
+      </c>
+      <c r="BP279">
+        <v>1.76</v>
+      </c>
+      <c r="BQ279">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BR279">
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="280" spans="1:70">
+      <c r="A280" t="s">
+        <v>70</v>
+      </c>
+      <c r="B280" t="s">
+        <v>148</v>
+      </c>
+      <c r="C280" t="s">
+        <v>92</v>
+      </c>
+      <c r="D280" t="s">
+        <v>86</v>
+      </c>
+      <c r="E280">
+        <v>4</v>
+      </c>
+      <c r="F280">
+        <v>1</v>
+      </c>
+      <c r="G280" t="s">
+        <v>74</v>
+      </c>
+      <c r="H280">
+        <v>2</v>
+      </c>
+      <c r="I280">
+        <v>1</v>
+      </c>
+      <c r="J280" t="s">
+        <v>74</v>
+      </c>
+      <c r="K280">
+        <v>20</v>
+      </c>
+      <c r="L280">
+        <v>9</v>
+      </c>
+      <c r="M280">
+        <v>10</v>
+      </c>
+      <c r="N280">
+        <v>1</v>
+      </c>
+      <c r="O280">
+        <v>14</v>
+      </c>
+      <c r="P280">
+        <v>10</v>
+      </c>
+      <c r="Q280">
+        <v>6</v>
+      </c>
+      <c r="R280">
+        <v>3</v>
+      </c>
+      <c r="S280">
+        <v>1</v>
+      </c>
+      <c r="T280">
+        <v>3</v>
+      </c>
+      <c r="U280">
+        <v>0</v>
+      </c>
+      <c r="V280">
+        <v>0</v>
+      </c>
+      <c r="W280">
+        <v>1.57</v>
+      </c>
+      <c r="X280">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="Y280">
+        <v>5.5</v>
+      </c>
+      <c r="Z280">
+        <v>1.62</v>
+      </c>
+      <c r="AA280">
+        <v>4</v>
+      </c>
+      <c r="AB280">
+        <v>5</v>
+      </c>
+      <c r="AC280">
+        <v>1.62</v>
+      </c>
+      <c r="AD280">
+        <v>4</v>
+      </c>
+      <c r="AE280">
+        <v>5</v>
+      </c>
+      <c r="AF280">
+        <v>1.65</v>
+      </c>
+      <c r="AG280">
+        <v>3.7</v>
+      </c>
+      <c r="AH280">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="AI280">
+        <v>1.57</v>
+      </c>
+      <c r="AJ280">
+        <v>4</v>
+      </c>
+      <c r="AK280">
+        <v>5.5</v>
+      </c>
+      <c r="AL280">
+        <v>1.57</v>
+      </c>
+      <c r="AM280">
+        <v>4.54</v>
+      </c>
+      <c r="AN280">
+        <v>6.12</v>
+      </c>
+      <c r="AO280">
+        <v>1.57</v>
+      </c>
+      <c r="AP280">
+        <v>3.8</v>
+      </c>
+      <c r="AQ280">
+        <v>6</v>
+      </c>
+      <c r="AR280">
+        <v>1.53</v>
+      </c>
+      <c r="AS280">
+        <v>3.8</v>
+      </c>
+      <c r="AT280">
+        <v>6</v>
+      </c>
+      <c r="AU280">
+        <v>1.57</v>
+      </c>
+      <c r="AV280">
+        <v>4.5</v>
+      </c>
+      <c r="AW280">
+        <v>5.75</v>
+      </c>
+      <c r="AX280">
+        <v>1.62</v>
+      </c>
+      <c r="AY280">
+        <v>4</v>
+      </c>
+      <c r="AZ280">
+        <v>5.25</v>
+      </c>
+      <c r="BA280">
+        <v>40</v>
+      </c>
+      <c r="BB280">
+        <v>1.65</v>
+      </c>
+      <c r="BC280">
+        <v>1.57</v>
+      </c>
+      <c r="BD280">
+        <v>4.54</v>
+      </c>
+      <c r="BE280">
+        <v>4.07</v>
+      </c>
+      <c r="BF280">
+        <v>6.3</v>
+      </c>
+      <c r="BG280">
+        <v>5.59</v>
+      </c>
+      <c r="BH280">
+        <v>26</v>
+      </c>
+      <c r="BI280">
+        <v>1.58</v>
+      </c>
+      <c r="BJ280">
+        <v>1.52</v>
+      </c>
+      <c r="BK280">
+        <v>2.63</v>
+      </c>
+      <c r="BL280">
+        <v>2.42</v>
+      </c>
+      <c r="BM280">
+        <v>26</v>
+      </c>
+      <c r="BN280">
+        <v>-1</v>
+      </c>
+      <c r="BO280">
+        <v>2.02</v>
+      </c>
+      <c r="BP280">
+        <v>1.94</v>
+      </c>
+      <c r="BQ280">
+        <v>1.99</v>
+      </c>
+      <c r="BR280">
+        <v>1.93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Funciones para generar ejemplos con SQL. Prueba Fuzzy para predecir Resultados. Prueba diferentes configuraciones de redes neuronales para predecir resultados
</commit_message>
<xml_diff>
--- a/DatosAle1/DP1213.xlsx
+++ b/DatosAle1/DP1213.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="315" windowWidth="18915" windowHeight="8220"/>
+    <workbookView xWindow="840" yWindow="630" windowWidth="8115" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="D1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1646" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="149">
   <si>
     <t>Div</t>
   </si>
@@ -1283,11 +1283,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BR280"/>
+  <dimension ref="A1:BR298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A255" workbookViewId="0">
-      <selection activeCell="B272" sqref="B272:B280"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -60651,6 +60649,3822 @@
         <v>1.93</v>
       </c>
     </row>
+    <row r="281" spans="1:70">
+      <c r="A281" t="s">
+        <v>70</v>
+      </c>
+      <c r="B281" s="1">
+        <v>41338</v>
+      </c>
+      <c r="C281" t="s">
+        <v>88</v>
+      </c>
+      <c r="D281" t="s">
+        <v>92</v>
+      </c>
+      <c r="E281">
+        <v>0</v>
+      </c>
+      <c r="F281">
+        <v>1</v>
+      </c>
+      <c r="G281" t="s">
+        <v>78</v>
+      </c>
+      <c r="H281">
+        <v>0</v>
+      </c>
+      <c r="I281">
+        <v>0</v>
+      </c>
+      <c r="J281" t="s">
+        <v>79</v>
+      </c>
+      <c r="K281">
+        <v>12</v>
+      </c>
+      <c r="L281">
+        <v>15</v>
+      </c>
+      <c r="M281">
+        <v>0</v>
+      </c>
+      <c r="N281">
+        <v>5</v>
+      </c>
+      <c r="O281">
+        <v>14</v>
+      </c>
+      <c r="P281">
+        <v>22</v>
+      </c>
+      <c r="Q281">
+        <v>6</v>
+      </c>
+      <c r="R281">
+        <v>8</v>
+      </c>
+      <c r="S281">
+        <v>2</v>
+      </c>
+      <c r="T281">
+        <v>3</v>
+      </c>
+      <c r="U281">
+        <v>0</v>
+      </c>
+      <c r="V281">
+        <v>0</v>
+      </c>
+      <c r="W281">
+        <v>3.5</v>
+      </c>
+      <c r="X281">
+        <v>3.4</v>
+      </c>
+      <c r="Y281">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="Z281">
+        <v>3.3</v>
+      </c>
+      <c r="AA281">
+        <v>3.6</v>
+      </c>
+      <c r="AB281">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AC281">
+        <v>3.3</v>
+      </c>
+      <c r="AD281">
+        <v>3.6</v>
+      </c>
+      <c r="AE281">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AF281">
+        <v>3</v>
+      </c>
+      <c r="AG281">
+        <v>3.3</v>
+      </c>
+      <c r="AH281">
+        <v>2.25</v>
+      </c>
+      <c r="AI281">
+        <v>3.5</v>
+      </c>
+      <c r="AJ281">
+        <v>3.4</v>
+      </c>
+      <c r="AK281">
+        <v>2.04</v>
+      </c>
+      <c r="AL281">
+        <v>3.66</v>
+      </c>
+      <c r="AM281">
+        <v>3.66</v>
+      </c>
+      <c r="AN281">
+        <v>2.11</v>
+      </c>
+      <c r="AO281">
+        <v>3.4</v>
+      </c>
+      <c r="AP281">
+        <v>3.6</v>
+      </c>
+      <c r="AQ281">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AR281">
+        <v>3.5</v>
+      </c>
+      <c r="AS281">
+        <v>3.4</v>
+      </c>
+      <c r="AT281">
+        <v>2</v>
+      </c>
+      <c r="AU281">
+        <v>3.6</v>
+      </c>
+      <c r="AV281">
+        <v>3.6</v>
+      </c>
+      <c r="AW281">
+        <v>2.1</v>
+      </c>
+      <c r="AX281">
+        <v>3.4</v>
+      </c>
+      <c r="AY281">
+        <v>3.4</v>
+      </c>
+      <c r="AZ281">
+        <v>2.1</v>
+      </c>
+      <c r="BA281">
+        <v>40</v>
+      </c>
+      <c r="BB281">
+        <v>3.63</v>
+      </c>
+      <c r="BC281">
+        <v>3.47</v>
+      </c>
+      <c r="BD281">
+        <v>3.65</v>
+      </c>
+      <c r="BE281">
+        <v>3.46</v>
+      </c>
+      <c r="BF281">
+        <v>2.25</v>
+      </c>
+      <c r="BG281">
+        <v>2.1</v>
+      </c>
+      <c r="BH281">
+        <v>38</v>
+      </c>
+      <c r="BI281">
+        <v>1.85</v>
+      </c>
+      <c r="BJ281">
+        <v>1.78</v>
+      </c>
+      <c r="BK281">
+        <v>2.12</v>
+      </c>
+      <c r="BL281">
+        <v>2.02</v>
+      </c>
+      <c r="BM281">
+        <v>25</v>
+      </c>
+      <c r="BN281">
+        <v>0.25</v>
+      </c>
+      <c r="BO281">
+        <v>2.11</v>
+      </c>
+      <c r="BP281">
+        <v>2.06</v>
+      </c>
+      <c r="BQ281">
+        <v>1.87</v>
+      </c>
+      <c r="BR281">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="282" spans="1:70">
+      <c r="A282" t="s">
+        <v>70</v>
+      </c>
+      <c r="B282" s="1">
+        <v>41369</v>
+      </c>
+      <c r="C282" t="s">
+        <v>72</v>
+      </c>
+      <c r="D282" t="s">
+        <v>85</v>
+      </c>
+      <c r="E282">
+        <v>1</v>
+      </c>
+      <c r="F282">
+        <v>1</v>
+      </c>
+      <c r="G282" t="s">
+        <v>79</v>
+      </c>
+      <c r="H282">
+        <v>1</v>
+      </c>
+      <c r="I282">
+        <v>1</v>
+      </c>
+      <c r="J282" t="s">
+        <v>79</v>
+      </c>
+      <c r="K282">
+        <v>11</v>
+      </c>
+      <c r="L282">
+        <v>6</v>
+      </c>
+      <c r="M282">
+        <v>3</v>
+      </c>
+      <c r="N282">
+        <v>2</v>
+      </c>
+      <c r="O282">
+        <v>18</v>
+      </c>
+      <c r="P282">
+        <v>15</v>
+      </c>
+      <c r="Q282">
+        <v>6</v>
+      </c>
+      <c r="R282">
+        <v>1</v>
+      </c>
+      <c r="S282">
+        <v>1</v>
+      </c>
+      <c r="T282">
+        <v>4</v>
+      </c>
+      <c r="U282">
+        <v>0</v>
+      </c>
+      <c r="V282">
+        <v>1</v>
+      </c>
+      <c r="W282">
+        <v>3.1</v>
+      </c>
+      <c r="X282">
+        <v>3.4</v>
+      </c>
+      <c r="Y282">
+        <v>2.25</v>
+      </c>
+      <c r="Z282">
+        <v>3.2</v>
+      </c>
+      <c r="AA282">
+        <v>3.4</v>
+      </c>
+      <c r="AB282">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AC282">
+        <v>3.2</v>
+      </c>
+      <c r="AD282">
+        <v>3.4</v>
+      </c>
+      <c r="AE282">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AF282">
+        <v>2.75</v>
+      </c>
+      <c r="AG282">
+        <v>3.3</v>
+      </c>
+      <c r="AH282">
+        <v>2.4</v>
+      </c>
+      <c r="AI282">
+        <v>3.1</v>
+      </c>
+      <c r="AJ282">
+        <v>3.4</v>
+      </c>
+      <c r="AK282">
+        <v>2.25</v>
+      </c>
+      <c r="AL282">
+        <v>3.21</v>
+      </c>
+      <c r="AM282">
+        <v>3.53</v>
+      </c>
+      <c r="AN282">
+        <v>2.35</v>
+      </c>
+      <c r="AO282">
+        <v>3.1</v>
+      </c>
+      <c r="AP282">
+        <v>3.2</v>
+      </c>
+      <c r="AQ282">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AR282">
+        <v>3</v>
+      </c>
+      <c r="AS282">
+        <v>3.3</v>
+      </c>
+      <c r="AT282">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AU282">
+        <v>3.12</v>
+      </c>
+      <c r="AV282">
+        <v>3.5</v>
+      </c>
+      <c r="AW282">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AX282">
+        <v>3.1</v>
+      </c>
+      <c r="AY282">
+        <v>3.4</v>
+      </c>
+      <c r="AZ282">
+        <v>2.25</v>
+      </c>
+      <c r="BA282">
+        <v>40</v>
+      </c>
+      <c r="BB282">
+        <v>3.21</v>
+      </c>
+      <c r="BC282">
+        <v>3.03</v>
+      </c>
+      <c r="BD282">
+        <v>3.47</v>
+      </c>
+      <c r="BE282">
+        <v>3.33</v>
+      </c>
+      <c r="BF282">
+        <v>2.42</v>
+      </c>
+      <c r="BG282">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="BH282">
+        <v>33</v>
+      </c>
+      <c r="BI282">
+        <v>1.77</v>
+      </c>
+      <c r="BJ282">
+        <v>1.69</v>
+      </c>
+      <c r="BK282">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="BL282">
+        <v>2.14</v>
+      </c>
+      <c r="BM282">
+        <v>25</v>
+      </c>
+      <c r="BN282">
+        <v>0.25</v>
+      </c>
+      <c r="BO282">
+        <v>1.89</v>
+      </c>
+      <c r="BP282">
+        <v>1.84</v>
+      </c>
+      <c r="BQ282">
+        <v>2.09</v>
+      </c>
+      <c r="BR282">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="283" spans="1:70">
+      <c r="A283" t="s">
+        <v>70</v>
+      </c>
+      <c r="B283" s="1">
+        <v>41369</v>
+      </c>
+      <c r="C283" t="s">
+        <v>80</v>
+      </c>
+      <c r="D283" t="s">
+        <v>77</v>
+      </c>
+      <c r="E283">
+        <v>3</v>
+      </c>
+      <c r="F283">
+        <v>1</v>
+      </c>
+      <c r="G283" t="s">
+        <v>74</v>
+      </c>
+      <c r="H283">
+        <v>1</v>
+      </c>
+      <c r="I283">
+        <v>0</v>
+      </c>
+      <c r="J283" t="s">
+        <v>74</v>
+      </c>
+      <c r="K283">
+        <v>17</v>
+      </c>
+      <c r="L283">
+        <v>6</v>
+      </c>
+      <c r="M283">
+        <v>7</v>
+      </c>
+      <c r="N283">
+        <v>2</v>
+      </c>
+      <c r="O283">
+        <v>18</v>
+      </c>
+      <c r="P283">
+        <v>15</v>
+      </c>
+      <c r="Q283">
+        <v>5</v>
+      </c>
+      <c r="R283">
+        <v>7</v>
+      </c>
+      <c r="S283">
+        <v>1</v>
+      </c>
+      <c r="T283">
+        <v>2</v>
+      </c>
+      <c r="U283">
+        <v>0</v>
+      </c>
+      <c r="V283">
+        <v>0</v>
+      </c>
+      <c r="W283">
+        <v>1.8</v>
+      </c>
+      <c r="X283">
+        <v>3.5</v>
+      </c>
+      <c r="Y283">
+        <v>4.5</v>
+      </c>
+      <c r="Z283">
+        <v>1.8</v>
+      </c>
+      <c r="AA283">
+        <v>3.7</v>
+      </c>
+      <c r="AB283">
+        <v>4.2</v>
+      </c>
+      <c r="AC283">
+        <v>1.8</v>
+      </c>
+      <c r="AD283">
+        <v>3.7</v>
+      </c>
+      <c r="AE283">
+        <v>4.2</v>
+      </c>
+      <c r="AF283">
+        <v>1.8</v>
+      </c>
+      <c r="AG283">
+        <v>3.5</v>
+      </c>
+      <c r="AH283">
+        <v>4.2</v>
+      </c>
+      <c r="AI283">
+        <v>1.72</v>
+      </c>
+      <c r="AJ283">
+        <v>3.6</v>
+      </c>
+      <c r="AK283">
+        <v>4.5</v>
+      </c>
+      <c r="AL283">
+        <v>1.84</v>
+      </c>
+      <c r="AM283">
+        <v>3.79</v>
+      </c>
+      <c r="AN283">
+        <v>4.7</v>
+      </c>
+      <c r="AO283">
+        <v>1.83</v>
+      </c>
+      <c r="AP283">
+        <v>3.2</v>
+      </c>
+      <c r="AQ283">
+        <v>4.8</v>
+      </c>
+      <c r="AR283">
+        <v>1.8</v>
+      </c>
+      <c r="AS283">
+        <v>3.5</v>
+      </c>
+      <c r="AT283">
+        <v>4.33</v>
+      </c>
+      <c r="AU283">
+        <v>1.85</v>
+      </c>
+      <c r="AV283">
+        <v>3.8</v>
+      </c>
+      <c r="AW283">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AX283">
+        <v>1.83</v>
+      </c>
+      <c r="AY283">
+        <v>3.5</v>
+      </c>
+      <c r="AZ283">
+        <v>4.33</v>
+      </c>
+      <c r="BA283">
+        <v>40</v>
+      </c>
+      <c r="BB283">
+        <v>1.85</v>
+      </c>
+      <c r="BC283">
+        <v>1.82</v>
+      </c>
+      <c r="BD283">
+        <v>3.85</v>
+      </c>
+      <c r="BE283">
+        <v>3.55</v>
+      </c>
+      <c r="BF283">
+        <v>4.8</v>
+      </c>
+      <c r="BG283">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="BH283">
+        <v>37</v>
+      </c>
+      <c r="BI283">
+        <v>1.88</v>
+      </c>
+      <c r="BJ283">
+        <v>1.79</v>
+      </c>
+      <c r="BK283">
+        <v>2.1</v>
+      </c>
+      <c r="BL283">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="BM283">
+        <v>25</v>
+      </c>
+      <c r="BN283">
+        <v>-0.75</v>
+      </c>
+      <c r="BO283">
+        <v>2.1</v>
+      </c>
+      <c r="BP283">
+        <v>2.04</v>
+      </c>
+      <c r="BQ283">
+        <v>1.87</v>
+      </c>
+      <c r="BR283">
+        <v>1.83</v>
+      </c>
+    </row>
+    <row r="284" spans="1:70">
+      <c r="A284" t="s">
+        <v>70</v>
+      </c>
+      <c r="B284" s="1">
+        <v>41369</v>
+      </c>
+      <c r="C284" t="s">
+        <v>91</v>
+      </c>
+      <c r="D284" t="s">
+        <v>83</v>
+      </c>
+      <c r="E284">
+        <v>2</v>
+      </c>
+      <c r="F284">
+        <v>2</v>
+      </c>
+      <c r="G284" t="s">
+        <v>79</v>
+      </c>
+      <c r="H284">
+        <v>1</v>
+      </c>
+      <c r="I284">
+        <v>1</v>
+      </c>
+      <c r="J284" t="s">
+        <v>79</v>
+      </c>
+      <c r="K284">
+        <v>13</v>
+      </c>
+      <c r="L284">
+        <v>10</v>
+      </c>
+      <c r="M284">
+        <v>5</v>
+      </c>
+      <c r="N284">
+        <v>6</v>
+      </c>
+      <c r="O284">
+        <v>19</v>
+      </c>
+      <c r="P284">
+        <v>13</v>
+      </c>
+      <c r="Q284">
+        <v>2</v>
+      </c>
+      <c r="R284">
+        <v>2</v>
+      </c>
+      <c r="S284">
+        <v>1</v>
+      </c>
+      <c r="T284">
+        <v>2</v>
+      </c>
+      <c r="U284">
+        <v>1</v>
+      </c>
+      <c r="V284">
+        <v>0</v>
+      </c>
+      <c r="W284">
+        <v>2.38</v>
+      </c>
+      <c r="X284">
+        <v>3.4</v>
+      </c>
+      <c r="Y284">
+        <v>2.9</v>
+      </c>
+      <c r="Z284">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AA284">
+        <v>3.5</v>
+      </c>
+      <c r="AB284">
+        <v>2.7</v>
+      </c>
+      <c r="AC284">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AD284">
+        <v>3.5</v>
+      </c>
+      <c r="AE284">
+        <v>2.7</v>
+      </c>
+      <c r="AF284">
+        <v>2.1</v>
+      </c>
+      <c r="AG284">
+        <v>3.3</v>
+      </c>
+      <c r="AH284">
+        <v>3.3</v>
+      </c>
+      <c r="AI284">
+        <v>2.25</v>
+      </c>
+      <c r="AJ284">
+        <v>3.5</v>
+      </c>
+      <c r="AK284">
+        <v>3</v>
+      </c>
+      <c r="AL284">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="AM284">
+        <v>3.53</v>
+      </c>
+      <c r="AN284">
+        <v>2.98</v>
+      </c>
+      <c r="AO284">
+        <v>2.5</v>
+      </c>
+      <c r="AP284">
+        <v>3</v>
+      </c>
+      <c r="AQ284">
+        <v>3</v>
+      </c>
+      <c r="AR284">
+        <v>2.38</v>
+      </c>
+      <c r="AS284">
+        <v>3.3</v>
+      </c>
+      <c r="AT284">
+        <v>2.8</v>
+      </c>
+      <c r="AU284">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AV284">
+        <v>3.5</v>
+      </c>
+      <c r="AW284">
+        <v>2.9</v>
+      </c>
+      <c r="AX284">
+        <v>2.4</v>
+      </c>
+      <c r="AY284">
+        <v>3.3</v>
+      </c>
+      <c r="AZ284">
+        <v>2.88</v>
+      </c>
+      <c r="BA284">
+        <v>40</v>
+      </c>
+      <c r="BB284">
+        <v>2.5</v>
+      </c>
+      <c r="BC284">
+        <v>2.38</v>
+      </c>
+      <c r="BD284">
+        <v>3.51</v>
+      </c>
+      <c r="BE284">
+        <v>3.36</v>
+      </c>
+      <c r="BF284">
+        <v>3.3</v>
+      </c>
+      <c r="BG284">
+        <v>2.93</v>
+      </c>
+      <c r="BH284">
+        <v>37</v>
+      </c>
+      <c r="BI284">
+        <v>1.93</v>
+      </c>
+      <c r="BJ284">
+        <v>1.82</v>
+      </c>
+      <c r="BK284">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="BL284">
+        <v>1.97</v>
+      </c>
+      <c r="BM284">
+        <v>25</v>
+      </c>
+      <c r="BN284">
+        <v>-0.25</v>
+      </c>
+      <c r="BO284">
+        <v>2.16</v>
+      </c>
+      <c r="BP284">
+        <v>2.08</v>
+      </c>
+      <c r="BQ284">
+        <v>1.87</v>
+      </c>
+      <c r="BR284">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="285" spans="1:70">
+      <c r="A285" t="s">
+        <v>70</v>
+      </c>
+      <c r="B285" s="1">
+        <v>41369</v>
+      </c>
+      <c r="C285" t="s">
+        <v>87</v>
+      </c>
+      <c r="D285" t="s">
+        <v>81</v>
+      </c>
+      <c r="E285">
+        <v>0</v>
+      </c>
+      <c r="F285">
+        <v>2</v>
+      </c>
+      <c r="G285" t="s">
+        <v>78</v>
+      </c>
+      <c r="H285">
+        <v>0</v>
+      </c>
+      <c r="I285">
+        <v>1</v>
+      </c>
+      <c r="J285" t="s">
+        <v>78</v>
+      </c>
+      <c r="K285">
+        <v>16</v>
+      </c>
+      <c r="L285">
+        <v>20</v>
+      </c>
+      <c r="M285">
+        <v>3</v>
+      </c>
+      <c r="N285">
+        <v>2</v>
+      </c>
+      <c r="O285">
+        <v>12</v>
+      </c>
+      <c r="P285">
+        <v>16</v>
+      </c>
+      <c r="Q285">
+        <v>14</v>
+      </c>
+      <c r="R285">
+        <v>8</v>
+      </c>
+      <c r="S285">
+        <v>2</v>
+      </c>
+      <c r="T285">
+        <v>1</v>
+      </c>
+      <c r="U285">
+        <v>0</v>
+      </c>
+      <c r="V285">
+        <v>0</v>
+      </c>
+      <c r="W285">
+        <v>3.75</v>
+      </c>
+      <c r="X285">
+        <v>3.6</v>
+      </c>
+      <c r="Y285">
+        <v>1.91</v>
+      </c>
+      <c r="Z285">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AA285">
+        <v>3.6</v>
+      </c>
+      <c r="AB285">
+        <v>1.85</v>
+      </c>
+      <c r="AC285">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AD285">
+        <v>3.6</v>
+      </c>
+      <c r="AE285">
+        <v>1.85</v>
+      </c>
+      <c r="AF285">
+        <v>3.5</v>
+      </c>
+      <c r="AG285">
+        <v>3.4</v>
+      </c>
+      <c r="AH285">
+        <v>2</v>
+      </c>
+      <c r="AI285">
+        <v>3.8</v>
+      </c>
+      <c r="AJ285">
+        <v>3.6</v>
+      </c>
+      <c r="AK285">
+        <v>1.9</v>
+      </c>
+      <c r="AL285">
+        <v>4.25</v>
+      </c>
+      <c r="AM285">
+        <v>3.76</v>
+      </c>
+      <c r="AN285">
+        <v>1.93</v>
+      </c>
+      <c r="AO285">
+        <v>4</v>
+      </c>
+      <c r="AP285">
+        <v>3.3</v>
+      </c>
+      <c r="AQ285">
+        <v>1.95</v>
+      </c>
+      <c r="AR285">
+        <v>4</v>
+      </c>
+      <c r="AS285">
+        <v>3.5</v>
+      </c>
+      <c r="AT285">
+        <v>1.83</v>
+      </c>
+      <c r="AU285">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AV285">
+        <v>3.75</v>
+      </c>
+      <c r="AW285">
+        <v>1.92</v>
+      </c>
+      <c r="AX285">
+        <v>4.2</v>
+      </c>
+      <c r="AY285">
+        <v>3.6</v>
+      </c>
+      <c r="AZ285">
+        <v>1.85</v>
+      </c>
+      <c r="BA285">
+        <v>40</v>
+      </c>
+      <c r="BB285">
+        <v>4.33</v>
+      </c>
+      <c r="BC285">
+        <v>3.94</v>
+      </c>
+      <c r="BD285">
+        <v>3.8</v>
+      </c>
+      <c r="BE285">
+        <v>3.57</v>
+      </c>
+      <c r="BF285">
+        <v>2</v>
+      </c>
+      <c r="BG285">
+        <v>1.9</v>
+      </c>
+      <c r="BH285">
+        <v>33</v>
+      </c>
+      <c r="BI285">
+        <v>1.75</v>
+      </c>
+      <c r="BJ285">
+        <v>1.68</v>
+      </c>
+      <c r="BK285">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="BL285">
+        <v>2.15</v>
+      </c>
+      <c r="BM285">
+        <v>24</v>
+      </c>
+      <c r="BN285">
+        <v>0.25</v>
+      </c>
+      <c r="BO285">
+        <v>2.39</v>
+      </c>
+      <c r="BP285">
+        <v>2.33</v>
+      </c>
+      <c r="BQ285">
+        <v>1.67</v>
+      </c>
+      <c r="BR285">
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="286" spans="1:70">
+      <c r="A286" t="s">
+        <v>70</v>
+      </c>
+      <c r="B286" s="1">
+        <v>41369</v>
+      </c>
+      <c r="C286" t="s">
+        <v>93</v>
+      </c>
+      <c r="D286" t="s">
+        <v>84</v>
+      </c>
+      <c r="E286">
+        <v>0</v>
+      </c>
+      <c r="F286">
+        <v>2</v>
+      </c>
+      <c r="G286" t="s">
+        <v>78</v>
+      </c>
+      <c r="H286">
+        <v>0</v>
+      </c>
+      <c r="I286">
+        <v>0</v>
+      </c>
+      <c r="J286" t="s">
+        <v>79</v>
+      </c>
+      <c r="K286">
+        <v>14</v>
+      </c>
+      <c r="L286">
+        <v>10</v>
+      </c>
+      <c r="M286">
+        <v>4</v>
+      </c>
+      <c r="N286">
+        <v>4</v>
+      </c>
+      <c r="O286">
+        <v>17</v>
+      </c>
+      <c r="P286">
+        <v>23</v>
+      </c>
+      <c r="Q286">
+        <v>5</v>
+      </c>
+      <c r="R286">
+        <v>2</v>
+      </c>
+      <c r="S286">
+        <v>1</v>
+      </c>
+      <c r="T286">
+        <v>2</v>
+      </c>
+      <c r="U286">
+        <v>1</v>
+      </c>
+      <c r="V286">
+        <v>0</v>
+      </c>
+      <c r="W286">
+        <v>1.67</v>
+      </c>
+      <c r="X286">
+        <v>3.75</v>
+      </c>
+      <c r="Y286">
+        <v>5</v>
+      </c>
+      <c r="Z286">
+        <v>1.65</v>
+      </c>
+      <c r="AA286">
+        <v>3.9</v>
+      </c>
+      <c r="AB286">
+        <v>5</v>
+      </c>
+      <c r="AC286">
+        <v>1.65</v>
+      </c>
+      <c r="AD286">
+        <v>3.9</v>
+      </c>
+      <c r="AE286">
+        <v>5</v>
+      </c>
+      <c r="AF286">
+        <v>1.6</v>
+      </c>
+      <c r="AG286">
+        <v>3.9</v>
+      </c>
+      <c r="AH286">
+        <v>5</v>
+      </c>
+      <c r="AI286">
+        <v>1.66</v>
+      </c>
+      <c r="AJ286">
+        <v>3.75</v>
+      </c>
+      <c r="AK286">
+        <v>5</v>
+      </c>
+      <c r="AL286">
+        <v>1.7</v>
+      </c>
+      <c r="AM286">
+        <v>3.96</v>
+      </c>
+      <c r="AN286">
+        <v>5.52</v>
+      </c>
+      <c r="AO286">
+        <v>1.67</v>
+      </c>
+      <c r="AP286">
+        <v>3.5</v>
+      </c>
+      <c r="AQ286">
+        <v>5.5</v>
+      </c>
+      <c r="AR286">
+        <v>1.62</v>
+      </c>
+      <c r="AS286">
+        <v>3.6</v>
+      </c>
+      <c r="AT286">
+        <v>5</v>
+      </c>
+      <c r="AU286">
+        <v>1.7</v>
+      </c>
+      <c r="AV286">
+        <v>3.9</v>
+      </c>
+      <c r="AW286">
+        <v>5.4</v>
+      </c>
+      <c r="AX286">
+        <v>1.67</v>
+      </c>
+      <c r="AY286">
+        <v>3.75</v>
+      </c>
+      <c r="AZ286">
+        <v>5</v>
+      </c>
+      <c r="BA286">
+        <v>40</v>
+      </c>
+      <c r="BB286">
+        <v>1.71</v>
+      </c>
+      <c r="BC286">
+        <v>1.67</v>
+      </c>
+      <c r="BD286">
+        <v>4</v>
+      </c>
+      <c r="BE286">
+        <v>3.73</v>
+      </c>
+      <c r="BF286">
+        <v>5.61</v>
+      </c>
+      <c r="BG286">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="BH286">
+        <v>37</v>
+      </c>
+      <c r="BI286">
+        <v>1.83</v>
+      </c>
+      <c r="BJ286">
+        <v>1.77</v>
+      </c>
+      <c r="BK286">
+        <v>2.14</v>
+      </c>
+      <c r="BL286">
+        <v>2.04</v>
+      </c>
+      <c r="BM286">
+        <v>25</v>
+      </c>
+      <c r="BN286">
+        <v>-0.75</v>
+      </c>
+      <c r="BO286">
+        <v>1.93</v>
+      </c>
+      <c r="BP286">
+        <v>1.87</v>
+      </c>
+      <c r="BQ286">
+        <v>2.06</v>
+      </c>
+      <c r="BR286">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="287" spans="1:70">
+      <c r="A287" t="s">
+        <v>70</v>
+      </c>
+      <c r="B287" s="1">
+        <v>41369</v>
+      </c>
+      <c r="C287" t="s">
+        <v>73</v>
+      </c>
+      <c r="D287" t="s">
+        <v>89</v>
+      </c>
+      <c r="E287">
+        <v>2</v>
+      </c>
+      <c r="F287">
+        <v>2</v>
+      </c>
+      <c r="G287" t="s">
+        <v>79</v>
+      </c>
+      <c r="H287">
+        <v>2</v>
+      </c>
+      <c r="I287">
+        <v>0</v>
+      </c>
+      <c r="J287" t="s">
+        <v>74</v>
+      </c>
+      <c r="K287">
+        <v>18</v>
+      </c>
+      <c r="L287">
+        <v>13</v>
+      </c>
+      <c r="M287">
+        <v>3</v>
+      </c>
+      <c r="N287">
+        <v>5</v>
+      </c>
+      <c r="O287">
+        <v>23</v>
+      </c>
+      <c r="P287">
+        <v>15</v>
+      </c>
+      <c r="Q287">
+        <v>4</v>
+      </c>
+      <c r="R287">
+        <v>2</v>
+      </c>
+      <c r="S287">
+        <v>3</v>
+      </c>
+      <c r="T287">
+        <v>3</v>
+      </c>
+      <c r="U287">
+        <v>0</v>
+      </c>
+      <c r="V287">
+        <v>0</v>
+      </c>
+      <c r="W287">
+        <v>2.1</v>
+      </c>
+      <c r="X287">
+        <v>3.6</v>
+      </c>
+      <c r="Y287">
+        <v>3.2</v>
+      </c>
+      <c r="Z287">
+        <v>2</v>
+      </c>
+      <c r="AA287">
+        <v>3.9</v>
+      </c>
+      <c r="AB287">
+        <v>3.25</v>
+      </c>
+      <c r="AC287">
+        <v>2</v>
+      </c>
+      <c r="AD287">
+        <v>3.9</v>
+      </c>
+      <c r="AE287">
+        <v>3.25</v>
+      </c>
+      <c r="AF287">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AG287">
+        <v>3.4</v>
+      </c>
+      <c r="AH287">
+        <v>3.4</v>
+      </c>
+      <c r="AI287">
+        <v>2.04</v>
+      </c>
+      <c r="AJ287">
+        <v>3.5</v>
+      </c>
+      <c r="AK287">
+        <v>3.4</v>
+      </c>
+      <c r="AL287">
+        <v>2.09</v>
+      </c>
+      <c r="AM287">
+        <v>3.86</v>
+      </c>
+      <c r="AN287">
+        <v>3.51</v>
+      </c>
+      <c r="AO287">
+        <v>2.15</v>
+      </c>
+      <c r="AP287">
+        <v>3.2</v>
+      </c>
+      <c r="AQ287">
+        <v>3.5</v>
+      </c>
+      <c r="AR287">
+        <v>2</v>
+      </c>
+      <c r="AS287">
+        <v>3.4</v>
+      </c>
+      <c r="AT287">
+        <v>3.4</v>
+      </c>
+      <c r="AU287">
+        <v>2.1</v>
+      </c>
+      <c r="AV287">
+        <v>3.8</v>
+      </c>
+      <c r="AW287">
+        <v>3.4</v>
+      </c>
+      <c r="AX287">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AY287">
+        <v>3.5</v>
+      </c>
+      <c r="AZ287">
+        <v>3.5</v>
+      </c>
+      <c r="BA287">
+        <v>40</v>
+      </c>
+      <c r="BB287">
+        <v>2.15</v>
+      </c>
+      <c r="BC287">
+        <v>2.06</v>
+      </c>
+      <c r="BD287">
+        <v>3.8</v>
+      </c>
+      <c r="BE287">
+        <v>3.54</v>
+      </c>
+      <c r="BF287">
+        <v>3.6</v>
+      </c>
+      <c r="BG287">
+        <v>3.39</v>
+      </c>
+      <c r="BH287">
+        <v>27</v>
+      </c>
+      <c r="BI287">
+        <v>1.61</v>
+      </c>
+      <c r="BJ287">
+        <v>1.53</v>
+      </c>
+      <c r="BK287">
+        <v>2.62</v>
+      </c>
+      <c r="BL287">
+        <v>2.4</v>
+      </c>
+      <c r="BM287">
+        <v>23</v>
+      </c>
+      <c r="BN287">
+        <v>-0.5</v>
+      </c>
+      <c r="BO287">
+        <v>2.15</v>
+      </c>
+      <c r="BP287">
+        <v>2.09</v>
+      </c>
+      <c r="BQ287">
+        <v>1.85</v>
+      </c>
+      <c r="BR287">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="288" spans="1:70">
+      <c r="A288" t="s">
+        <v>70</v>
+      </c>
+      <c r="B288" s="1">
+        <v>41399</v>
+      </c>
+      <c r="C288" t="s">
+        <v>82</v>
+      </c>
+      <c r="D288" t="s">
+        <v>76</v>
+      </c>
+      <c r="E288">
+        <v>2</v>
+      </c>
+      <c r="F288">
+        <v>0</v>
+      </c>
+      <c r="G288" t="s">
+        <v>74</v>
+      </c>
+      <c r="H288">
+        <v>1</v>
+      </c>
+      <c r="I288">
+        <v>0</v>
+      </c>
+      <c r="J288" t="s">
+        <v>74</v>
+      </c>
+      <c r="K288">
+        <v>17</v>
+      </c>
+      <c r="L288">
+        <v>19</v>
+      </c>
+      <c r="M288">
+        <v>10</v>
+      </c>
+      <c r="N288">
+        <v>6</v>
+      </c>
+      <c r="O288">
+        <v>15</v>
+      </c>
+      <c r="P288">
+        <v>19</v>
+      </c>
+      <c r="Q288">
+        <v>5</v>
+      </c>
+      <c r="R288">
+        <v>8</v>
+      </c>
+      <c r="S288">
+        <v>3</v>
+      </c>
+      <c r="T288">
+        <v>2</v>
+      </c>
+      <c r="U288">
+        <v>0</v>
+      </c>
+      <c r="V288">
+        <v>0</v>
+      </c>
+      <c r="W288">
+        <v>1.91</v>
+      </c>
+      <c r="X288">
+        <v>3.4</v>
+      </c>
+      <c r="Y288">
+        <v>4</v>
+      </c>
+      <c r="Z288">
+        <v>1.95</v>
+      </c>
+      <c r="AA288">
+        <v>3.6</v>
+      </c>
+      <c r="AB288">
+        <v>3.6</v>
+      </c>
+      <c r="AC288">
+        <v>1.95</v>
+      </c>
+      <c r="AD288">
+        <v>3.6</v>
+      </c>
+      <c r="AE288">
+        <v>3.6</v>
+      </c>
+      <c r="AF288">
+        <v>2</v>
+      </c>
+      <c r="AG288">
+        <v>3.4</v>
+      </c>
+      <c r="AH288">
+        <v>3.5</v>
+      </c>
+      <c r="AI288">
+        <v>1.9</v>
+      </c>
+      <c r="AJ288">
+        <v>3.6</v>
+      </c>
+      <c r="AK288">
+        <v>3.75</v>
+      </c>
+      <c r="AL288">
+        <v>2.06</v>
+      </c>
+      <c r="AM288">
+        <v>3.56</v>
+      </c>
+      <c r="AN288">
+        <v>3.93</v>
+      </c>
+      <c r="AO288">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AP288">
+        <v>3.2</v>
+      </c>
+      <c r="AQ288">
+        <v>3.75</v>
+      </c>
+      <c r="AR288">
+        <v>1.95</v>
+      </c>
+      <c r="AS288">
+        <v>3.5</v>
+      </c>
+      <c r="AT288">
+        <v>3.6</v>
+      </c>
+      <c r="AU288">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AV288">
+        <v>3.5</v>
+      </c>
+      <c r="AW288">
+        <v>3.9</v>
+      </c>
+      <c r="AX288">
+        <v>2</v>
+      </c>
+      <c r="AY288">
+        <v>3.5</v>
+      </c>
+      <c r="AZ288">
+        <v>3.6</v>
+      </c>
+      <c r="BA288">
+        <v>40</v>
+      </c>
+      <c r="BB288">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="BC288">
+        <v>2</v>
+      </c>
+      <c r="BD288">
+        <v>3.6</v>
+      </c>
+      <c r="BE288">
+        <v>3.45</v>
+      </c>
+      <c r="BF288">
+        <v>4</v>
+      </c>
+      <c r="BG288">
+        <v>3.7</v>
+      </c>
+      <c r="BH288">
+        <v>37</v>
+      </c>
+      <c r="BI288">
+        <v>2.02</v>
+      </c>
+      <c r="BJ288">
+        <v>1.93</v>
+      </c>
+      <c r="BK288">
+        <v>1.96</v>
+      </c>
+      <c r="BL288">
+        <v>1.87</v>
+      </c>
+      <c r="BM288">
+        <v>23</v>
+      </c>
+      <c r="BN288">
+        <v>-0.5</v>
+      </c>
+      <c r="BO288">
+        <v>2.08</v>
+      </c>
+      <c r="BP288">
+        <v>2.02</v>
+      </c>
+      <c r="BQ288">
+        <v>1.9</v>
+      </c>
+      <c r="BR288">
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="289" spans="1:70">
+      <c r="A289" t="s">
+        <v>70</v>
+      </c>
+      <c r="B289" s="1">
+        <v>41399</v>
+      </c>
+      <c r="C289" t="s">
+        <v>86</v>
+      </c>
+      <c r="D289" t="s">
+        <v>94</v>
+      </c>
+      <c r="E289">
+        <v>1</v>
+      </c>
+      <c r="F289">
+        <v>1</v>
+      </c>
+      <c r="G289" t="s">
+        <v>79</v>
+      </c>
+      <c r="H289">
+        <v>1</v>
+      </c>
+      <c r="I289">
+        <v>0</v>
+      </c>
+      <c r="J289" t="s">
+        <v>74</v>
+      </c>
+      <c r="K289">
+        <v>15</v>
+      </c>
+      <c r="L289">
+        <v>19</v>
+      </c>
+      <c r="M289">
+        <v>8</v>
+      </c>
+      <c r="N289">
+        <v>8</v>
+      </c>
+      <c r="O289">
+        <v>16</v>
+      </c>
+      <c r="P289">
+        <v>19</v>
+      </c>
+      <c r="Q289">
+        <v>4</v>
+      </c>
+      <c r="R289">
+        <v>9</v>
+      </c>
+      <c r="S289">
+        <v>3</v>
+      </c>
+      <c r="T289">
+        <v>2</v>
+      </c>
+      <c r="U289">
+        <v>0</v>
+      </c>
+      <c r="V289">
+        <v>0</v>
+      </c>
+      <c r="W289">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="X289">
+        <v>3.4</v>
+      </c>
+      <c r="Y289">
+        <v>3.2</v>
+      </c>
+      <c r="Z289">
+        <v>2.25</v>
+      </c>
+      <c r="AA289">
+        <v>3.6</v>
+      </c>
+      <c r="AB289">
+        <v>2.9</v>
+      </c>
+      <c r="AC289">
+        <v>2.25</v>
+      </c>
+      <c r="AD289">
+        <v>3.6</v>
+      </c>
+      <c r="AE289">
+        <v>2.9</v>
+      </c>
+      <c r="AF289">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AG289">
+        <v>3.4</v>
+      </c>
+      <c r="AH289">
+        <v>2.8</v>
+      </c>
+      <c r="AI289">
+        <v>2.25</v>
+      </c>
+      <c r="AJ289">
+        <v>3.4</v>
+      </c>
+      <c r="AK289">
+        <v>3.1</v>
+      </c>
+      <c r="AL289">
+        <v>2.31</v>
+      </c>
+      <c r="AM289">
+        <v>3.69</v>
+      </c>
+      <c r="AN289">
+        <v>3.16</v>
+      </c>
+      <c r="AO289">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AP289">
+        <v>3.1</v>
+      </c>
+      <c r="AQ289">
+        <v>3.3</v>
+      </c>
+      <c r="AR289">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AS289">
+        <v>3.3</v>
+      </c>
+      <c r="AT289">
+        <v>3.13</v>
+      </c>
+      <c r="AU289">
+        <v>2.25</v>
+      </c>
+      <c r="AV289">
+        <v>3.6</v>
+      </c>
+      <c r="AW289">
+        <v>3.12</v>
+      </c>
+      <c r="AX289">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AY289">
+        <v>3.4</v>
+      </c>
+      <c r="AZ289">
+        <v>3.2</v>
+      </c>
+      <c r="BA289">
+        <v>40</v>
+      </c>
+      <c r="BB289">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="BC289">
+        <v>2.23</v>
+      </c>
+      <c r="BD289">
+        <v>3.75</v>
+      </c>
+      <c r="BE289">
+        <v>3.44</v>
+      </c>
+      <c r="BF289">
+        <v>3.3</v>
+      </c>
+      <c r="BG289">
+        <v>3.11</v>
+      </c>
+      <c r="BH289">
+        <v>31</v>
+      </c>
+      <c r="BI289">
+        <v>1.7</v>
+      </c>
+      <c r="BJ289">
+        <v>1.61</v>
+      </c>
+      <c r="BK289">
+        <v>2.39</v>
+      </c>
+      <c r="BL289">
+        <v>2.27</v>
+      </c>
+      <c r="BM289">
+        <v>25</v>
+      </c>
+      <c r="BN289">
+        <v>-0.25</v>
+      </c>
+      <c r="BO289">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="BP289">
+        <v>1.96</v>
+      </c>
+      <c r="BQ289">
+        <v>1.95</v>
+      </c>
+      <c r="BR289">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="290" spans="1:70">
+      <c r="A290" t="s">
+        <v>70</v>
+      </c>
+      <c r="B290" s="1">
+        <v>41583</v>
+      </c>
+      <c r="C290" t="s">
+        <v>85</v>
+      </c>
+      <c r="D290" t="s">
+        <v>76</v>
+      </c>
+      <c r="E290">
+        <v>3</v>
+      </c>
+      <c r="F290">
+        <v>0</v>
+      </c>
+      <c r="G290" t="s">
+        <v>74</v>
+      </c>
+      <c r="H290">
+        <v>0</v>
+      </c>
+      <c r="I290">
+        <v>0</v>
+      </c>
+      <c r="J290" t="s">
+        <v>79</v>
+      </c>
+      <c r="K290">
+        <v>15</v>
+      </c>
+      <c r="L290">
+        <v>6</v>
+      </c>
+      <c r="M290">
+        <v>7</v>
+      </c>
+      <c r="N290">
+        <v>3</v>
+      </c>
+      <c r="O290">
+        <v>10</v>
+      </c>
+      <c r="P290">
+        <v>13</v>
+      </c>
+      <c r="Q290">
+        <v>9</v>
+      </c>
+      <c r="R290">
+        <v>2</v>
+      </c>
+      <c r="S290">
+        <v>0</v>
+      </c>
+      <c r="T290">
+        <v>1</v>
+      </c>
+      <c r="U290">
+        <v>0</v>
+      </c>
+      <c r="V290">
+        <v>0</v>
+      </c>
+      <c r="W290">
+        <v>1.2</v>
+      </c>
+      <c r="X290">
+        <v>6.5</v>
+      </c>
+      <c r="Y290">
+        <v>13</v>
+      </c>
+      <c r="Z290">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="AA290">
+        <v>7</v>
+      </c>
+      <c r="AB290">
+        <v>15.5</v>
+      </c>
+      <c r="AC290">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="AD290">
+        <v>7</v>
+      </c>
+      <c r="AE290">
+        <v>15.5</v>
+      </c>
+      <c r="AF290">
+        <v>1.22</v>
+      </c>
+      <c r="AG290">
+        <v>6.2</v>
+      </c>
+      <c r="AH290">
+        <v>10</v>
+      </c>
+      <c r="AI290">
+        <v>1.2</v>
+      </c>
+      <c r="AJ290">
+        <v>6.5</v>
+      </c>
+      <c r="AK290">
+        <v>12</v>
+      </c>
+      <c r="AL290">
+        <v>1.22</v>
+      </c>
+      <c r="AM290">
+        <v>7.31</v>
+      </c>
+      <c r="AN290">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="AO290">
+        <v>1.22</v>
+      </c>
+      <c r="AP290">
+        <v>5.5</v>
+      </c>
+      <c r="AQ290">
+        <v>15</v>
+      </c>
+      <c r="AR290">
+        <v>1.2</v>
+      </c>
+      <c r="AS290">
+        <v>6.25</v>
+      </c>
+      <c r="AT290">
+        <v>12</v>
+      </c>
+      <c r="AU290">
+        <v>1.2</v>
+      </c>
+      <c r="AV290">
+        <v>7</v>
+      </c>
+      <c r="AW290">
+        <v>17</v>
+      </c>
+      <c r="AX290">
+        <v>1.2</v>
+      </c>
+      <c r="AY290">
+        <v>6.5</v>
+      </c>
+      <c r="AZ290">
+        <v>12</v>
+      </c>
+      <c r="BA290">
+        <v>37</v>
+      </c>
+      <c r="BB290">
+        <v>1.23</v>
+      </c>
+      <c r="BC290">
+        <v>1.2</v>
+      </c>
+      <c r="BD290">
+        <v>7.48</v>
+      </c>
+      <c r="BE290">
+        <v>6.6</v>
+      </c>
+      <c r="BF290">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="BG290">
+        <v>13.09</v>
+      </c>
+      <c r="BH290">
+        <v>24</v>
+      </c>
+      <c r="BI290">
+        <v>1.46</v>
+      </c>
+      <c r="BJ290">
+        <v>1.4</v>
+      </c>
+      <c r="BK290">
+        <v>3</v>
+      </c>
+      <c r="BL290">
+        <v>2.82</v>
+      </c>
+      <c r="BM290">
+        <v>24</v>
+      </c>
+      <c r="BN290">
+        <v>-1.75</v>
+      </c>
+      <c r="BO290">
+        <v>1.83</v>
+      </c>
+      <c r="BP290">
+        <v>1.76</v>
+      </c>
+      <c r="BQ290">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="BR290">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="291" spans="1:70">
+      <c r="A291" t="s">
+        <v>70</v>
+      </c>
+      <c r="B291" s="1">
+        <v>41583</v>
+      </c>
+      <c r="C291" t="s">
+        <v>77</v>
+      </c>
+      <c r="D291" t="s">
+        <v>87</v>
+      </c>
+      <c r="E291">
+        <v>1</v>
+      </c>
+      <c r="F291">
+        <v>2</v>
+      </c>
+      <c r="G291" t="s">
+        <v>78</v>
+      </c>
+      <c r="H291">
+        <v>1</v>
+      </c>
+      <c r="I291">
+        <v>0</v>
+      </c>
+      <c r="J291" t="s">
+        <v>74</v>
+      </c>
+      <c r="K291">
+        <v>6</v>
+      </c>
+      <c r="L291">
+        <v>13</v>
+      </c>
+      <c r="M291">
+        <v>2</v>
+      </c>
+      <c r="N291">
+        <v>4</v>
+      </c>
+      <c r="O291">
+        <v>19</v>
+      </c>
+      <c r="P291">
+        <v>19</v>
+      </c>
+      <c r="Q291">
+        <v>1</v>
+      </c>
+      <c r="R291">
+        <v>5</v>
+      </c>
+      <c r="S291">
+        <v>4</v>
+      </c>
+      <c r="T291">
+        <v>1</v>
+      </c>
+      <c r="U291">
+        <v>0</v>
+      </c>
+      <c r="V291">
+        <v>0</v>
+      </c>
+      <c r="W291">
+        <v>1.85</v>
+      </c>
+      <c r="X291">
+        <v>3.5</v>
+      </c>
+      <c r="Y291">
+        <v>4.2</v>
+      </c>
+      <c r="Z291">
+        <v>1.83</v>
+      </c>
+      <c r="AA291">
+        <v>3.7</v>
+      </c>
+      <c r="AB291">
+        <v>3.9</v>
+      </c>
+      <c r="AC291">
+        <v>1.83</v>
+      </c>
+      <c r="AD291">
+        <v>3.7</v>
+      </c>
+      <c r="AE291">
+        <v>3.9</v>
+      </c>
+      <c r="AF291">
+        <v>1.75</v>
+      </c>
+      <c r="AG291">
+        <v>3.8</v>
+      </c>
+      <c r="AH291">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AI291">
+        <v>1.83</v>
+      </c>
+      <c r="AJ291">
+        <v>3.5</v>
+      </c>
+      <c r="AK291">
+        <v>4.33</v>
+      </c>
+      <c r="AL291">
+        <v>1.88</v>
+      </c>
+      <c r="AM291">
+        <v>3.77</v>
+      </c>
+      <c r="AN291">
+        <v>4.46</v>
+      </c>
+      <c r="AO291">
+        <v>1.91</v>
+      </c>
+      <c r="AP291">
+        <v>3.5</v>
+      </c>
+      <c r="AQ291">
+        <v>4</v>
+      </c>
+      <c r="AR291">
+        <v>1.8</v>
+      </c>
+      <c r="AS291">
+        <v>3.6</v>
+      </c>
+      <c r="AT291">
+        <v>4</v>
+      </c>
+      <c r="AU291">
+        <v>1.87</v>
+      </c>
+      <c r="AV291">
+        <v>3.7</v>
+      </c>
+      <c r="AW291">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AX291">
+        <v>1.8</v>
+      </c>
+      <c r="AY291">
+        <v>3.6</v>
+      </c>
+      <c r="AZ291">
+        <v>4.2</v>
+      </c>
+      <c r="BA291">
+        <v>40</v>
+      </c>
+      <c r="BB291">
+        <v>1.91</v>
+      </c>
+      <c r="BC291">
+        <v>1.84</v>
+      </c>
+      <c r="BD291">
+        <v>3.8</v>
+      </c>
+      <c r="BE291">
+        <v>3.57</v>
+      </c>
+      <c r="BF291">
+        <v>4.55</v>
+      </c>
+      <c r="BG291">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="BH291">
+        <v>37</v>
+      </c>
+      <c r="BI291">
+        <v>2</v>
+      </c>
+      <c r="BJ291">
+        <v>1.91</v>
+      </c>
+      <c r="BK291">
+        <v>1.97</v>
+      </c>
+      <c r="BL291">
+        <v>1.89</v>
+      </c>
+      <c r="BM291">
+        <v>24</v>
+      </c>
+      <c r="BN291">
+        <v>-0.75</v>
+      </c>
+      <c r="BO291">
+        <v>2.17</v>
+      </c>
+      <c r="BP291">
+        <v>2.1</v>
+      </c>
+      <c r="BQ291">
+        <v>1.82</v>
+      </c>
+      <c r="BR291">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="292" spans="1:70">
+      <c r="A292" t="s">
+        <v>70</v>
+      </c>
+      <c r="B292" s="1">
+        <v>41583</v>
+      </c>
+      <c r="C292" t="s">
+        <v>84</v>
+      </c>
+      <c r="D292" t="s">
+        <v>82</v>
+      </c>
+      <c r="E292">
+        <v>1</v>
+      </c>
+      <c r="F292">
+        <v>2</v>
+      </c>
+      <c r="G292" t="s">
+        <v>78</v>
+      </c>
+      <c r="H292">
+        <v>1</v>
+      </c>
+      <c r="I292">
+        <v>0</v>
+      </c>
+      <c r="J292" t="s">
+        <v>74</v>
+      </c>
+      <c r="K292">
+        <v>18</v>
+      </c>
+      <c r="L292">
+        <v>15</v>
+      </c>
+      <c r="M292">
+        <v>6</v>
+      </c>
+      <c r="N292">
+        <v>5</v>
+      </c>
+      <c r="O292">
+        <v>20</v>
+      </c>
+      <c r="P292">
+        <v>16</v>
+      </c>
+      <c r="Q292">
+        <v>5</v>
+      </c>
+      <c r="R292">
+        <v>8</v>
+      </c>
+      <c r="S292">
+        <v>0</v>
+      </c>
+      <c r="T292">
+        <v>2</v>
+      </c>
+      <c r="U292">
+        <v>0</v>
+      </c>
+      <c r="V292">
+        <v>0</v>
+      </c>
+      <c r="W292">
+        <v>4.5</v>
+      </c>
+      <c r="X292">
+        <v>3.75</v>
+      </c>
+      <c r="Y292">
+        <v>1.75</v>
+      </c>
+      <c r="Z292">
+        <v>4.25</v>
+      </c>
+      <c r="AA292">
+        <v>3.8</v>
+      </c>
+      <c r="AB292">
+        <v>1.75</v>
+      </c>
+      <c r="AC292">
+        <v>4.25</v>
+      </c>
+      <c r="AD292">
+        <v>3.8</v>
+      </c>
+      <c r="AE292">
+        <v>1.75</v>
+      </c>
+      <c r="AF292">
+        <v>3.9</v>
+      </c>
+      <c r="AG292">
+        <v>3.5</v>
+      </c>
+      <c r="AH292">
+        <v>1.85</v>
+      </c>
+      <c r="AI292">
+        <v>4.33</v>
+      </c>
+      <c r="AJ292">
+        <v>3.6</v>
+      </c>
+      <c r="AK292">
+        <v>1.8</v>
+      </c>
+      <c r="AL292">
+        <v>4.84</v>
+      </c>
+      <c r="AM292">
+        <v>3.88</v>
+      </c>
+      <c r="AN292">
+        <v>1.8</v>
+      </c>
+      <c r="AO292">
+        <v>4.5</v>
+      </c>
+      <c r="AP292">
+        <v>3.5</v>
+      </c>
+      <c r="AQ292">
+        <v>1.8</v>
+      </c>
+      <c r="AR292">
+        <v>4.5</v>
+      </c>
+      <c r="AS292">
+        <v>3.6</v>
+      </c>
+      <c r="AT292">
+        <v>1.73</v>
+      </c>
+      <c r="AU292">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AV292">
+        <v>3.8</v>
+      </c>
+      <c r="AW292">
+        <v>1.8</v>
+      </c>
+      <c r="AX292">
+        <v>4.33</v>
+      </c>
+      <c r="AY292">
+        <v>3.75</v>
+      </c>
+      <c r="AZ292">
+        <v>1.75</v>
+      </c>
+      <c r="BA292">
+        <v>40</v>
+      </c>
+      <c r="BB292">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="BC292">
+        <v>4.41</v>
+      </c>
+      <c r="BD292">
+        <v>3.87</v>
+      </c>
+      <c r="BE292">
+        <v>3.66</v>
+      </c>
+      <c r="BF292">
+        <v>1.85</v>
+      </c>
+      <c r="BG292">
+        <v>1.77</v>
+      </c>
+      <c r="BH292">
+        <v>35</v>
+      </c>
+      <c r="BI292">
+        <v>1.77</v>
+      </c>
+      <c r="BJ292">
+        <v>1.71</v>
+      </c>
+      <c r="BK292">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BL292">
+        <v>2.12</v>
+      </c>
+      <c r="BM292">
+        <v>22</v>
+      </c>
+      <c r="BN292">
+        <v>0.5</v>
+      </c>
+      <c r="BO292">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BP292">
+        <v>2.14</v>
+      </c>
+      <c r="BQ292">
+        <v>1.8</v>
+      </c>
+      <c r="BR292">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="293" spans="1:70">
+      <c r="A293" t="s">
+        <v>70</v>
+      </c>
+      <c r="B293" s="1">
+        <v>41583</v>
+      </c>
+      <c r="C293" t="s">
+        <v>89</v>
+      </c>
+      <c r="D293" t="s">
+        <v>86</v>
+      </c>
+      <c r="E293">
+        <v>1</v>
+      </c>
+      <c r="F293">
+        <v>4</v>
+      </c>
+      <c r="G293" t="s">
+        <v>78</v>
+      </c>
+      <c r="H293">
+        <v>0</v>
+      </c>
+      <c r="I293">
+        <v>2</v>
+      </c>
+      <c r="J293" t="s">
+        <v>78</v>
+      </c>
+      <c r="K293">
+        <v>18</v>
+      </c>
+      <c r="L293">
+        <v>15</v>
+      </c>
+      <c r="M293">
+        <v>5</v>
+      </c>
+      <c r="N293">
+        <v>5</v>
+      </c>
+      <c r="O293">
+        <v>20</v>
+      </c>
+      <c r="P293">
+        <v>20</v>
+      </c>
+      <c r="Q293">
+        <v>5</v>
+      </c>
+      <c r="R293">
+        <v>1</v>
+      </c>
+      <c r="S293">
+        <v>0</v>
+      </c>
+      <c r="T293">
+        <v>1</v>
+      </c>
+      <c r="U293">
+        <v>0</v>
+      </c>
+      <c r="V293">
+        <v>0</v>
+      </c>
+      <c r="W293">
+        <v>1.83</v>
+      </c>
+      <c r="X293">
+        <v>3.75</v>
+      </c>
+      <c r="Y293">
+        <v>4</v>
+      </c>
+      <c r="Z293">
+        <v>1.9</v>
+      </c>
+      <c r="AA293">
+        <v>3.7</v>
+      </c>
+      <c r="AB293">
+        <v>3.7</v>
+      </c>
+      <c r="AC293">
+        <v>1.9</v>
+      </c>
+      <c r="AD293">
+        <v>3.7</v>
+      </c>
+      <c r="AE293">
+        <v>3.7</v>
+      </c>
+      <c r="AF293">
+        <v>1.9</v>
+      </c>
+      <c r="AG293">
+        <v>3.5</v>
+      </c>
+      <c r="AH293">
+        <v>3.7</v>
+      </c>
+      <c r="AI293">
+        <v>1.91</v>
+      </c>
+      <c r="AJ293">
+        <v>3.6</v>
+      </c>
+      <c r="AK293">
+        <v>3.8</v>
+      </c>
+      <c r="AL293">
+        <v>1.88</v>
+      </c>
+      <c r="AM293">
+        <v>4.07</v>
+      </c>
+      <c r="AN293">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AO293">
+        <v>1.91</v>
+      </c>
+      <c r="AP293">
+        <v>3.5</v>
+      </c>
+      <c r="AQ293">
+        <v>4</v>
+      </c>
+      <c r="AR293">
+        <v>1.83</v>
+      </c>
+      <c r="AS293">
+        <v>3.6</v>
+      </c>
+      <c r="AT293">
+        <v>3.8</v>
+      </c>
+      <c r="AU293">
+        <v>1.91</v>
+      </c>
+      <c r="AV293">
+        <v>4</v>
+      </c>
+      <c r="AW293">
+        <v>3.9</v>
+      </c>
+      <c r="AX293">
+        <v>1.83</v>
+      </c>
+      <c r="AY293">
+        <v>3.8</v>
+      </c>
+      <c r="AZ293">
+        <v>3.75</v>
+      </c>
+      <c r="BA293">
+        <v>40</v>
+      </c>
+      <c r="BB293">
+        <v>1.91</v>
+      </c>
+      <c r="BC293">
+        <v>1.88</v>
+      </c>
+      <c r="BD293">
+        <v>4.07</v>
+      </c>
+      <c r="BE293">
+        <v>3.71</v>
+      </c>
+      <c r="BF293">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="BG293">
+        <v>3.78</v>
+      </c>
+      <c r="BH293">
+        <v>26</v>
+      </c>
+      <c r="BI293">
+        <v>1.62</v>
+      </c>
+      <c r="BJ293">
+        <v>1.56</v>
+      </c>
+      <c r="BK293">
+        <v>2.6</v>
+      </c>
+      <c r="BL293">
+        <v>2.35</v>
+      </c>
+      <c r="BM293">
+        <v>24</v>
+      </c>
+      <c r="BN293">
+        <v>-0.75</v>
+      </c>
+      <c r="BO293">
+        <v>2.17</v>
+      </c>
+      <c r="BP293">
+        <v>2.11</v>
+      </c>
+      <c r="BQ293">
+        <v>1.82</v>
+      </c>
+      <c r="BR293">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="294" spans="1:70">
+      <c r="A294" t="s">
+        <v>70</v>
+      </c>
+      <c r="B294" s="1">
+        <v>41583</v>
+      </c>
+      <c r="C294" t="s">
+        <v>81</v>
+      </c>
+      <c r="D294" t="s">
+        <v>91</v>
+      </c>
+      <c r="E294">
+        <v>3</v>
+      </c>
+      <c r="F294">
+        <v>1</v>
+      </c>
+      <c r="G294" t="s">
+        <v>74</v>
+      </c>
+      <c r="H294">
+        <v>2</v>
+      </c>
+      <c r="I294">
+        <v>0</v>
+      </c>
+      <c r="J294" t="s">
+        <v>74</v>
+      </c>
+      <c r="K294">
+        <v>22</v>
+      </c>
+      <c r="L294">
+        <v>11</v>
+      </c>
+      <c r="M294">
+        <v>12</v>
+      </c>
+      <c r="N294">
+        <v>3</v>
+      </c>
+      <c r="O294">
+        <v>14</v>
+      </c>
+      <c r="P294">
+        <v>10</v>
+      </c>
+      <c r="Q294">
+        <v>3</v>
+      </c>
+      <c r="R294">
+        <v>6</v>
+      </c>
+      <c r="S294">
+        <v>1</v>
+      </c>
+      <c r="T294">
+        <v>1</v>
+      </c>
+      <c r="U294">
+        <v>0</v>
+      </c>
+      <c r="V294">
+        <v>0</v>
+      </c>
+      <c r="W294">
+        <v>1.3</v>
+      </c>
+      <c r="X294">
+        <v>5.5</v>
+      </c>
+      <c r="Y294">
+        <v>9</v>
+      </c>
+      <c r="Z294">
+        <v>1.3</v>
+      </c>
+      <c r="AA294">
+        <v>5.75</v>
+      </c>
+      <c r="AB294">
+        <v>7.75</v>
+      </c>
+      <c r="AC294">
+        <v>1.3</v>
+      </c>
+      <c r="AD294">
+        <v>5.75</v>
+      </c>
+      <c r="AE294">
+        <v>7.75</v>
+      </c>
+      <c r="AF294">
+        <v>1.4</v>
+      </c>
+      <c r="AG294">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AH294">
+        <v>7.1</v>
+      </c>
+      <c r="AI294">
+        <v>1.33</v>
+      </c>
+      <c r="AJ294">
+        <v>5</v>
+      </c>
+      <c r="AK294">
+        <v>9</v>
+      </c>
+      <c r="AL294">
+        <v>1.32</v>
+      </c>
+      <c r="AM294">
+        <v>6.15</v>
+      </c>
+      <c r="AN294">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="AO294">
+        <v>1.3</v>
+      </c>
+      <c r="AP294">
+        <v>5</v>
+      </c>
+      <c r="AQ294">
+        <v>10</v>
+      </c>
+      <c r="AR294">
+        <v>1.33</v>
+      </c>
+      <c r="AS294">
+        <v>4.8</v>
+      </c>
+      <c r="AT294">
+        <v>8.5</v>
+      </c>
+      <c r="AU294">
+        <v>1.33</v>
+      </c>
+      <c r="AV294">
+        <v>6</v>
+      </c>
+      <c r="AW294">
+        <v>9</v>
+      </c>
+      <c r="AX294">
+        <v>1.3</v>
+      </c>
+      <c r="AY294">
+        <v>5</v>
+      </c>
+      <c r="AZ294">
+        <v>10</v>
+      </c>
+      <c r="BA294">
+        <v>40</v>
+      </c>
+      <c r="BB294">
+        <v>1.4</v>
+      </c>
+      <c r="BC294">
+        <v>1.32</v>
+      </c>
+      <c r="BD294">
+        <v>6.15</v>
+      </c>
+      <c r="BE294">
+        <v>5.18</v>
+      </c>
+      <c r="BF294">
+        <v>10</v>
+      </c>
+      <c r="BG294">
+        <v>8.77</v>
+      </c>
+      <c r="BH294">
+        <v>24</v>
+      </c>
+      <c r="BI294">
+        <v>1.43</v>
+      </c>
+      <c r="BJ294">
+        <v>1.36</v>
+      </c>
+      <c r="BK294">
+        <v>3.25</v>
+      </c>
+      <c r="BL294">
+        <v>2.98</v>
+      </c>
+      <c r="BM294">
+        <v>25</v>
+      </c>
+      <c r="BN294">
+        <v>-1.5</v>
+      </c>
+      <c r="BO294">
+        <v>1.92</v>
+      </c>
+      <c r="BP294">
+        <v>1.86</v>
+      </c>
+      <c r="BQ294">
+        <v>2.06</v>
+      </c>
+      <c r="BR294">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="295" spans="1:70">
+      <c r="A295" t="s">
+        <v>70</v>
+      </c>
+      <c r="B295" s="1">
+        <v>41583</v>
+      </c>
+      <c r="C295" t="s">
+        <v>83</v>
+      </c>
+      <c r="D295" t="s">
+        <v>88</v>
+      </c>
+      <c r="E295">
+        <v>2</v>
+      </c>
+      <c r="F295">
+        <v>4</v>
+      </c>
+      <c r="G295" t="s">
+        <v>78</v>
+      </c>
+      <c r="H295">
+        <v>1</v>
+      </c>
+      <c r="I295">
+        <v>1</v>
+      </c>
+      <c r="J295" t="s">
+        <v>79</v>
+      </c>
+      <c r="K295">
+        <v>10</v>
+      </c>
+      <c r="L295">
+        <v>17</v>
+      </c>
+      <c r="M295">
+        <v>4</v>
+      </c>
+      <c r="N295">
+        <v>6</v>
+      </c>
+      <c r="O295">
+        <v>10</v>
+      </c>
+      <c r="P295">
+        <v>12</v>
+      </c>
+      <c r="Q295">
+        <v>3</v>
+      </c>
+      <c r="R295">
+        <v>3</v>
+      </c>
+      <c r="S295">
+        <v>1</v>
+      </c>
+      <c r="T295">
+        <v>0</v>
+      </c>
+      <c r="U295">
+        <v>0</v>
+      </c>
+      <c r="V295">
+        <v>0</v>
+      </c>
+      <c r="W295">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="X295">
+        <v>3.3</v>
+      </c>
+      <c r="Y295">
+        <v>3.3</v>
+      </c>
+      <c r="Z295">
+        <v>2.15</v>
+      </c>
+      <c r="AA295">
+        <v>3.4</v>
+      </c>
+      <c r="AB295">
+        <v>3.2</v>
+      </c>
+      <c r="AC295">
+        <v>2.15</v>
+      </c>
+      <c r="AD295">
+        <v>3.4</v>
+      </c>
+      <c r="AE295">
+        <v>3.2</v>
+      </c>
+      <c r="AF295">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AG295">
+        <v>3.3</v>
+      </c>
+      <c r="AH295">
+        <v>2.9</v>
+      </c>
+      <c r="AI295">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AJ295">
+        <v>3.4</v>
+      </c>
+      <c r="AK295">
+        <v>3.2</v>
+      </c>
+      <c r="AL295">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="AM295">
+        <v>3.61</v>
+      </c>
+      <c r="AN295">
+        <v>3.42</v>
+      </c>
+      <c r="AO295">
+        <v>2.25</v>
+      </c>
+      <c r="AP295">
+        <v>3.2</v>
+      </c>
+      <c r="AQ295">
+        <v>3.3</v>
+      </c>
+      <c r="AR295">
+        <v>2.1</v>
+      </c>
+      <c r="AS295">
+        <v>3.4</v>
+      </c>
+      <c r="AT295">
+        <v>3.2</v>
+      </c>
+      <c r="AU295">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AV295">
+        <v>3.6</v>
+      </c>
+      <c r="AW295">
+        <v>3.3</v>
+      </c>
+      <c r="AX295">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AY295">
+        <v>3.4</v>
+      </c>
+      <c r="AZ295">
+        <v>3.1</v>
+      </c>
+      <c r="BA295">
+        <v>39</v>
+      </c>
+      <c r="BB295">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="BC295">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="BD295">
+        <v>3.61</v>
+      </c>
+      <c r="BE295">
+        <v>3.38</v>
+      </c>
+      <c r="BF295">
+        <v>3.44</v>
+      </c>
+      <c r="BG295">
+        <v>3.21</v>
+      </c>
+      <c r="BH295">
+        <v>36</v>
+      </c>
+      <c r="BI295">
+        <v>1.92</v>
+      </c>
+      <c r="BJ295">
+        <v>1.85</v>
+      </c>
+      <c r="BK295">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="BL295">
+        <v>1.96</v>
+      </c>
+      <c r="BM295">
+        <v>24</v>
+      </c>
+      <c r="BN295">
+        <v>-0.25</v>
+      </c>
+      <c r="BO295">
+        <v>1.92</v>
+      </c>
+      <c r="BP295">
+        <v>1.88</v>
+      </c>
+      <c r="BQ295">
+        <v>2.04</v>
+      </c>
+      <c r="BR295">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="296" spans="1:70">
+      <c r="A296" t="s">
+        <v>70</v>
+      </c>
+      <c r="B296" s="1">
+        <v>41583</v>
+      </c>
+      <c r="C296" t="s">
+        <v>92</v>
+      </c>
+      <c r="D296" t="s">
+        <v>93</v>
+      </c>
+      <c r="E296">
+        <v>1</v>
+      </c>
+      <c r="F296">
+        <v>2</v>
+      </c>
+      <c r="G296" t="s">
+        <v>78</v>
+      </c>
+      <c r="H296">
+        <v>0</v>
+      </c>
+      <c r="I296">
+        <v>1</v>
+      </c>
+      <c r="J296" t="s">
+        <v>78</v>
+      </c>
+      <c r="K296">
+        <v>19</v>
+      </c>
+      <c r="L296">
+        <v>8</v>
+      </c>
+      <c r="M296">
+        <v>4</v>
+      </c>
+      <c r="N296">
+        <v>4</v>
+      </c>
+      <c r="O296">
+        <v>12</v>
+      </c>
+      <c r="P296">
+        <v>20</v>
+      </c>
+      <c r="Q296">
+        <v>3</v>
+      </c>
+      <c r="R296">
+        <v>1</v>
+      </c>
+      <c r="S296">
+        <v>0</v>
+      </c>
+      <c r="T296">
+        <v>2</v>
+      </c>
+      <c r="U296">
+        <v>0</v>
+      </c>
+      <c r="V296">
+        <v>0</v>
+      </c>
+      <c r="W296">
+        <v>1.36</v>
+      </c>
+      <c r="X296">
+        <v>4.75</v>
+      </c>
+      <c r="Y296">
+        <v>8.5</v>
+      </c>
+      <c r="Z296">
+        <v>1.36</v>
+      </c>
+      <c r="AA296">
+        <v>5.25</v>
+      </c>
+      <c r="AB296">
+        <v>7</v>
+      </c>
+      <c r="AC296">
+        <v>1.36</v>
+      </c>
+      <c r="AD296">
+        <v>5.25</v>
+      </c>
+      <c r="AE296">
+        <v>7</v>
+      </c>
+      <c r="AF296">
+        <v>1.35</v>
+      </c>
+      <c r="AG296">
+        <v>5</v>
+      </c>
+      <c r="AH296">
+        <v>7.2</v>
+      </c>
+      <c r="AI296">
+        <v>1.36</v>
+      </c>
+      <c r="AJ296">
+        <v>5</v>
+      </c>
+      <c r="AK296">
+        <v>7.5</v>
+      </c>
+      <c r="AL296">
+        <v>1.38</v>
+      </c>
+      <c r="AM296">
+        <v>5.45</v>
+      </c>
+      <c r="AN296">
+        <v>8.75</v>
+      </c>
+      <c r="AO296">
+        <v>1.4</v>
+      </c>
+      <c r="AP296">
+        <v>4.5</v>
+      </c>
+      <c r="AQ296">
+        <v>8</v>
+      </c>
+      <c r="AR296">
+        <v>1.36</v>
+      </c>
+      <c r="AS296">
+        <v>4.5</v>
+      </c>
+      <c r="AT296">
+        <v>8</v>
+      </c>
+      <c r="AU296">
+        <v>1.4</v>
+      </c>
+      <c r="AV296">
+        <v>5.4</v>
+      </c>
+      <c r="AW296">
+        <v>7.5</v>
+      </c>
+      <c r="AX296">
+        <v>1.36</v>
+      </c>
+      <c r="AY296">
+        <v>4.75</v>
+      </c>
+      <c r="AZ296">
+        <v>8</v>
+      </c>
+      <c r="BA296">
+        <v>40</v>
+      </c>
+      <c r="BB296">
+        <v>1.4</v>
+      </c>
+      <c r="BC296">
+        <v>1.36</v>
+      </c>
+      <c r="BD296">
+        <v>5.6</v>
+      </c>
+      <c r="BE296">
+        <v>4.8899999999999997</v>
+      </c>
+      <c r="BF296">
+        <v>9.5</v>
+      </c>
+      <c r="BG296">
+        <v>7.79</v>
+      </c>
+      <c r="BH296">
+        <v>24</v>
+      </c>
+      <c r="BI296">
+        <v>1.46</v>
+      </c>
+      <c r="BJ296">
+        <v>1.4</v>
+      </c>
+      <c r="BK296">
+        <v>3.1</v>
+      </c>
+      <c r="BL296">
+        <v>2.83</v>
+      </c>
+      <c r="BM296">
+        <v>25</v>
+      </c>
+      <c r="BN296">
+        <v>-1.5</v>
+      </c>
+      <c r="BO296">
+        <v>2.09</v>
+      </c>
+      <c r="BP296">
+        <v>2.02</v>
+      </c>
+      <c r="BQ296">
+        <v>1.9</v>
+      </c>
+      <c r="BR296">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="297" spans="1:70">
+      <c r="A297" t="s">
+        <v>70</v>
+      </c>
+      <c r="B297" s="1">
+        <v>41583</v>
+      </c>
+      <c r="C297" t="s">
+        <v>73</v>
+      </c>
+      <c r="D297" t="s">
+        <v>80</v>
+      </c>
+      <c r="E297">
+        <v>1</v>
+      </c>
+      <c r="F297">
+        <v>1</v>
+      </c>
+      <c r="G297" t="s">
+        <v>79</v>
+      </c>
+      <c r="H297">
+        <v>1</v>
+      </c>
+      <c r="I297">
+        <v>0</v>
+      </c>
+      <c r="J297" t="s">
+        <v>74</v>
+      </c>
+      <c r="K297">
+        <v>15</v>
+      </c>
+      <c r="L297">
+        <v>10</v>
+      </c>
+      <c r="M297">
+        <v>3</v>
+      </c>
+      <c r="N297">
+        <v>2</v>
+      </c>
+      <c r="O297">
+        <v>10</v>
+      </c>
+      <c r="P297">
+        <v>11</v>
+      </c>
+      <c r="Q297">
+        <v>8</v>
+      </c>
+      <c r="R297">
+        <v>3</v>
+      </c>
+      <c r="S297">
+        <v>1</v>
+      </c>
+      <c r="T297">
+        <v>1</v>
+      </c>
+      <c r="U297">
+        <v>0</v>
+      </c>
+      <c r="V297">
+        <v>0</v>
+      </c>
+      <c r="W297">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="X297">
+        <v>3.6</v>
+      </c>
+      <c r="Y297">
+        <v>3</v>
+      </c>
+      <c r="Z297">
+        <v>2.15</v>
+      </c>
+      <c r="AA297">
+        <v>3.5</v>
+      </c>
+      <c r="AB297">
+        <v>3.1</v>
+      </c>
+      <c r="AC297">
+        <v>2.15</v>
+      </c>
+      <c r="AD297">
+        <v>3.5</v>
+      </c>
+      <c r="AE297">
+        <v>3.1</v>
+      </c>
+      <c r="AF297">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AG297">
+        <v>3.3</v>
+      </c>
+      <c r="AH297">
+        <v>3.1</v>
+      </c>
+      <c r="AI297">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AJ297">
+        <v>3.5</v>
+      </c>
+      <c r="AK297">
+        <v>3.1</v>
+      </c>
+      <c r="AL297">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AM297">
+        <v>3.78</v>
+      </c>
+      <c r="AN297">
+        <v>3.3</v>
+      </c>
+      <c r="AO297">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AP297">
+        <v>3.3</v>
+      </c>
+      <c r="AQ297">
+        <v>3.3</v>
+      </c>
+      <c r="AR297">
+        <v>2.1</v>
+      </c>
+      <c r="AS297">
+        <v>3.4</v>
+      </c>
+      <c r="AT297">
+        <v>3.13</v>
+      </c>
+      <c r="AU297">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AV297">
+        <v>3.75</v>
+      </c>
+      <c r="AW297">
+        <v>3.25</v>
+      </c>
+      <c r="AX297">
+        <v>2.15</v>
+      </c>
+      <c r="AY297">
+        <v>3.5</v>
+      </c>
+      <c r="AZ297">
+        <v>3.1</v>
+      </c>
+      <c r="BA297">
+        <v>40</v>
+      </c>
+      <c r="BB297">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="BC297">
+        <v>2.17</v>
+      </c>
+      <c r="BD297">
+        <v>3.8</v>
+      </c>
+      <c r="BE297">
+        <v>3.5</v>
+      </c>
+      <c r="BF297">
+        <v>3.35</v>
+      </c>
+      <c r="BG297">
+        <v>3.14</v>
+      </c>
+      <c r="BH297">
+        <v>24</v>
+      </c>
+      <c r="BI297">
+        <v>1.56</v>
+      </c>
+      <c r="BJ297">
+        <v>1.5</v>
+      </c>
+      <c r="BK297">
+        <v>2.74</v>
+      </c>
+      <c r="BL297">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="BM297">
+        <v>24</v>
+      </c>
+      <c r="BN297">
+        <v>-0.25</v>
+      </c>
+      <c r="BO297">
+        <v>1.92</v>
+      </c>
+      <c r="BP297">
+        <v>1.88</v>
+      </c>
+      <c r="BQ297">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="BR297">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="298" spans="1:70">
+      <c r="A298" t="s">
+        <v>70</v>
+      </c>
+      <c r="B298" s="1">
+        <v>41583</v>
+      </c>
+      <c r="C298" t="s">
+        <v>94</v>
+      </c>
+      <c r="D298" t="s">
+        <v>72</v>
+      </c>
+      <c r="E298">
+        <v>3</v>
+      </c>
+      <c r="F298">
+        <v>3</v>
+      </c>
+      <c r="G298" t="s">
+        <v>79</v>
+      </c>
+      <c r="H298">
+        <v>3</v>
+      </c>
+      <c r="I298">
+        <v>1</v>
+      </c>
+      <c r="J298" t="s">
+        <v>74</v>
+      </c>
+      <c r="K298">
+        <v>10</v>
+      </c>
+      <c r="L298">
+        <v>10</v>
+      </c>
+      <c r="M298">
+        <v>3</v>
+      </c>
+      <c r="N298">
+        <v>4</v>
+      </c>
+      <c r="O298">
+        <v>23</v>
+      </c>
+      <c r="P298">
+        <v>12</v>
+      </c>
+      <c r="Q298">
+        <v>7</v>
+      </c>
+      <c r="R298">
+        <v>4</v>
+      </c>
+      <c r="S298">
+        <v>1</v>
+      </c>
+      <c r="T298">
+        <v>2</v>
+      </c>
+      <c r="U298">
+        <v>0</v>
+      </c>
+      <c r="V298">
+        <v>0</v>
+      </c>
+      <c r="W298">
+        <v>4</v>
+      </c>
+      <c r="X298">
+        <v>3.6</v>
+      </c>
+      <c r="Y298">
+        <v>1.85</v>
+      </c>
+      <c r="Z298">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AA298">
+        <v>3.6</v>
+      </c>
+      <c r="AB298">
+        <v>1.83</v>
+      </c>
+      <c r="AC298">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AD298">
+        <v>3.6</v>
+      </c>
+      <c r="AE298">
+        <v>1.83</v>
+      </c>
+      <c r="AF298">
+        <v>3.7</v>
+      </c>
+      <c r="AG298">
+        <v>3.5</v>
+      </c>
+      <c r="AH298">
+        <v>1.9</v>
+      </c>
+      <c r="AI298">
+        <v>4.33</v>
+      </c>
+      <c r="AJ298">
+        <v>3.75</v>
+      </c>
+      <c r="AK298">
+        <v>1.75</v>
+      </c>
+      <c r="AL298">
+        <v>4.29</v>
+      </c>
+      <c r="AM298">
+        <v>4</v>
+      </c>
+      <c r="AN298">
+        <v>1.86</v>
+      </c>
+      <c r="AO298">
+        <v>4</v>
+      </c>
+      <c r="AP298">
+        <v>3.5</v>
+      </c>
+      <c r="AQ298">
+        <v>1.91</v>
+      </c>
+      <c r="AR298">
+        <v>4.33</v>
+      </c>
+      <c r="AS298">
+        <v>3.5</v>
+      </c>
+      <c r="AT298">
+        <v>1.8</v>
+      </c>
+      <c r="AU298">
+        <v>3.9</v>
+      </c>
+      <c r="AV298">
+        <v>4</v>
+      </c>
+      <c r="AW298">
+        <v>1.91</v>
+      </c>
+      <c r="AX298">
+        <v>3.75</v>
+      </c>
+      <c r="AY298">
+        <v>3.8</v>
+      </c>
+      <c r="AZ298">
+        <v>1.83</v>
+      </c>
+      <c r="BA298">
+        <v>40</v>
+      </c>
+      <c r="BB298">
+        <v>4.33</v>
+      </c>
+      <c r="BC298">
+        <v>3.95</v>
+      </c>
+      <c r="BD298">
+        <v>4.05</v>
+      </c>
+      <c r="BE298">
+        <v>3.7</v>
+      </c>
+      <c r="BF298">
+        <v>1.91</v>
+      </c>
+      <c r="BG298">
+        <v>1.84</v>
+      </c>
+      <c r="BH298">
+        <v>24</v>
+      </c>
+      <c r="BI298">
+        <v>1.57</v>
+      </c>
+      <c r="BJ298">
+        <v>1.48</v>
+      </c>
+      <c r="BK298">
+        <v>2.75</v>
+      </c>
+      <c r="BL298">
+        <v>2.54</v>
+      </c>
+      <c r="BM298">
+        <v>24</v>
+      </c>
+      <c r="BN298">
+        <v>0.75</v>
+      </c>
+      <c r="BO298">
+        <v>1.84</v>
+      </c>
+      <c r="BP298">
+        <v>1.8</v>
+      </c>
+      <c r="BQ298">
+        <v>2.15</v>
+      </c>
+      <c r="BR298">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizaciones finales temporada 1213
</commit_message>
<xml_diff>
--- a/DatosAle1/DP1213.xlsx
+++ b/DatosAle1/DP1213.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="630" windowWidth="8115" windowHeight="7680"/>
+    <workbookView xWindow="720" yWindow="660" windowWidth="9075" windowHeight="3855"/>
   </bookViews>
   <sheets>
     <sheet name="D1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1736" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1790" uniqueCount="150">
   <si>
     <t>Div</t>
   </si>
@@ -461,6 +461,9 @@
   </si>
   <si>
     <t>28/04/13</t>
+  </si>
+  <si>
+    <t>18/05/13</t>
   </si>
 </sst>
 </file>
@@ -1283,7 +1286,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BR298"/>
+  <dimension ref="A1:BR307"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -64465,6 +64468,1914 @@
         <v>2.0699999999999998</v>
       </c>
     </row>
+    <row r="299" spans="1:70">
+      <c r="A299" t="s">
+        <v>70</v>
+      </c>
+      <c r="B299" t="s">
+        <v>149</v>
+      </c>
+      <c r="C299" t="s">
+        <v>76</v>
+      </c>
+      <c r="D299" t="s">
+        <v>84</v>
+      </c>
+      <c r="E299">
+        <v>3</v>
+      </c>
+      <c r="F299">
+        <v>1</v>
+      </c>
+      <c r="G299" t="s">
+        <v>74</v>
+      </c>
+      <c r="H299">
+        <v>1</v>
+      </c>
+      <c r="I299">
+        <v>0</v>
+      </c>
+      <c r="J299" t="s">
+        <v>74</v>
+      </c>
+      <c r="K299">
+        <v>16</v>
+      </c>
+      <c r="L299">
+        <v>6</v>
+      </c>
+      <c r="M299">
+        <v>5</v>
+      </c>
+      <c r="N299">
+        <v>2</v>
+      </c>
+      <c r="O299">
+        <v>19</v>
+      </c>
+      <c r="P299">
+        <v>22</v>
+      </c>
+      <c r="Q299">
+        <v>8</v>
+      </c>
+      <c r="R299">
+        <v>3</v>
+      </c>
+      <c r="S299">
+        <v>2</v>
+      </c>
+      <c r="T299">
+        <v>3</v>
+      </c>
+      <c r="U299">
+        <v>0</v>
+      </c>
+      <c r="V299">
+        <v>0</v>
+      </c>
+      <c r="W299">
+        <v>1.5</v>
+      </c>
+      <c r="X299">
+        <v>4.33</v>
+      </c>
+      <c r="Y299">
+        <v>6</v>
+      </c>
+      <c r="Z299">
+        <v>1.42</v>
+      </c>
+      <c r="AA299">
+        <v>4.5</v>
+      </c>
+      <c r="AB299">
+        <v>7</v>
+      </c>
+      <c r="AC299">
+        <v>1.42</v>
+      </c>
+      <c r="AD299">
+        <v>4.5</v>
+      </c>
+      <c r="AE299">
+        <v>7</v>
+      </c>
+      <c r="AF299">
+        <v>1.42</v>
+      </c>
+      <c r="AG299">
+        <v>4.5</v>
+      </c>
+      <c r="AH299">
+        <v>6.5</v>
+      </c>
+      <c r="AI299">
+        <v>1.44</v>
+      </c>
+      <c r="AJ299">
+        <v>4.33</v>
+      </c>
+      <c r="AK299">
+        <v>7</v>
+      </c>
+      <c r="AL299">
+        <v>1.49</v>
+      </c>
+      <c r="AM299">
+        <v>4.66</v>
+      </c>
+      <c r="AN299">
+        <v>7.35</v>
+      </c>
+      <c r="AO299">
+        <v>1.44</v>
+      </c>
+      <c r="AP299">
+        <v>4.33</v>
+      </c>
+      <c r="AQ299">
+        <v>7</v>
+      </c>
+      <c r="AR299">
+        <v>1.44</v>
+      </c>
+      <c r="AS299">
+        <v>4.33</v>
+      </c>
+      <c r="AT299">
+        <v>6.5</v>
+      </c>
+      <c r="AU299">
+        <v>1.5</v>
+      </c>
+      <c r="AV299">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AW299">
+        <v>7</v>
+      </c>
+      <c r="AX299">
+        <v>1.44</v>
+      </c>
+      <c r="AY299">
+        <v>4.5</v>
+      </c>
+      <c r="AZ299">
+        <v>6.5</v>
+      </c>
+      <c r="BA299">
+        <v>40</v>
+      </c>
+      <c r="BB299">
+        <v>1.5</v>
+      </c>
+      <c r="BC299">
+        <v>1.46</v>
+      </c>
+      <c r="BD299">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="BE299">
+        <v>4.42</v>
+      </c>
+      <c r="BF299">
+        <v>7.5</v>
+      </c>
+      <c r="BG299">
+        <v>6.81</v>
+      </c>
+      <c r="BH299">
+        <v>33</v>
+      </c>
+      <c r="BI299">
+        <v>1.71</v>
+      </c>
+      <c r="BJ299">
+        <v>1.63</v>
+      </c>
+      <c r="BK299">
+        <v>2.35</v>
+      </c>
+      <c r="BL299">
+        <v>2.23</v>
+      </c>
+      <c r="BM299">
+        <v>25</v>
+      </c>
+      <c r="BN299">
+        <v>-1.25</v>
+      </c>
+      <c r="BO299">
+        <v>2.15</v>
+      </c>
+      <c r="BP299">
+        <v>2.08</v>
+      </c>
+      <c r="BQ299">
+        <v>1.83</v>
+      </c>
+      <c r="BR299">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="300" spans="1:70">
+      <c r="A300" t="s">
+        <v>70</v>
+      </c>
+      <c r="B300" t="s">
+        <v>149</v>
+      </c>
+      <c r="C300" t="s">
+        <v>72</v>
+      </c>
+      <c r="D300" t="s">
+        <v>89</v>
+      </c>
+      <c r="E300">
+        <v>1</v>
+      </c>
+      <c r="F300">
+        <v>2</v>
+      </c>
+      <c r="G300" t="s">
+        <v>78</v>
+      </c>
+      <c r="H300">
+        <v>1</v>
+      </c>
+      <c r="I300">
+        <v>0</v>
+      </c>
+      <c r="J300" t="s">
+        <v>74</v>
+      </c>
+      <c r="K300">
+        <v>21</v>
+      </c>
+      <c r="L300">
+        <v>9</v>
+      </c>
+      <c r="M300">
+        <v>8</v>
+      </c>
+      <c r="N300">
+        <v>5</v>
+      </c>
+      <c r="O300">
+        <v>13</v>
+      </c>
+      <c r="P300">
+        <v>20</v>
+      </c>
+      <c r="Q300">
+        <v>3</v>
+      </c>
+      <c r="R300">
+        <v>0</v>
+      </c>
+      <c r="S300">
+        <v>1</v>
+      </c>
+      <c r="T300">
+        <v>4</v>
+      </c>
+      <c r="U300">
+        <v>1</v>
+      </c>
+      <c r="V300">
+        <v>0</v>
+      </c>
+      <c r="W300">
+        <v>1.33</v>
+      </c>
+      <c r="X300">
+        <v>5</v>
+      </c>
+      <c r="Y300">
+        <v>8.5</v>
+      </c>
+      <c r="Z300">
+        <v>1.3</v>
+      </c>
+      <c r="AA300">
+        <v>5.75</v>
+      </c>
+      <c r="AB300">
+        <v>8</v>
+      </c>
+      <c r="AC300">
+        <v>1.3</v>
+      </c>
+      <c r="AD300">
+        <v>5.75</v>
+      </c>
+      <c r="AE300">
+        <v>8</v>
+      </c>
+      <c r="AF300">
+        <v>1.45</v>
+      </c>
+      <c r="AG300">
+        <v>4.3</v>
+      </c>
+      <c r="AH300">
+        <v>6.3</v>
+      </c>
+      <c r="AI300">
+        <v>1.4</v>
+      </c>
+      <c r="AJ300">
+        <v>5</v>
+      </c>
+      <c r="AK300">
+        <v>6.5</v>
+      </c>
+      <c r="AL300">
+        <v>1.38</v>
+      </c>
+      <c r="AM300">
+        <v>5.78</v>
+      </c>
+      <c r="AN300">
+        <v>8.11</v>
+      </c>
+      <c r="AO300">
+        <v>1.4</v>
+      </c>
+      <c r="AP300">
+        <v>4.8</v>
+      </c>
+      <c r="AQ300">
+        <v>7</v>
+      </c>
+      <c r="AR300">
+        <v>1.33</v>
+      </c>
+      <c r="AS300">
+        <v>5</v>
+      </c>
+      <c r="AT300">
+        <v>7.5</v>
+      </c>
+      <c r="AU300">
+        <v>1.4</v>
+      </c>
+      <c r="AV300">
+        <v>5.5</v>
+      </c>
+      <c r="AW300">
+        <v>7.5</v>
+      </c>
+      <c r="AX300">
+        <v>1.4</v>
+      </c>
+      <c r="AY300">
+        <v>5</v>
+      </c>
+      <c r="AZ300">
+        <v>6.5</v>
+      </c>
+      <c r="BA300">
+        <v>40</v>
+      </c>
+      <c r="BB300">
+        <v>1.45</v>
+      </c>
+      <c r="BC300">
+        <v>1.37</v>
+      </c>
+      <c r="BD300">
+        <v>5.83</v>
+      </c>
+      <c r="BE300">
+        <v>5.21</v>
+      </c>
+      <c r="BF300">
+        <v>8.5</v>
+      </c>
+      <c r="BG300">
+        <v>7.31</v>
+      </c>
+      <c r="BH300">
+        <v>26</v>
+      </c>
+      <c r="BI300">
+        <v>1.36</v>
+      </c>
+      <c r="BJ300">
+        <v>1.3</v>
+      </c>
+      <c r="BK300">
+        <v>3.65</v>
+      </c>
+      <c r="BL300">
+        <v>3.32</v>
+      </c>
+      <c r="BM300">
+        <v>26</v>
+      </c>
+      <c r="BN300">
+        <v>-1.5</v>
+      </c>
+      <c r="BO300">
+        <v>1.98</v>
+      </c>
+      <c r="BP300">
+        <v>1.94</v>
+      </c>
+      <c r="BQ300">
+        <v>2</v>
+      </c>
+      <c r="BR300">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="301" spans="1:70">
+      <c r="A301" t="s">
+        <v>70</v>
+      </c>
+      <c r="B301" t="s">
+        <v>149</v>
+      </c>
+      <c r="C301" t="s">
+        <v>80</v>
+      </c>
+      <c r="D301" t="s">
+        <v>94</v>
+      </c>
+      <c r="E301">
+        <v>2</v>
+      </c>
+      <c r="F301">
+        <v>2</v>
+      </c>
+      <c r="G301" t="s">
+        <v>79</v>
+      </c>
+      <c r="H301">
+        <v>1</v>
+      </c>
+      <c r="I301">
+        <v>2</v>
+      </c>
+      <c r="J301" t="s">
+        <v>78</v>
+      </c>
+      <c r="K301">
+        <v>11</v>
+      </c>
+      <c r="L301">
+        <v>14</v>
+      </c>
+      <c r="M301">
+        <v>3</v>
+      </c>
+      <c r="N301">
+        <v>4</v>
+      </c>
+      <c r="O301">
+        <v>18</v>
+      </c>
+      <c r="P301">
+        <v>13</v>
+      </c>
+      <c r="Q301">
+        <v>6</v>
+      </c>
+      <c r="R301">
+        <v>9</v>
+      </c>
+      <c r="S301">
+        <v>3</v>
+      </c>
+      <c r="T301">
+        <v>1</v>
+      </c>
+      <c r="U301">
+        <v>0</v>
+      </c>
+      <c r="V301">
+        <v>1</v>
+      </c>
+      <c r="W301">
+        <v>2</v>
+      </c>
+      <c r="X301">
+        <v>3.6</v>
+      </c>
+      <c r="Y301">
+        <v>3.5</v>
+      </c>
+      <c r="Z301">
+        <v>2</v>
+      </c>
+      <c r="AA301">
+        <v>3.6</v>
+      </c>
+      <c r="AB301">
+        <v>3.4</v>
+      </c>
+      <c r="AC301">
+        <v>2</v>
+      </c>
+      <c r="AD301">
+        <v>3.6</v>
+      </c>
+      <c r="AE301">
+        <v>3.4</v>
+      </c>
+      <c r="AF301">
+        <v>1.75</v>
+      </c>
+      <c r="AG301">
+        <v>3.7</v>
+      </c>
+      <c r="AH301">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AI301">
+        <v>2</v>
+      </c>
+      <c r="AJ301">
+        <v>3.6</v>
+      </c>
+      <c r="AK301">
+        <v>3.5</v>
+      </c>
+      <c r="AL301">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="AM301">
+        <v>3.73</v>
+      </c>
+      <c r="AN301">
+        <v>3.72</v>
+      </c>
+      <c r="AO301">
+        <v>2</v>
+      </c>
+      <c r="AP301">
+        <v>3.6</v>
+      </c>
+      <c r="AQ301">
+        <v>3.5</v>
+      </c>
+      <c r="AR301">
+        <v>1.95</v>
+      </c>
+      <c r="AS301">
+        <v>3.6</v>
+      </c>
+      <c r="AT301">
+        <v>3.5</v>
+      </c>
+      <c r="AU301">
+        <v>2.1</v>
+      </c>
+      <c r="AV301">
+        <v>3.75</v>
+      </c>
+      <c r="AW301">
+        <v>3.5</v>
+      </c>
+      <c r="AX301">
+        <v>1.83</v>
+      </c>
+      <c r="AY301">
+        <v>3.8</v>
+      </c>
+      <c r="AZ301">
+        <v>3.75</v>
+      </c>
+      <c r="BA301">
+        <v>40</v>
+      </c>
+      <c r="BB301">
+        <v>2.1</v>
+      </c>
+      <c r="BC301">
+        <v>1.98</v>
+      </c>
+      <c r="BD301">
+        <v>3.75</v>
+      </c>
+      <c r="BE301">
+        <v>3.59</v>
+      </c>
+      <c r="BF301">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="BG301">
+        <v>3.63</v>
+      </c>
+      <c r="BH301">
+        <v>26</v>
+      </c>
+      <c r="BI301">
+        <v>1.57</v>
+      </c>
+      <c r="BJ301">
+        <v>1.49</v>
+      </c>
+      <c r="BK301">
+        <v>2.62</v>
+      </c>
+      <c r="BL301">
+        <v>2.5</v>
+      </c>
+      <c r="BM301">
+        <v>24</v>
+      </c>
+      <c r="BN301">
+        <v>-0.25</v>
+      </c>
+      <c r="BO301">
+        <v>1.82</v>
+      </c>
+      <c r="BP301">
+        <v>1.76</v>
+      </c>
+      <c r="BQ301">
+        <v>2.17</v>
+      </c>
+      <c r="BR301">
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="302" spans="1:70">
+      <c r="A302" t="s">
+        <v>70</v>
+      </c>
+      <c r="B302" t="s">
+        <v>149</v>
+      </c>
+      <c r="C302" t="s">
+        <v>82</v>
+      </c>
+      <c r="D302" t="s">
+        <v>92</v>
+      </c>
+      <c r="E302">
+        <v>1</v>
+      </c>
+      <c r="F302">
+        <v>2</v>
+      </c>
+      <c r="G302" t="s">
+        <v>78</v>
+      </c>
+      <c r="H302">
+        <v>0</v>
+      </c>
+      <c r="I302">
+        <v>1</v>
+      </c>
+      <c r="J302" t="s">
+        <v>78</v>
+      </c>
+      <c r="K302">
+        <v>14</v>
+      </c>
+      <c r="L302">
+        <v>12</v>
+      </c>
+      <c r="M302">
+        <v>3</v>
+      </c>
+      <c r="N302">
+        <v>3</v>
+      </c>
+      <c r="O302">
+        <v>16</v>
+      </c>
+      <c r="P302">
+        <v>14</v>
+      </c>
+      <c r="Q302">
+        <v>5</v>
+      </c>
+      <c r="R302">
+        <v>2</v>
+      </c>
+      <c r="S302">
+        <v>2</v>
+      </c>
+      <c r="T302">
+        <v>1</v>
+      </c>
+      <c r="U302">
+        <v>0</v>
+      </c>
+      <c r="V302">
+        <v>0</v>
+      </c>
+      <c r="W302">
+        <v>2.75</v>
+      </c>
+      <c r="X302">
+        <v>3.5</v>
+      </c>
+      <c r="Y302">
+        <v>2.4</v>
+      </c>
+      <c r="Z302">
+        <v>2.75</v>
+      </c>
+      <c r="AA302">
+        <v>3.6</v>
+      </c>
+      <c r="AB302">
+        <v>2.35</v>
+      </c>
+      <c r="AC302">
+        <v>2.75</v>
+      </c>
+      <c r="AD302">
+        <v>3.6</v>
+      </c>
+      <c r="AE302">
+        <v>2.35</v>
+      </c>
+      <c r="AF302">
+        <v>2.6</v>
+      </c>
+      <c r="AG302">
+        <v>3.2</v>
+      </c>
+      <c r="AH302">
+        <v>2.6</v>
+      </c>
+      <c r="AI302">
+        <v>2.8</v>
+      </c>
+      <c r="AJ302">
+        <v>3.6</v>
+      </c>
+      <c r="AK302">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AL302">
+        <v>2.95</v>
+      </c>
+      <c r="AM302">
+        <v>3.64</v>
+      </c>
+      <c r="AN302">
+        <v>2.46</v>
+      </c>
+      <c r="AO302">
+        <v>2.8</v>
+      </c>
+      <c r="AP302">
+        <v>3.4</v>
+      </c>
+      <c r="AQ302">
+        <v>2.4</v>
+      </c>
+      <c r="AR302">
+        <v>2.75</v>
+      </c>
+      <c r="AS302">
+        <v>3.5</v>
+      </c>
+      <c r="AT302">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AU302">
+        <v>3</v>
+      </c>
+      <c r="AV302">
+        <v>3.5</v>
+      </c>
+      <c r="AW302">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="AX302">
+        <v>2.8</v>
+      </c>
+      <c r="AY302">
+        <v>3.6</v>
+      </c>
+      <c r="AZ302">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="BA302">
+        <v>40</v>
+      </c>
+      <c r="BB302">
+        <v>3</v>
+      </c>
+      <c r="BC302">
+        <v>2.84</v>
+      </c>
+      <c r="BD302">
+        <v>3.7</v>
+      </c>
+      <c r="BE302">
+        <v>3.5</v>
+      </c>
+      <c r="BF302">
+        <v>2.6</v>
+      </c>
+      <c r="BG302">
+        <v>2.38</v>
+      </c>
+      <c r="BH302">
+        <v>34</v>
+      </c>
+      <c r="BI302">
+        <v>1.76</v>
+      </c>
+      <c r="BJ302">
+        <v>1.6</v>
+      </c>
+      <c r="BK302">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="BL302">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="BM302">
+        <v>25</v>
+      </c>
+      <c r="BN302">
+        <v>0.25</v>
+      </c>
+      <c r="BO302">
+        <v>1.86</v>
+      </c>
+      <c r="BP302">
+        <v>1.81</v>
+      </c>
+      <c r="BQ302">
+        <v>2.13</v>
+      </c>
+      <c r="BR302">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="303" spans="1:70">
+      <c r="A303" t="s">
+        <v>70</v>
+      </c>
+      <c r="B303" t="s">
+        <v>149</v>
+      </c>
+      <c r="C303" t="s">
+        <v>86</v>
+      </c>
+      <c r="D303" t="s">
+        <v>81</v>
+      </c>
+      <c r="E303">
+        <v>0</v>
+      </c>
+      <c r="F303">
+        <v>1</v>
+      </c>
+      <c r="G303" t="s">
+        <v>78</v>
+      </c>
+      <c r="H303">
+        <v>0</v>
+      </c>
+      <c r="I303">
+        <v>0</v>
+      </c>
+      <c r="J303" t="s">
+        <v>79</v>
+      </c>
+      <c r="K303">
+        <v>13</v>
+      </c>
+      <c r="L303">
+        <v>15</v>
+      </c>
+      <c r="M303">
+        <v>1</v>
+      </c>
+      <c r="N303">
+        <v>7</v>
+      </c>
+      <c r="O303">
+        <v>17</v>
+      </c>
+      <c r="P303">
+        <v>13</v>
+      </c>
+      <c r="Q303">
+        <v>2</v>
+      </c>
+      <c r="R303">
+        <v>6</v>
+      </c>
+      <c r="S303">
+        <v>4</v>
+      </c>
+      <c r="T303">
+        <v>2</v>
+      </c>
+      <c r="U303">
+        <v>0</v>
+      </c>
+      <c r="V303">
+        <v>0</v>
+      </c>
+      <c r="W303">
+        <v>3</v>
+      </c>
+      <c r="X303">
+        <v>4</v>
+      </c>
+      <c r="Y303">
+        <v>2.1</v>
+      </c>
+      <c r="Z303">
+        <v>3</v>
+      </c>
+      <c r="AA303">
+        <v>3.8</v>
+      </c>
+      <c r="AB303">
+        <v>2.1</v>
+      </c>
+      <c r="AC303">
+        <v>3</v>
+      </c>
+      <c r="AD303">
+        <v>3.8</v>
+      </c>
+      <c r="AE303">
+        <v>2.1</v>
+      </c>
+      <c r="AF303">
+        <v>2.8</v>
+      </c>
+      <c r="AG303">
+        <v>3.6</v>
+      </c>
+      <c r="AH303">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AI303">
+        <v>3</v>
+      </c>
+      <c r="AJ303">
+        <v>4</v>
+      </c>
+      <c r="AK303">
+        <v>2.1</v>
+      </c>
+      <c r="AL303">
+        <v>3.33</v>
+      </c>
+      <c r="AM303">
+        <v>3.96</v>
+      </c>
+      <c r="AN303">
+        <v>2.14</v>
+      </c>
+      <c r="AO303">
+        <v>3.2</v>
+      </c>
+      <c r="AP303">
+        <v>3.8</v>
+      </c>
+      <c r="AQ303">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AR303">
+        <v>3.2</v>
+      </c>
+      <c r="AS303">
+        <v>3.75</v>
+      </c>
+      <c r="AT303">
+        <v>2</v>
+      </c>
+      <c r="AU303">
+        <v>3.2</v>
+      </c>
+      <c r="AV303">
+        <v>4</v>
+      </c>
+      <c r="AW303">
+        <v>2.15</v>
+      </c>
+      <c r="AX303">
+        <v>3.2</v>
+      </c>
+      <c r="AY303">
+        <v>3.75</v>
+      </c>
+      <c r="AZ303">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="BA303">
+        <v>40</v>
+      </c>
+      <c r="BB303">
+        <v>3.4</v>
+      </c>
+      <c r="BC303">
+        <v>3.17</v>
+      </c>
+      <c r="BD303">
+        <v>4</v>
+      </c>
+      <c r="BE303">
+        <v>3.75</v>
+      </c>
+      <c r="BF303">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BG303">
+        <v>2.09</v>
+      </c>
+      <c r="BH303">
+        <v>26</v>
+      </c>
+      <c r="BI303">
+        <v>1.49</v>
+      </c>
+      <c r="BJ303">
+        <v>1.42</v>
+      </c>
+      <c r="BK303">
+        <v>3</v>
+      </c>
+      <c r="BL303">
+        <v>2.73</v>
+      </c>
+      <c r="BM303">
+        <v>25</v>
+      </c>
+      <c r="BN303">
+        <v>0.25</v>
+      </c>
+      <c r="BO303">
+        <v>2.08</v>
+      </c>
+      <c r="BP303">
+        <v>2.02</v>
+      </c>
+      <c r="BQ303">
+        <v>1.88</v>
+      </c>
+      <c r="BR303">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="304" spans="1:70">
+      <c r="A304" t="s">
+        <v>70</v>
+      </c>
+      <c r="B304" t="s">
+        <v>149</v>
+      </c>
+      <c r="C304" t="s">
+        <v>91</v>
+      </c>
+      <c r="D304" t="s">
+        <v>77</v>
+      </c>
+      <c r="E304">
+        <v>3</v>
+      </c>
+      <c r="F304">
+        <v>0</v>
+      </c>
+      <c r="G304" t="s">
+        <v>74</v>
+      </c>
+      <c r="H304">
+        <v>1</v>
+      </c>
+      <c r="I304">
+        <v>0</v>
+      </c>
+      <c r="J304" t="s">
+        <v>74</v>
+      </c>
+      <c r="K304">
+        <v>15</v>
+      </c>
+      <c r="L304">
+        <v>13</v>
+      </c>
+      <c r="M304">
+        <v>6</v>
+      </c>
+      <c r="N304">
+        <v>2</v>
+      </c>
+      <c r="O304">
+        <v>15</v>
+      </c>
+      <c r="P304">
+        <v>14</v>
+      </c>
+      <c r="Q304">
+        <v>7</v>
+      </c>
+      <c r="R304">
+        <v>4</v>
+      </c>
+      <c r="S304">
+        <v>1</v>
+      </c>
+      <c r="T304">
+        <v>3</v>
+      </c>
+      <c r="U304">
+        <v>0</v>
+      </c>
+      <c r="V304">
+        <v>0</v>
+      </c>
+      <c r="W304">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="X304">
+        <v>3.6</v>
+      </c>
+      <c r="Y304">
+        <v>2.8</v>
+      </c>
+      <c r="Z304">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AA304">
+        <v>3.7</v>
+      </c>
+      <c r="AB304">
+        <v>2.75</v>
+      </c>
+      <c r="AC304">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AD304">
+        <v>3.7</v>
+      </c>
+      <c r="AE304">
+        <v>2.75</v>
+      </c>
+      <c r="AF304">
+        <v>2.5</v>
+      </c>
+      <c r="AG304">
+        <v>3.5</v>
+      </c>
+      <c r="AH304">
+        <v>2.5</v>
+      </c>
+      <c r="AI304">
+        <v>2.25</v>
+      </c>
+      <c r="AJ304">
+        <v>3.75</v>
+      </c>
+      <c r="AK304">
+        <v>2.8</v>
+      </c>
+      <c r="AL304">
+        <v>2.4</v>
+      </c>
+      <c r="AM304">
+        <v>3.91</v>
+      </c>
+      <c r="AN304">
+        <v>2.87</v>
+      </c>
+      <c r="AO304">
+        <v>2.38</v>
+      </c>
+      <c r="AP304">
+        <v>3.75</v>
+      </c>
+      <c r="AQ304">
+        <v>2.7</v>
+      </c>
+      <c r="AR304">
+        <v>2.25</v>
+      </c>
+      <c r="AS304">
+        <v>3.5</v>
+      </c>
+      <c r="AT304">
+        <v>2.8</v>
+      </c>
+      <c r="AU304">
+        <v>2.4</v>
+      </c>
+      <c r="AV304">
+        <v>3.7</v>
+      </c>
+      <c r="AW304">
+        <v>2.9</v>
+      </c>
+      <c r="AX304">
+        <v>2.4</v>
+      </c>
+      <c r="AY304">
+        <v>3.5</v>
+      </c>
+      <c r="AZ304">
+        <v>2.75</v>
+      </c>
+      <c r="BA304">
+        <v>40</v>
+      </c>
+      <c r="BB304">
+        <v>2.5</v>
+      </c>
+      <c r="BC304">
+        <v>2.35</v>
+      </c>
+      <c r="BD304">
+        <v>3.91</v>
+      </c>
+      <c r="BE304">
+        <v>3.6</v>
+      </c>
+      <c r="BF304">
+        <v>2.9</v>
+      </c>
+      <c r="BG304">
+        <v>2.8</v>
+      </c>
+      <c r="BH304">
+        <v>26</v>
+      </c>
+      <c r="BI304">
+        <v>1.57</v>
+      </c>
+      <c r="BJ304">
+        <v>1.49</v>
+      </c>
+      <c r="BK304">
+        <v>2.7</v>
+      </c>
+      <c r="BL304">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="BM304">
+        <v>24</v>
+      </c>
+      <c r="BN304">
+        <v>-0.25</v>
+      </c>
+      <c r="BO304">
+        <v>2.11</v>
+      </c>
+      <c r="BP304">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="BQ304">
+        <v>1.86</v>
+      </c>
+      <c r="BR304">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="305" spans="1:70">
+      <c r="A305" t="s">
+        <v>70</v>
+      </c>
+      <c r="B305" t="s">
+        <v>149</v>
+      </c>
+      <c r="C305" t="s">
+        <v>88</v>
+      </c>
+      <c r="D305" t="s">
+        <v>85</v>
+      </c>
+      <c r="E305">
+        <v>3</v>
+      </c>
+      <c r="F305">
+        <v>4</v>
+      </c>
+      <c r="G305" t="s">
+        <v>78</v>
+      </c>
+      <c r="H305">
+        <v>3</v>
+      </c>
+      <c r="I305">
+        <v>2</v>
+      </c>
+      <c r="J305" t="s">
+        <v>74</v>
+      </c>
+      <c r="K305">
+        <v>11</v>
+      </c>
+      <c r="L305">
+        <v>26</v>
+      </c>
+      <c r="M305">
+        <v>5</v>
+      </c>
+      <c r="N305">
+        <v>13</v>
+      </c>
+      <c r="O305">
+        <v>7</v>
+      </c>
+      <c r="P305">
+        <v>7</v>
+      </c>
+      <c r="Q305">
+        <v>1</v>
+      </c>
+      <c r="R305">
+        <v>10</v>
+      </c>
+      <c r="S305">
+        <v>0</v>
+      </c>
+      <c r="T305">
+        <v>0</v>
+      </c>
+      <c r="U305">
+        <v>0</v>
+      </c>
+      <c r="V305">
+        <v>0</v>
+      </c>
+      <c r="W305">
+        <v>7</v>
+      </c>
+      <c r="X305">
+        <v>4.33</v>
+      </c>
+      <c r="Y305">
+        <v>1.44</v>
+      </c>
+      <c r="Z305">
+        <v>6.75</v>
+      </c>
+      <c r="AA305">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AB305">
+        <v>1.44</v>
+      </c>
+      <c r="AC305">
+        <v>6.75</v>
+      </c>
+      <c r="AD305">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AE305">
+        <v>1.44</v>
+      </c>
+      <c r="AF305">
+        <v>4.7</v>
+      </c>
+      <c r="AG305">
+        <v>3.8</v>
+      </c>
+      <c r="AH305">
+        <v>1.65</v>
+      </c>
+      <c r="AI305">
+        <v>6.5</v>
+      </c>
+      <c r="AJ305">
+        <v>4.5</v>
+      </c>
+      <c r="AK305">
+        <v>1.44</v>
+      </c>
+      <c r="AL305">
+        <v>7.68</v>
+      </c>
+      <c r="AM305">
+        <v>4.8</v>
+      </c>
+      <c r="AN305">
+        <v>1.47</v>
+      </c>
+      <c r="AO305">
+        <v>6</v>
+      </c>
+      <c r="AP305">
+        <v>4.5</v>
+      </c>
+      <c r="AQ305">
+        <v>1.5</v>
+      </c>
+      <c r="AR305">
+        <v>7</v>
+      </c>
+      <c r="AS305">
+        <v>4.33</v>
+      </c>
+      <c r="AT305">
+        <v>1.4</v>
+      </c>
+      <c r="AU305">
+        <v>6.5</v>
+      </c>
+      <c r="AV305">
+        <v>4.75</v>
+      </c>
+      <c r="AW305">
+        <v>1.5</v>
+      </c>
+      <c r="AX305">
+        <v>6</v>
+      </c>
+      <c r="AY305">
+        <v>4</v>
+      </c>
+      <c r="AZ305">
+        <v>1.53</v>
+      </c>
+      <c r="BA305">
+        <v>40</v>
+      </c>
+      <c r="BB305">
+        <v>7.61</v>
+      </c>
+      <c r="BC305">
+        <v>6.78</v>
+      </c>
+      <c r="BD305">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="BE305">
+        <v>4.42</v>
+      </c>
+      <c r="BF305">
+        <v>1.65</v>
+      </c>
+      <c r="BG305">
+        <v>1.46</v>
+      </c>
+      <c r="BH305">
+        <v>26</v>
+      </c>
+      <c r="BI305">
+        <v>1.6</v>
+      </c>
+      <c r="BJ305">
+        <v>1.51</v>
+      </c>
+      <c r="BK305">
+        <v>2.65</v>
+      </c>
+      <c r="BL305">
+        <v>2.46</v>
+      </c>
+      <c r="BM305">
+        <v>26</v>
+      </c>
+      <c r="BN305">
+        <v>1</v>
+      </c>
+      <c r="BO305">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="BP305">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="BQ305">
+        <v>1.75</v>
+      </c>
+      <c r="BR305">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="306" spans="1:70">
+      <c r="A306" t="s">
+        <v>70</v>
+      </c>
+      <c r="B306" t="s">
+        <v>149</v>
+      </c>
+      <c r="C306" t="s">
+        <v>87</v>
+      </c>
+      <c r="D306" t="s">
+        <v>73</v>
+      </c>
+      <c r="E306">
+        <v>3</v>
+      </c>
+      <c r="F306">
+        <v>2</v>
+      </c>
+      <c r="G306" t="s">
+        <v>74</v>
+      </c>
+      <c r="H306">
+        <v>0</v>
+      </c>
+      <c r="I306">
+        <v>1</v>
+      </c>
+      <c r="J306" t="s">
+        <v>78</v>
+      </c>
+      <c r="K306">
+        <v>16</v>
+      </c>
+      <c r="L306">
+        <v>18</v>
+      </c>
+      <c r="M306">
+        <v>5</v>
+      </c>
+      <c r="N306">
+        <v>4</v>
+      </c>
+      <c r="O306">
+        <v>16</v>
+      </c>
+      <c r="P306">
+        <v>12</v>
+      </c>
+      <c r="Q306">
+        <v>3</v>
+      </c>
+      <c r="R306">
+        <v>2</v>
+      </c>
+      <c r="S306">
+        <v>2</v>
+      </c>
+      <c r="T306">
+        <v>0</v>
+      </c>
+      <c r="U306">
+        <v>0</v>
+      </c>
+      <c r="V306">
+        <v>0</v>
+      </c>
+      <c r="W306">
+        <v>2.5</v>
+      </c>
+      <c r="X306">
+        <v>3.6</v>
+      </c>
+      <c r="Y306">
+        <v>2.6</v>
+      </c>
+      <c r="Z306">
+        <v>2.35</v>
+      </c>
+      <c r="AA306">
+        <v>3.6</v>
+      </c>
+      <c r="AB306">
+        <v>2.75</v>
+      </c>
+      <c r="AC306">
+        <v>2.35</v>
+      </c>
+      <c r="AD306">
+        <v>3.6</v>
+      </c>
+      <c r="AE306">
+        <v>2.75</v>
+      </c>
+      <c r="AF306">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="AG306">
+        <v>3.5</v>
+      </c>
+      <c r="AH306">
+        <v>2.9</v>
+      </c>
+      <c r="AI306">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AJ306">
+        <v>3.6</v>
+      </c>
+      <c r="AK306">
+        <v>2.8</v>
+      </c>
+      <c r="AL306">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AM306">
+        <v>3.7</v>
+      </c>
+      <c r="AN306">
+        <v>2.79</v>
+      </c>
+      <c r="AO306">
+        <v>2.5</v>
+      </c>
+      <c r="AP306">
+        <v>3.2</v>
+      </c>
+      <c r="AQ306">
+        <v>2.8</v>
+      </c>
+      <c r="AR306">
+        <v>2.4</v>
+      </c>
+      <c r="AS306">
+        <v>3.5</v>
+      </c>
+      <c r="AT306">
+        <v>2.63</v>
+      </c>
+      <c r="AU306">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="AV306">
+        <v>3.7</v>
+      </c>
+      <c r="AW306">
+        <v>2.7</v>
+      </c>
+      <c r="AX306">
+        <v>2.4</v>
+      </c>
+      <c r="AY306">
+        <v>3.5</v>
+      </c>
+      <c r="AZ306">
+        <v>2.75</v>
+      </c>
+      <c r="BA306">
+        <v>40</v>
+      </c>
+      <c r="BB306">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="BC306">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="BD306">
+        <v>3.75</v>
+      </c>
+      <c r="BE306">
+        <v>3.5</v>
+      </c>
+      <c r="BF306">
+        <v>2.9</v>
+      </c>
+      <c r="BG306">
+        <v>2.73</v>
+      </c>
+      <c r="BH306">
+        <v>26</v>
+      </c>
+      <c r="BI306">
+        <v>1.57</v>
+      </c>
+      <c r="BJ306">
+        <v>1.51</v>
+      </c>
+      <c r="BK306">
+        <v>2.65</v>
+      </c>
+      <c r="BL306">
+        <v>2.5</v>
+      </c>
+      <c r="BM306">
+        <v>25</v>
+      </c>
+      <c r="BN306">
+        <v>-0.25</v>
+      </c>
+      <c r="BO306">
+        <v>2.27</v>
+      </c>
+      <c r="BP306">
+        <v>2.16</v>
+      </c>
+      <c r="BQ306">
+        <v>1.78</v>
+      </c>
+      <c r="BR306">
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="307" spans="1:70">
+      <c r="A307" t="s">
+        <v>70</v>
+      </c>
+      <c r="B307" t="s">
+        <v>149</v>
+      </c>
+      <c r="C307" t="s">
+        <v>93</v>
+      </c>
+      <c r="D307" t="s">
+        <v>83</v>
+      </c>
+      <c r="E307">
+        <v>2</v>
+      </c>
+      <c r="F307">
+        <v>2</v>
+      </c>
+      <c r="G307" t="s">
+        <v>79</v>
+      </c>
+      <c r="H307">
+        <v>2</v>
+      </c>
+      <c r="I307">
+        <v>2</v>
+      </c>
+      <c r="J307" t="s">
+        <v>79</v>
+      </c>
+      <c r="K307">
+        <v>10</v>
+      </c>
+      <c r="L307">
+        <v>15</v>
+      </c>
+      <c r="M307">
+        <v>3</v>
+      </c>
+      <c r="N307">
+        <v>3</v>
+      </c>
+      <c r="O307">
+        <v>17</v>
+      </c>
+      <c r="P307">
+        <v>13</v>
+      </c>
+      <c r="Q307">
+        <v>5</v>
+      </c>
+      <c r="R307">
+        <v>5</v>
+      </c>
+      <c r="S307">
+        <v>2</v>
+      </c>
+      <c r="T307">
+        <v>0</v>
+      </c>
+      <c r="U307">
+        <v>0</v>
+      </c>
+      <c r="V307">
+        <v>0</v>
+      </c>
+      <c r="W307">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="X307">
+        <v>3.6</v>
+      </c>
+      <c r="Y307">
+        <v>3.3</v>
+      </c>
+      <c r="Z307">
+        <v>1.95</v>
+      </c>
+      <c r="AA307">
+        <v>3.6</v>
+      </c>
+      <c r="AB307">
+        <v>3.6</v>
+      </c>
+      <c r="AC307">
+        <v>1.95</v>
+      </c>
+      <c r="AD307">
+        <v>3.6</v>
+      </c>
+      <c r="AE307">
+        <v>3.6</v>
+      </c>
+      <c r="AF307">
+        <v>1.9</v>
+      </c>
+      <c r="AG307">
+        <v>3.6</v>
+      </c>
+      <c r="AH307">
+        <v>3.6</v>
+      </c>
+      <c r="AI307">
+        <v>1.95</v>
+      </c>
+      <c r="AJ307">
+        <v>3.75</v>
+      </c>
+      <c r="AK307">
+        <v>3.5</v>
+      </c>
+      <c r="AL307">
+        <v>2.09</v>
+      </c>
+      <c r="AM307">
+        <v>3.84</v>
+      </c>
+      <c r="AN307">
+        <v>3.59</v>
+      </c>
+      <c r="AO307">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AP307">
+        <v>3.6</v>
+      </c>
+      <c r="AQ307">
+        <v>3.4</v>
+      </c>
+      <c r="AR307">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AS307">
+        <v>3.5</v>
+      </c>
+      <c r="AT307">
+        <v>3.3</v>
+      </c>
+      <c r="AU307">
+        <v>2.15</v>
+      </c>
+      <c r="AV307">
+        <v>3.75</v>
+      </c>
+      <c r="AW307">
+        <v>3.3</v>
+      </c>
+      <c r="AX307">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="AY307">
+        <v>3.5</v>
+      </c>
+      <c r="AZ307">
+        <v>3.4</v>
+      </c>
+      <c r="BA307">
+        <v>40</v>
+      </c>
+      <c r="BB307">
+        <v>2.15</v>
+      </c>
+      <c r="BC307">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="BD307">
+        <v>3.8</v>
+      </c>
+      <c r="BE307">
+        <v>3.58</v>
+      </c>
+      <c r="BF307">
+        <v>3.6</v>
+      </c>
+      <c r="BG307">
+        <v>3.43</v>
+      </c>
+      <c r="BH307">
+        <v>26</v>
+      </c>
+      <c r="BI307">
+        <v>1.7</v>
+      </c>
+      <c r="BJ307">
+        <v>1.6</v>
+      </c>
+      <c r="BK307">
+        <v>2.4</v>
+      </c>
+      <c r="BL307">
+        <v>2.25</v>
+      </c>
+      <c r="BM307">
+        <v>25</v>
+      </c>
+      <c r="BN307">
+        <v>-0.25</v>
+      </c>
+      <c r="BO307">
+        <v>1.86</v>
+      </c>
+      <c r="BP307">
+        <v>1.81</v>
+      </c>
+      <c r="BQ307">
+        <v>2.12</v>
+      </c>
+      <c r="BR307">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>